<commit_message>
Pegando novos casos de teste Koerkel Ghosh simetrico e assimetrico
</commit_message>
<xml_diff>
--- a/solutions.xlsx
+++ b/solutions.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="258">
   <si>
     <t>ILP</t>
   </si>
@@ -822,6 +822,18 @@
   <si>
     <t>flp1000x6000.txt</t>
   </si>
+  <si>
+    <t>flp1000x10000.txt</t>
+  </si>
+  <si>
+    <t>flp2000x6000.txt</t>
+  </si>
+  <si>
+    <t>flp3000x10000.txt</t>
+  </si>
+  <si>
+    <t>MIP - ILP</t>
+  </si>
 </sst>
 </file>
 
@@ -970,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -997,6 +1009,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1014,20 +1030,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="43">
     <dxf>
       <font>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1037,7 +1051,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1142,38 +1156,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -1270,38 +1252,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1486,6 +1436,16 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1778,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ1002"/>
+  <dimension ref="A1:AJ1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J237" sqref="J237"/>
+    <sheetView tabSelected="1" topLeftCell="N208" zoomScale="111" workbookViewId="0">
+      <selection activeCell="AB250" sqref="AB250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1798,9 +1758,9 @@
     <col min="19" max="21" width="13.5" customWidth="1"/>
     <col min="22" max="22" width="16" customWidth="1"/>
     <col min="23" max="26" width="13.5" customWidth="1"/>
-    <col min="27" max="27" width="14.33203125" customWidth="1"/>
+    <col min="27" max="27" width="18.1640625" customWidth="1"/>
     <col min="28" max="28" width="14.83203125" customWidth="1"/>
-    <col min="29" max="29" width="10.6640625" customWidth="1"/>
+    <col min="29" max="29" width="14.6640625" customWidth="1"/>
     <col min="30" max="30" width="10.5" customWidth="1"/>
     <col min="31" max="31" width="16" customWidth="1"/>
     <col min="32" max="33" width="10.5" customWidth="1"/>
@@ -1810,61 +1770,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="19"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="19"/>
+      <c r="L1" s="23"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="19"/>
+      <c r="O1" s="23"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="22" t="s">
+      <c r="Q1" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
       <c r="T1" s="15"/>
-      <c r="U1" s="23" t="s">
+      <c r="U1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="19"/>
+      <c r="V1" s="23"/>
       <c r="W1" s="1"/>
-      <c r="X1" s="23" t="s">
+      <c r="X1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="19"/>
+      <c r="Y1" s="23"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="23" t="s">
+      <c r="AA1" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="19"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="23"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="23" t="s">
+      <c r="AE1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="AF1" s="19"/>
+      <c r="AF1" s="23"/>
       <c r="AG1" s="1"/>
-      <c r="AH1" s="23" t="s">
+      <c r="AH1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="AI1" s="19"/>
+      <c r="AI1" s="23"/>
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1919,14 +1879,14 @@
       </c>
       <c r="T2" s="16"/>
       <c r="U2" s="2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>8</v>
@@ -2030,7 +1990,7 @@
         <v>-0.62232164738142393</v>
       </c>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="25" t="s">
+      <c r="AA3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="AB3" s="9">
@@ -2132,7 +2092,7 @@
         <v>-0.71606507713131318</v>
       </c>
       <c r="Z4" s="1"/>
-      <c r="AA4" s="25" t="s">
+      <c r="AA4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="AB4" s="9">
@@ -2234,7 +2194,7 @@
         <v>-0.27304584665160181</v>
       </c>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="25" t="s">
+      <c r="AA5" s="18" t="s">
         <v>11</v>
       </c>
       <c r="AB5" s="9">
@@ -2336,7 +2296,7 @@
         <v>4.9487206240678663E-2</v>
       </c>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="25" t="s">
+      <c r="AA6" s="18" t="s">
         <v>12</v>
       </c>
       <c r="AB6" s="9">
@@ -2438,7 +2398,7 @@
         <v>-6.375056505912273E-2</v>
       </c>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="25" t="s">
+      <c r="AA7" s="18" t="s">
         <v>13</v>
       </c>
       <c r="AB7" s="9">
@@ -2540,7 +2500,7 @@
         <v>-8.6385319611066408E-2</v>
       </c>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="25" t="s">
+      <c r="AA8" s="18" t="s">
         <v>14</v>
       </c>
       <c r="AB8" s="9">
@@ -2642,7 +2602,7 @@
         <v>7.6821348913401321E-3</v>
       </c>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="25" t="s">
+      <c r="AA9" s="18" t="s">
         <v>15</v>
       </c>
       <c r="AB9" s="9">
@@ -2744,7 +2704,7 @@
         <v>-1.3612781418077978E-2</v>
       </c>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="25" t="s">
+      <c r="AA10" s="18" t="s">
         <v>16</v>
       </c>
       <c r="AB10" s="9">
@@ -2846,7 +2806,7 @@
         <v>-0.14942649048718221</v>
       </c>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="25" t="s">
+      <c r="AA11" s="18" t="s">
         <v>17</v>
       </c>
       <c r="AB11" s="9">
@@ -2948,7 +2908,7 @@
         <v>-0.15689816634115145</v>
       </c>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="25" t="s">
+      <c r="AA12" s="18" t="s">
         <v>18</v>
       </c>
       <c r="AB12" s="9">
@@ -3050,7 +3010,7 @@
         <v>-0.28577482998133247</v>
       </c>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="25" t="s">
+      <c r="AA13" s="18" t="s">
         <v>19</v>
       </c>
       <c r="AB13" s="9">
@@ -3152,7 +3112,7 @@
         <v>-0.17185321467392925</v>
       </c>
       <c r="Z14" s="1"/>
-      <c r="AA14" s="25" t="s">
+      <c r="AA14" s="18" t="s">
         <v>20</v>
       </c>
       <c r="AB14" s="9">
@@ -3254,7 +3214,7 @@
         <v>-4.380002513219728E-2</v>
       </c>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="25" t="s">
+      <c r="AA15" s="18" t="s">
         <v>21</v>
       </c>
       <c r="AB15" s="9">
@@ -3356,7 +3316,7 @@
         <v>3.78479027517266E-2</v>
       </c>
       <c r="Z16" s="1"/>
-      <c r="AA16" s="25" t="s">
+      <c r="AA16" s="18" t="s">
         <v>22</v>
       </c>
       <c r="AB16" s="9">
@@ -3458,7 +3418,7 @@
         <v>-0.19664447354542663</v>
       </c>
       <c r="Z17" s="1"/>
-      <c r="AA17" s="25" t="s">
+      <c r="AA17" s="18" t="s">
         <v>23</v>
       </c>
       <c r="AB17" s="9">
@@ -21597,11 +21557,11 @@
       </c>
       <c r="T195" s="1"/>
       <c r="U195" s="10">
-        <f t="shared" ref="U195:U239" si="44">R195-B195</f>
+        <f t="shared" ref="U195:U238" si="44">R195-B195</f>
         <v>0</v>
       </c>
       <c r="V195" s="17">
-        <f t="shared" ref="V195:V239" si="45">U195/B195</f>
+        <f t="shared" ref="V195:V238" si="45">U195/B195</f>
         <v>0</v>
       </c>
       <c r="W195" s="1"/>
@@ -21610,7 +21570,7 @@
         <v>-6.0131993293762207</v>
       </c>
       <c r="Y195" s="17">
-        <f t="shared" ref="Y195:Y239" si="46">X195/C195</f>
+        <f t="shared" ref="Y195:Y238" si="46">X195/C195</f>
         <v>-0.68128708798284765</v>
       </c>
       <c r="Z195" s="1"/>
@@ -21625,20 +21585,20 @@
       </c>
       <c r="AD195" s="1"/>
       <c r="AE195" s="6">
-        <f t="shared" ref="AE195:AE239" si="47">AB195-B195</f>
+        <f t="shared" ref="AE195:AE238" si="47">AB195-B195</f>
         <v>20898</v>
       </c>
       <c r="AF195" s="8">
-        <f t="shared" ref="AF195:AF239" si="48">AE195/B195</f>
+        <f t="shared" ref="AF195:AF242" si="48">AE195/B195</f>
         <v>0.58454308970378455</v>
       </c>
       <c r="AG195" s="1"/>
       <c r="AH195" s="7">
-        <f t="shared" ref="AH195:AH239" si="49">AC195-C195</f>
+        <f t="shared" ref="AH195:AH238" si="49">AC195-C195</f>
         <v>-8.2629691022491407</v>
       </c>
       <c r="AI195" s="8">
-        <f t="shared" ref="AI195:AI239" si="50">AH195/C195</f>
+        <f t="shared" ref="AI195:AI238" si="50">AH195/C195</f>
         <v>-0.9361828619686775</v>
       </c>
       <c r="AJ195" s="1"/>
@@ -25941,7 +25901,7 @@
         <v>1</v>
       </c>
       <c r="E238" s="12"/>
-      <c r="F238" s="26" t="s">
+      <c r="F238" s="19" t="s">
         <v>252</v>
       </c>
       <c r="G238" s="10">
@@ -25972,7 +25932,7 @@
         <v>-0.76312910262946942</v>
       </c>
       <c r="P238" s="1"/>
-      <c r="Q238" s="26" t="s">
+      <c r="Q238" s="19" t="s">
         <v>252</v>
       </c>
       <c r="R238" s="10">
@@ -26043,7 +26003,7 @@
         <v>0</v>
       </c>
       <c r="E239" s="12"/>
-      <c r="F239" s="26" t="s">
+      <c r="F239" s="19" t="s">
         <v>253</v>
       </c>
       <c r="G239" s="10">
@@ -26074,7 +26034,7 @@
         <v>-0.12610399435484415</v>
       </c>
       <c r="P239" s="1"/>
-      <c r="Q239" s="26" t="s">
+      <c r="Q239" s="19" t="s">
         <v>253</v>
       </c>
       <c r="R239" s="10">
@@ -26085,11 +26045,11 @@
       </c>
       <c r="T239" s="1"/>
       <c r="U239" s="10">
-        <f t="shared" si="44"/>
+        <f>R239-B239</f>
         <v>-29975660</v>
       </c>
       <c r="V239" s="17">
-        <f t="shared" si="45"/>
+        <f>U239/B239</f>
         <v>-0.85660215539504025</v>
       </c>
       <c r="W239" s="1"/>
@@ -26098,7 +26058,7 @@
         <v>-28.54945516586298</v>
       </c>
       <c r="Y239" s="17">
-        <f t="shared" si="46"/>
+        <f>X239/C239</f>
         <v>-7.3925791644069899E-2</v>
       </c>
       <c r="Z239" s="1"/>
@@ -26113,7 +26073,7 @@
       </c>
       <c r="AD239" s="1"/>
       <c r="AE239" s="6">
-        <f t="shared" si="47"/>
+        <f>AB239-B239</f>
         <v>-32987638</v>
       </c>
       <c r="AF239" s="8">
@@ -26122,245 +26082,212 @@
       </c>
       <c r="AG239" s="1"/>
       <c r="AH239" s="7">
-        <f t="shared" si="49"/>
+        <f>AC239-C239</f>
         <v>-19.216726280212015</v>
       </c>
       <c r="AI239" s="8">
-        <f t="shared" si="50"/>
+        <f>AH239/C239</f>
         <v>-4.9759678243202439E-2</v>
       </c>
       <c r="AJ239" s="1"/>
     </row>
     <row r="240" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A240" s="1"/>
-      <c r="B240" s="1"/>
-      <c r="C240" s="1"/>
-      <c r="D240" s="1"/>
-      <c r="E240" s="1"/>
-      <c r="F240" s="1"/>
-      <c r="G240" s="1"/>
-      <c r="H240" s="1"/>
-      <c r="I240" s="1"/>
+      <c r="A240" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B240" s="10">
+        <v>55342977</v>
+      </c>
+      <c r="C240" s="20">
+        <v>1606.694</v>
+      </c>
+      <c r="D240" s="10">
+        <v>0</v>
+      </c>
+      <c r="E240" s="12"/>
+      <c r="F240" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G240" s="10"/>
+      <c r="H240" s="10"/>
+      <c r="I240" s="10"/>
       <c r="J240" s="1"/>
-      <c r="K240" s="1"/>
-      <c r="L240" s="1"/>
+      <c r="K240" s="10"/>
+      <c r="L240" s="17"/>
       <c r="M240" s="1"/>
-      <c r="N240" s="1"/>
-      <c r="O240" s="1"/>
+      <c r="N240" s="10"/>
+      <c r="O240" s="17"/>
       <c r="P240" s="1"/>
-      <c r="Q240" s="1"/>
-      <c r="R240" s="1"/>
-      <c r="S240" s="1"/>
+      <c r="Q240" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="R240" s="10"/>
+      <c r="S240" s="10"/>
       <c r="T240" s="1"/>
-      <c r="U240" s="1"/>
-      <c r="V240" s="1"/>
+      <c r="U240" s="10"/>
+      <c r="V240" s="17"/>
       <c r="W240" s="1"/>
-      <c r="X240" s="1"/>
-      <c r="Y240" s="1"/>
+      <c r="X240" s="10"/>
+      <c r="Y240" s="17"/>
       <c r="Z240" s="1"/>
-      <c r="AA240" s="1"/>
-      <c r="AB240" s="1"/>
-      <c r="AC240" s="1"/>
+      <c r="AA240" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB240" s="21">
+        <v>4479570</v>
+      </c>
+      <c r="AC240">
+        <v>795.18200000000002</v>
+      </c>
       <c r="AD240" s="1"/>
-      <c r="AE240" s="1"/>
-      <c r="AF240" s="1"/>
+      <c r="AE240" s="6">
+        <f>AB240-B240</f>
+        <v>-50863407</v>
+      </c>
+      <c r="AF240" s="8">
+        <f t="shared" si="48"/>
+        <v>-0.91905802248404522</v>
+      </c>
       <c r="AG240" s="1"/>
-      <c r="AH240" s="1"/>
-      <c r="AI240" s="1"/>
+      <c r="AH240" s="7">
+        <f>AC240-C240</f>
+        <v>-811.51199999999994</v>
+      </c>
+      <c r="AI240" s="8">
+        <f>AH240/C240</f>
+        <v>-0.5050818637525254</v>
+      </c>
       <c r="AJ240" s="1"/>
     </row>
     <row r="241" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A241" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="B241" s="19"/>
-      <c r="C241" s="7">
-        <f>SUM(C3:C239)</f>
-        <v>2404.6531496047946</v>
-      </c>
-      <c r="D241" s="1"/>
-      <c r="E241" s="1"/>
-      <c r="F241" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="G241" s="19"/>
-      <c r="H241" s="7">
-        <f>SUM(H3:H239)</f>
-        <v>442.46593046188286</v>
-      </c>
-      <c r="I241" s="1"/>
+      <c r="A241" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B241" s="10">
+        <v>39631404</v>
+      </c>
+      <c r="C241" s="10">
+        <v>1903.46</v>
+      </c>
+      <c r="D241" s="10">
+        <v>0</v>
+      </c>
+      <c r="E241" s="12"/>
+      <c r="F241" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G241" s="10"/>
+      <c r="H241" s="10"/>
+      <c r="I241" s="10"/>
       <c r="J241" s="1"/>
-      <c r="K241" s="1"/>
-      <c r="L241" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="M241" s="19"/>
-      <c r="N241" s="7">
-        <f>H241-C241</f>
-        <v>-1962.1872191429118</v>
-      </c>
-      <c r="O241" s="20">
-        <f>N241/C241</f>
-        <v>-0.81599594497252037</v>
-      </c>
+      <c r="K241" s="10"/>
+      <c r="L241" s="17"/>
+      <c r="M241" s="1"/>
+      <c r="N241" s="10"/>
+      <c r="O241" s="17"/>
       <c r="P241" s="1"/>
-      <c r="Q241" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="R241" s="19"/>
-      <c r="S241" s="7">
-        <f>SUM(S3:S239)</f>
-        <v>999.63952136039632</v>
-      </c>
+      <c r="Q241" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="R241" s="10"/>
+      <c r="S241" s="10"/>
       <c r="T241" s="1"/>
-      <c r="U241" s="1"/>
-      <c r="V241" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="W241" s="19"/>
-      <c r="X241" s="7">
-        <f>S241-C241</f>
-        <v>-1405.0136282443982</v>
-      </c>
-      <c r="Y241" s="20">
-        <f>X241/C241</f>
-        <v>-0.58428951737813517</v>
-      </c>
+      <c r="U241" s="10"/>
+      <c r="V241" s="17"/>
+      <c r="W241" s="1"/>
+      <c r="X241" s="10"/>
+      <c r="Y241" s="17"/>
       <c r="Z241" s="1"/>
-      <c r="AA241" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="AB241" s="19"/>
-      <c r="AC241" s="7">
-        <f>SUM(AC3:AC239)</f>
-        <v>2301.6296520000005</v>
+      <c r="AA241" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AB241" s="21">
+        <v>1724630</v>
+      </c>
+      <c r="AC241">
+        <v>890.11</v>
       </c>
       <c r="AD241" s="1"/>
-      <c r="AE241" s="1"/>
-      <c r="AF241" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="AG241" s="19"/>
+      <c r="AE241" s="6">
+        <f>AB241-B241</f>
+        <v>-37906774</v>
+      </c>
+      <c r="AF241" s="8">
+        <f t="shared" si="48"/>
+        <v>-0.95648324747717739</v>
+      </c>
+      <c r="AG241" s="1"/>
       <c r="AH241" s="7">
         <f>AC241-C241</f>
-        <v>-103.0234976047941</v>
-      </c>
-      <c r="AI241" s="20">
+        <v>-1013.35</v>
+      </c>
+      <c r="AI241" s="8">
         <f>AH241/C241</f>
-        <v>-4.2843392038359476E-2</v>
+        <v>-0.5323726266903428</v>
       </c>
       <c r="AJ241" s="1"/>
     </row>
     <row r="242" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A242" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="B242" s="19"/>
-      <c r="C242" s="7">
-        <f>C241/60</f>
-        <v>40.077552493413243</v>
-      </c>
-      <c r="D242" s="1"/>
-      <c r="E242" s="1"/>
-      <c r="F242" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="G242" s="19"/>
-      <c r="H242" s="7">
-        <f>H241/60</f>
-        <v>7.3744321743647143</v>
-      </c>
-      <c r="I242" s="1"/>
+      <c r="A242" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B242" s="10">
+        <v>64172666</v>
+      </c>
+      <c r="C242" s="10">
+        <v>5842.8617999999997</v>
+      </c>
+      <c r="D242" s="10">
+        <v>0</v>
+      </c>
+      <c r="E242" s="12"/>
+      <c r="F242" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G242" s="10"/>
+      <c r="H242" s="10"/>
+      <c r="I242" s="10"/>
       <c r="J242" s="1"/>
-      <c r="K242" s="1"/>
-      <c r="L242" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="M242" s="19"/>
-      <c r="N242" s="7">
-        <f>H242-C242</f>
-        <v>-32.70312031904853</v>
-      </c>
-      <c r="O242" s="21"/>
+      <c r="K242" s="10"/>
+      <c r="L242" s="17"/>
+      <c r="M242" s="1"/>
+      <c r="N242" s="10"/>
+      <c r="O242" s="17"/>
       <c r="P242" s="1"/>
-      <c r="Q242" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="R242" s="19"/>
-      <c r="S242" s="7">
-        <f>S241/60</f>
-        <v>16.66065868933994</v>
-      </c>
+      <c r="Q242" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="R242" s="10"/>
+      <c r="S242" s="10"/>
       <c r="T242" s="1"/>
-      <c r="U242" s="1"/>
-      <c r="V242" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="W242" s="19"/>
-      <c r="X242" s="7">
-        <f>S242-C242</f>
-        <v>-23.416893804073304</v>
-      </c>
-      <c r="Y242" s="21"/>
+      <c r="U242" s="10"/>
+      <c r="V242" s="17"/>
+      <c r="W242" s="1"/>
+      <c r="X242" s="10"/>
+      <c r="Y242" s="17"/>
       <c r="Z242" s="1"/>
-      <c r="AA242" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="AB242" s="19"/>
-      <c r="AC242" s="7">
-        <f>AC241/60</f>
-        <v>38.360494200000012</v>
+      <c r="AA242" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB242" s="21">
+        <v>2428440</v>
+      </c>
+      <c r="AC242">
+        <v>2457.98</v>
       </c>
       <c r="AD242" s="1"/>
-      <c r="AE242" s="1"/>
-      <c r="AF242" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="AG242" s="19"/>
-      <c r="AH242" s="7">
-        <f>AC242-C242</f>
-        <v>-1.7170582934132312</v>
-      </c>
-      <c r="AI242" s="21"/>
+      <c r="AE242" s="6">
+        <f>AB242-B242</f>
+        <v>-61744226</v>
+      </c>
+      <c r="AF242" s="8">
+        <f t="shared" ref="AF242" si="66">AE242/B242</f>
+        <v>-0.96215771992393151</v>
+      </c>
+      <c r="AG242" s="1"/>
+      <c r="AH242" s="7"/>
+      <c r="AI242" s="8"/>
       <c r="AJ242" s="1"/>
-    </row>
-    <row r="243" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A243" s="1"/>
-      <c r="B243" s="1"/>
-      <c r="C243" s="1"/>
-      <c r="D243" s="1"/>
-      <c r="E243" s="1"/>
-      <c r="F243" s="1"/>
-      <c r="G243" s="1"/>
-      <c r="H243" s="1"/>
-      <c r="I243" s="1"/>
-      <c r="J243" s="1"/>
-      <c r="K243" s="1"/>
-      <c r="L243" s="1"/>
-      <c r="M243" s="1"/>
-      <c r="N243" s="1"/>
-      <c r="O243" s="1"/>
-      <c r="P243" s="1"/>
-      <c r="Q243" s="1"/>
-      <c r="R243" s="1"/>
-      <c r="S243" s="1"/>
-      <c r="T243" s="1"/>
-      <c r="U243" s="1"/>
-      <c r="V243" s="1"/>
-      <c r="W243" s="1"/>
-      <c r="X243" s="1"/>
-      <c r="Y243" s="1"/>
-      <c r="Z243" s="1"/>
-      <c r="AA243" s="1"/>
-      <c r="AB243" s="1"/>
-      <c r="AC243" s="1"/>
-      <c r="AD243" s="1"/>
-      <c r="AE243" s="1"/>
-      <c r="AF243" s="1"/>
-      <c r="AG243" s="1"/>
-      <c r="AH243" s="1"/>
-      <c r="AI243" s="1"/>
-      <c r="AJ243" s="1"/>
     </row>
     <row r="244" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
@@ -26401,79 +26328,158 @@
       <c r="AJ244" s="1"/>
     </row>
     <row r="245" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A245" s="1"/>
-      <c r="B245" s="1"/>
-      <c r="C245" s="1"/>
+      <c r="A245" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="B245" s="23"/>
+      <c r="C245" s="7">
+        <f>SUM(C3:C242)</f>
+        <v>11757.668949604795</v>
+      </c>
       <c r="D245" s="1"/>
       <c r="E245" s="1"/>
-      <c r="F245" s="1"/>
-      <c r="G245" s="1"/>
-      <c r="H245" s="1"/>
+      <c r="F245" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="G245" s="23"/>
+      <c r="H245" s="7">
+        <f>SUM(H3:H242)</f>
+        <v>442.46593046188286</v>
+      </c>
       <c r="I245" s="1"/>
       <c r="J245" s="1"/>
       <c r="K245" s="1"/>
-      <c r="L245" s="1"/>
-      <c r="M245" s="1"/>
-      <c r="N245" s="1"/>
-      <c r="O245" s="1"/>
+      <c r="L245" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="M245" s="23"/>
+      <c r="N245" s="7">
+        <f>H245-C245</f>
+        <v>-11315.203019142911</v>
+      </c>
+      <c r="O245" s="24">
+        <f>N245/C245</f>
+        <v>-0.96236788666542994</v>
+      </c>
       <c r="P245" s="1"/>
-      <c r="Q245" s="1"/>
-      <c r="R245" s="1"/>
-      <c r="S245" s="1"/>
+      <c r="Q245" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="R245" s="23"/>
+      <c r="S245" s="7">
+        <f>SUM(S3:S242)</f>
+        <v>999.63952136039632</v>
+      </c>
       <c r="T245" s="1"/>
       <c r="U245" s="1"/>
-      <c r="V245" s="1"/>
-      <c r="W245" s="1"/>
-      <c r="X245" s="1"/>
-      <c r="Y245" s="1"/>
+      <c r="V245" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="W245" s="23"/>
+      <c r="X245" s="7">
+        <f>S245-C245</f>
+        <v>-10758.029428244399</v>
+      </c>
+      <c r="Y245" s="24">
+        <f>X245/C245</f>
+        <v>-0.91497978675492508</v>
+      </c>
       <c r="Z245" s="1"/>
-      <c r="AA245" s="1"/>
-      <c r="AB245" s="1"/>
-      <c r="AC245" s="1"/>
+      <c r="AA245" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="AB245" s="23"/>
+      <c r="AC245" s="7">
+        <f>SUM(AC3:AC242)</f>
+        <v>6444.9016520000005</v>
+      </c>
       <c r="AD245" s="1"/>
       <c r="AE245" s="1"/>
-      <c r="AF245" s="1"/>
-      <c r="AG245" s="1"/>
-      <c r="AH245" s="1"/>
-      <c r="AI245" s="1"/>
+      <c r="AF245" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="AG245" s="23"/>
+      <c r="AH245" s="7">
+        <f>AC245-C245</f>
+        <v>-5312.7672976047943</v>
+      </c>
+      <c r="AI245" s="24">
+        <f>AH245/C245</f>
+        <v>-0.45185549281716847</v>
+      </c>
       <c r="AJ245" s="1"/>
     </row>
     <row r="246" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A246" s="1"/>
-      <c r="B246" s="1"/>
-      <c r="C246" s="1"/>
+      <c r="A246" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="B246" s="23"/>
+      <c r="C246" s="7">
+        <f>C245/60</f>
+        <v>195.96114916007991</v>
+      </c>
       <c r="D246" s="1"/>
       <c r="E246" s="1"/>
-      <c r="F246" s="1"/>
-      <c r="G246" s="1"/>
-      <c r="H246" s="1"/>
+      <c r="F246" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="G246" s="23"/>
+      <c r="H246" s="7">
+        <f>H245/60</f>
+        <v>7.3744321743647143</v>
+      </c>
       <c r="I246" s="1"/>
       <c r="J246" s="1"/>
       <c r="K246" s="1"/>
-      <c r="L246" s="1"/>
-      <c r="M246" s="1"/>
-      <c r="N246" s="1"/>
-      <c r="O246" s="1"/>
+      <c r="L246" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="M246" s="23"/>
+      <c r="N246" s="7">
+        <f>H246-C246</f>
+        <v>-188.58671698571519</v>
+      </c>
+      <c r="O246" s="25"/>
       <c r="P246" s="1"/>
-      <c r="Q246" s="1"/>
-      <c r="R246" s="1"/>
-      <c r="S246" s="1"/>
+      <c r="Q246" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="R246" s="23"/>
+      <c r="S246" s="7">
+        <f>S245/60</f>
+        <v>16.66065868933994</v>
+      </c>
       <c r="T246" s="1"/>
       <c r="U246" s="1"/>
-      <c r="V246" s="1"/>
-      <c r="W246" s="1"/>
-      <c r="X246" s="1"/>
-      <c r="Y246" s="1"/>
+      <c r="V246" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="W246" s="23"/>
+      <c r="X246" s="7">
+        <f>S246-C246</f>
+        <v>-179.30049047073999</v>
+      </c>
+      <c r="Y246" s="25"/>
       <c r="Z246" s="1"/>
-      <c r="AA246" s="1"/>
-      <c r="AB246" s="1"/>
-      <c r="AC246" s="1"/>
+      <c r="AA246" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB246" s="23"/>
+      <c r="AC246" s="7">
+        <f>AC245/60</f>
+        <v>107.41502753333334</v>
+      </c>
       <c r="AD246" s="1"/>
       <c r="AE246" s="1"/>
-      <c r="AF246" s="1"/>
-      <c r="AG246" s="1"/>
-      <c r="AH246" s="1"/>
-      <c r="AI246" s="1"/>
+      <c r="AF246" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="AG246" s="23"/>
+      <c r="AH246" s="7">
+        <f>AC246-C246</f>
+        <v>-88.546121626746569</v>
+      </c>
+      <c r="AI246" s="25"/>
       <c r="AJ246" s="1"/>
     </row>
     <row r="247" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -55204,240 +55210,355 @@
       <c r="AI1002" s="1"/>
       <c r="AJ1002" s="1"/>
     </row>
+    <row r="1003" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+      <c r="AA1003" s="1"/>
+      <c r="AB1003" s="1"/>
+      <c r="AC1003" s="1"/>
+      <c r="AD1003" s="1"/>
+      <c r="AE1003" s="1"/>
+      <c r="AF1003" s="1"/>
+      <c r="AG1003" s="1"/>
+      <c r="AH1003" s="1"/>
+      <c r="AI1003" s="1"/>
+      <c r="AJ1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="1"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+      <c r="S1004" s="1"/>
+      <c r="T1004" s="1"/>
+      <c r="U1004" s="1"/>
+      <c r="V1004" s="1"/>
+      <c r="W1004" s="1"/>
+      <c r="X1004" s="1"/>
+      <c r="Y1004" s="1"/>
+      <c r="Z1004" s="1"/>
+      <c r="AA1004" s="1"/>
+      <c r="AB1004" s="1"/>
+      <c r="AC1004" s="1"/>
+      <c r="AD1004" s="1"/>
+      <c r="AE1004" s="1"/>
+      <c r="AF1004" s="1"/>
+      <c r="AG1004" s="1"/>
+      <c r="AH1004" s="1"/>
+      <c r="AI1004" s="1"/>
+      <c r="AJ1004" s="1"/>
+    </row>
+    <row r="1005" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="1"/>
+      <c r="E1005" s="1"/>
+      <c r="F1005" s="1"/>
+      <c r="G1005" s="1"/>
+      <c r="H1005" s="1"/>
+      <c r="I1005" s="1"/>
+      <c r="J1005" s="1"/>
+      <c r="K1005" s="1"/>
+      <c r="L1005" s="1"/>
+      <c r="M1005" s="1"/>
+      <c r="N1005" s="1"/>
+      <c r="O1005" s="1"/>
+      <c r="P1005" s="1"/>
+      <c r="Q1005" s="1"/>
+      <c r="R1005" s="1"/>
+      <c r="S1005" s="1"/>
+      <c r="T1005" s="1"/>
+      <c r="U1005" s="1"/>
+      <c r="V1005" s="1"/>
+      <c r="W1005" s="1"/>
+      <c r="X1005" s="1"/>
+      <c r="Y1005" s="1"/>
+      <c r="Z1005" s="1"/>
+      <c r="AA1005" s="1"/>
+      <c r="AB1005" s="1"/>
+      <c r="AC1005" s="1"/>
+      <c r="AD1005" s="1"/>
+      <c r="AE1005" s="1"/>
+      <c r="AF1005" s="1"/>
+      <c r="AG1005" s="1"/>
+      <c r="AH1005" s="1"/>
+      <c r="AI1005" s="1"/>
+      <c r="AJ1005" s="1"/>
+    </row>
+    <row r="1006" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="1"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="1"/>
+      <c r="G1006" s="1"/>
+      <c r="H1006" s="1"/>
+      <c r="I1006" s="1"/>
+      <c r="J1006" s="1"/>
+      <c r="K1006" s="1"/>
+      <c r="L1006" s="1"/>
+      <c r="M1006" s="1"/>
+      <c r="N1006" s="1"/>
+      <c r="O1006" s="1"/>
+      <c r="P1006" s="1"/>
+      <c r="Q1006" s="1"/>
+      <c r="R1006" s="1"/>
+      <c r="S1006" s="1"/>
+      <c r="T1006" s="1"/>
+      <c r="U1006" s="1"/>
+      <c r="V1006" s="1"/>
+      <c r="W1006" s="1"/>
+      <c r="X1006" s="1"/>
+      <c r="Y1006" s="1"/>
+      <c r="Z1006" s="1"/>
+      <c r="AA1006" s="1"/>
+      <c r="AB1006" s="1"/>
+      <c r="AC1006" s="1"/>
+      <c r="AD1006" s="1"/>
+      <c r="AE1006" s="1"/>
+      <c r="AF1006" s="1"/>
+      <c r="AG1006" s="1"/>
+      <c r="AH1006" s="1"/>
+      <c r="AI1006" s="1"/>
+      <c r="AJ1006" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="27">
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="F241:G241"/>
-    <mergeCell ref="F242:G242"/>
-    <mergeCell ref="L241:M241"/>
-    <mergeCell ref="O241:O242"/>
-    <mergeCell ref="L242:M242"/>
-    <mergeCell ref="A241:B241"/>
-    <mergeCell ref="A242:B242"/>
-    <mergeCell ref="AI241:AI242"/>
+    <mergeCell ref="F245:G245"/>
+    <mergeCell ref="F246:G246"/>
+    <mergeCell ref="L245:M245"/>
+    <mergeCell ref="O245:O246"/>
+    <mergeCell ref="L246:M246"/>
+    <mergeCell ref="A245:B245"/>
+    <mergeCell ref="A246:B246"/>
+    <mergeCell ref="AI245:AI246"/>
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AF241:AG241"/>
-    <mergeCell ref="AF242:AG242"/>
-    <mergeCell ref="AA241:AB241"/>
-    <mergeCell ref="AA242:AB242"/>
+    <mergeCell ref="AF245:AG245"/>
+    <mergeCell ref="AF246:AG246"/>
+    <mergeCell ref="AA245:AB245"/>
+    <mergeCell ref="AA246:AB246"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Q241:R241"/>
+    <mergeCell ref="Q245:R245"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="V241:W241"/>
-    <mergeCell ref="Y241:Y242"/>
-    <mergeCell ref="Q242:R242"/>
-    <mergeCell ref="V242:W242"/>
+    <mergeCell ref="V245:W245"/>
+    <mergeCell ref="Y245:Y246"/>
+    <mergeCell ref="Q246:R246"/>
+    <mergeCell ref="V246:W246"/>
     <mergeCell ref="Q1:S1"/>
   </mergeCells>
-  <conditionalFormatting sqref="AF3:AF237">
-    <cfRule type="cellIs" dxfId="49" priority="48" operator="greaterThan">
+  <conditionalFormatting sqref="AF3:AF242">
+    <cfRule type="cellIs" dxfId="42" priority="49" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF3:AF242">
+    <cfRule type="cellIs" dxfId="40" priority="50" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF3:AF242">
+    <cfRule type="cellIs" dxfId="39" priority="51" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF3:AF242">
+    <cfRule type="cellIs" dxfId="38" priority="52" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF3:AF237">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF3:AF237">
-    <cfRule type="cellIs" dxfId="47" priority="50" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF3:AF237">
-    <cfRule type="cellIs" dxfId="46" priority="51" operator="lessThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI241:AI242">
-    <cfRule type="cellIs" dxfId="45" priority="43" operator="lessThan">
+  <conditionalFormatting sqref="AI245:AI246">
+    <cfRule type="cellIs" dxfId="37" priority="44" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="44" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="45" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O241:O242">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="lessThan">
+  <conditionalFormatting sqref="O245:O246">
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3:AI237 O3:O237">
-    <cfRule type="cellIs" dxfId="41" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="46" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="46" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="47" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L237">
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="41" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y241:Y242">
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="lessThan">
+  <conditionalFormatting sqref="Y245:Y246">
+    <cfRule type="cellIs" dxfId="28" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="36" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y237">
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="38" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V237">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="32" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="34" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF238">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="greaterThan">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF238">
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF238">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF238">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="lessThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI238 O238">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="lessThan">
+  <conditionalFormatting sqref="AI238 O238 O240:O242 AI242">
+    <cfRule type="cellIs" dxfId="21" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L238">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="greaterThan">
+  <conditionalFormatting sqref="L238 L240:L242">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y238">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="lessThan">
+  <conditionalFormatting sqref="Y238 Y240:Y242">
+    <cfRule type="cellIs" dxfId="16" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="22" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V238">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="greaterThan">
+  <conditionalFormatting sqref="V238 V240:V242">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF239">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="greaterThan">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF239">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF239">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF239">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="lessThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI239 O239">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+  <conditionalFormatting sqref="O239 AI239:AI241">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L239">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y239">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V239">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D239">
+  <conditionalFormatting sqref="D3:D242">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Analises ILP com os novos casos de teste Koerkel Ghosh simetrico e assi
</commit_message>
<xml_diff>
--- a/solutions.xlsx
+++ b/solutions.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solutions1" localSheetId="0">Plan1!$F$2:$I$17</definedName>
-    <definedName name="solutions1_1" localSheetId="0">Plan1!$AA$3:$AC$17</definedName>
-    <definedName name="solutions1_2" localSheetId="0">Plan1!$Q$2:$S$17</definedName>
-    <definedName name="solutions2" localSheetId="0">Plan1!$Z$4:$AC$224</definedName>
-    <definedName name="solutions2_1" localSheetId="0">Plan1!$AA$18:$AC$237</definedName>
+    <definedName name="solutions1" localSheetId="1">Plan1!$F$2:$I$17</definedName>
+    <definedName name="solutions1_1" localSheetId="1">Plan1!$AA$3:$AC$17</definedName>
+    <definedName name="solutions1_2" localSheetId="1">Plan1!$Q$2:$S$17</definedName>
+    <definedName name="solutions2" localSheetId="1">Plan1!$Z$4:$AC$224</definedName>
+    <definedName name="solutions2_1" localSheetId="1">Plan1!$AA$18:$AC$237</definedName>
+    <definedName name="solutions2_2" localSheetId="0">Plan2!$A$1:$D$91</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -55,11 +57,21 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="solutions2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Macbook/Documents/GitKraken_Projects/ICAlgoritmos/gurobi/solutions2.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="348">
   <si>
     <t>ILP</t>
   </si>
@@ -834,6 +846,276 @@
   <si>
     <t>MIP - ILP</t>
   </si>
+  <si>
+    <t>ga250a-1</t>
+  </si>
+  <si>
+    <t>ga250a-2</t>
+  </si>
+  <si>
+    <t>ga250a-3</t>
+  </si>
+  <si>
+    <t>ga250a-4</t>
+  </si>
+  <si>
+    <t>ga250a-5</t>
+  </si>
+  <si>
+    <t>ga250b-1</t>
+  </si>
+  <si>
+    <t>ga250b-2</t>
+  </si>
+  <si>
+    <t>ga250b-3</t>
+  </si>
+  <si>
+    <t>ga250b-4</t>
+  </si>
+  <si>
+    <t>ga250b-5</t>
+  </si>
+  <si>
+    <t>ga250c-1</t>
+  </si>
+  <si>
+    <t>ga250c-2</t>
+  </si>
+  <si>
+    <t>ga250c-3</t>
+  </si>
+  <si>
+    <t>ga250c-4</t>
+  </si>
+  <si>
+    <t>ga250c-5</t>
+  </si>
+  <si>
+    <t>ga500a-1</t>
+  </si>
+  <si>
+    <t>ga500a-2</t>
+  </si>
+  <si>
+    <t>ga500a-3</t>
+  </si>
+  <si>
+    <t>ga500a-4</t>
+  </si>
+  <si>
+    <t>ga500a-5</t>
+  </si>
+  <si>
+    <t>ga500b-1</t>
+  </si>
+  <si>
+    <t>ga500b-2</t>
+  </si>
+  <si>
+    <t>ga500b-3</t>
+  </si>
+  <si>
+    <t>ga500b-4</t>
+  </si>
+  <si>
+    <t>ga500b-5</t>
+  </si>
+  <si>
+    <t>ga500c-1</t>
+  </si>
+  <si>
+    <t>ga500c-2</t>
+  </si>
+  <si>
+    <t>ga500c-3</t>
+  </si>
+  <si>
+    <t>ga500c-4</t>
+  </si>
+  <si>
+    <t>ga500c-5</t>
+  </si>
+  <si>
+    <t>ga750a-1</t>
+  </si>
+  <si>
+    <t>ga750a-2</t>
+  </si>
+  <si>
+    <t>ga750a-3</t>
+  </si>
+  <si>
+    <t>ga750a-4</t>
+  </si>
+  <si>
+    <t>ga750a-5</t>
+  </si>
+  <si>
+    <t>ga750b-1</t>
+  </si>
+  <si>
+    <t>ga750b-2</t>
+  </si>
+  <si>
+    <t>ga750b-3</t>
+  </si>
+  <si>
+    <t>ga750b-4</t>
+  </si>
+  <si>
+    <t>ga750b-5</t>
+  </si>
+  <si>
+    <t>ga750c-1</t>
+  </si>
+  <si>
+    <t>ga750c-2</t>
+  </si>
+  <si>
+    <t>ga750c-3</t>
+  </si>
+  <si>
+    <t>ga750c-4</t>
+  </si>
+  <si>
+    <t>ga750c-5</t>
+  </si>
+  <si>
+    <t>gs250a-1</t>
+  </si>
+  <si>
+    <t>gs250a-2</t>
+  </si>
+  <si>
+    <t>gs250a-3</t>
+  </si>
+  <si>
+    <t>gs250a-4</t>
+  </si>
+  <si>
+    <t>gs250a-5</t>
+  </si>
+  <si>
+    <t>gs250b-1</t>
+  </si>
+  <si>
+    <t>gs250b-2</t>
+  </si>
+  <si>
+    <t>gs250b-3</t>
+  </si>
+  <si>
+    <t>gs250b-4</t>
+  </si>
+  <si>
+    <t>gs250b-5</t>
+  </si>
+  <si>
+    <t>gs250c-1</t>
+  </si>
+  <si>
+    <t>gs250c-2</t>
+  </si>
+  <si>
+    <t>gs250c-3</t>
+  </si>
+  <si>
+    <t>gs250c-4</t>
+  </si>
+  <si>
+    <t>gs250c-5</t>
+  </si>
+  <si>
+    <t>gs500a-1</t>
+  </si>
+  <si>
+    <t>gs500a-2</t>
+  </si>
+  <si>
+    <t>gs500a-3</t>
+  </si>
+  <si>
+    <t>gs500a-4</t>
+  </si>
+  <si>
+    <t>gs500a-5</t>
+  </si>
+  <si>
+    <t>gs500b-1</t>
+  </si>
+  <si>
+    <t>gs500b-2</t>
+  </si>
+  <si>
+    <t>gs500b-3</t>
+  </si>
+  <si>
+    <t>gs500b-4</t>
+  </si>
+  <si>
+    <t>gs500b-5</t>
+  </si>
+  <si>
+    <t>gs500c-1</t>
+  </si>
+  <si>
+    <t>gs500c-2</t>
+  </si>
+  <si>
+    <t>gs500c-3</t>
+  </si>
+  <si>
+    <t>gs500c-4</t>
+  </si>
+  <si>
+    <t>gs500c-5</t>
+  </si>
+  <si>
+    <t>gs750a-1</t>
+  </si>
+  <si>
+    <t>gs750a-2</t>
+  </si>
+  <si>
+    <t>gs750a-3</t>
+  </si>
+  <si>
+    <t>gs750a-4</t>
+  </si>
+  <si>
+    <t>gs750a-5</t>
+  </si>
+  <si>
+    <t>gs750b-1</t>
+  </si>
+  <si>
+    <t>gs750b-2</t>
+  </si>
+  <si>
+    <t>gs750b-3</t>
+  </si>
+  <si>
+    <t>gs750b-4</t>
+  </si>
+  <si>
+    <t>gs750b-5</t>
+  </si>
+  <si>
+    <t>gs750c-1</t>
+  </si>
+  <si>
+    <t>gs750c-2</t>
+  </si>
+  <si>
+    <t>gs750c-3</t>
+  </si>
+  <si>
+    <t>gs750c-4</t>
+  </si>
+  <si>
+    <t>gs750c-5</t>
+  </si>
 </sst>
 </file>
 
@@ -1013,23 +1295,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1440,20 +1722,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
           <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1468,10 +1750,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions2_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -1738,10 +2024,1305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ1006"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N208" zoomScale="111" workbookViewId="0">
-      <selection activeCell="AB250" sqref="AB250"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D91"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2">
+        <v>257988</v>
+      </c>
+      <c r="C2">
+        <v>905.518512010574</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3">
+        <v>257502</v>
+      </c>
+      <c r="C3">
+        <v>902.75716519355694</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4">
+        <v>258182</v>
+      </c>
+      <c r="C4">
+        <v>903.18458223342896</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5">
+        <v>257987</v>
+      </c>
+      <c r="C5">
+        <v>902.67631506919804</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B6">
+        <v>258280</v>
+      </c>
+      <c r="C6">
+        <v>902.95274996757496</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B7">
+        <v>277387</v>
+      </c>
+      <c r="C7">
+        <v>902.45952630042996</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B8">
+        <v>276108</v>
+      </c>
+      <c r="C8">
+        <v>902.45691275596596</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9">
+        <v>277320</v>
+      </c>
+      <c r="C9">
+        <v>902.72219800949097</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B10">
+        <v>278647</v>
+      </c>
+      <c r="C10">
+        <v>902.727436780929</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B11">
+        <v>277579</v>
+      </c>
+      <c r="C11">
+        <v>902.81754302978504</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B12">
+        <v>341259</v>
+      </c>
+      <c r="C12">
+        <v>902.71302103996197</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13">
+        <v>334500</v>
+      </c>
+      <c r="C13">
+        <v>902.76530218124299</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>270</v>
+      </c>
+      <c r="B14">
+        <v>336912</v>
+      </c>
+      <c r="C14">
+        <v>902.78485202789295</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B15">
+        <v>333923</v>
+      </c>
+      <c r="C15">
+        <v>902.75450706481899</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B16">
+        <v>337657</v>
+      </c>
+      <c r="C16">
+        <v>902.712965011596</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>273</v>
+      </c>
+      <c r="B17">
+        <v>511857</v>
+      </c>
+      <c r="C17">
+        <v>911.37733507156304</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>274</v>
+      </c>
+      <c r="B18">
+        <v>511692</v>
+      </c>
+      <c r="C18">
+        <v>911.29974985122601</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B19">
+        <v>511164</v>
+      </c>
+      <c r="C19">
+        <v>909.99310088157597</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>276</v>
+      </c>
+      <c r="B20">
+        <v>511333</v>
+      </c>
+      <c r="C20">
+        <v>909.94816899299599</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>277</v>
+      </c>
+      <c r="B21">
+        <v>511659</v>
+      </c>
+      <c r="C21">
+        <v>909.94293403625397</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>278</v>
+      </c>
+      <c r="B22">
+        <v>544990</v>
+      </c>
+      <c r="C22">
+        <v>909.91394376754704</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>279</v>
+      </c>
+      <c r="B23">
+        <v>543833</v>
+      </c>
+      <c r="C23">
+        <v>909.87025308608997</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>280</v>
+      </c>
+      <c r="B24">
+        <v>544177</v>
+      </c>
+      <c r="C24">
+        <v>910.11111402511597</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>281</v>
+      </c>
+      <c r="B25">
+        <v>544017</v>
+      </c>
+      <c r="C25">
+        <v>909.91126084327698</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>282</v>
+      </c>
+      <c r="B26">
+        <v>542311</v>
+      </c>
+      <c r="C26">
+        <v>910.70027804374695</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>283</v>
+      </c>
+      <c r="B27">
+        <v>651242</v>
+      </c>
+      <c r="C27">
+        <v>909.854112148284</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>284</v>
+      </c>
+      <c r="B28">
+        <v>650678</v>
+      </c>
+      <c r="C28">
+        <v>909.89395713806096</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>285</v>
+      </c>
+      <c r="B29">
+        <v>635921</v>
+      </c>
+      <c r="C29">
+        <v>917.24749302863995</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>286</v>
+      </c>
+      <c r="B30">
+        <v>653109</v>
+      </c>
+      <c r="C30">
+        <v>914.40007305145195</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>287</v>
+      </c>
+      <c r="B31">
+        <v>656085</v>
+      </c>
+      <c r="C31">
+        <v>909.84456491470303</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>288</v>
+      </c>
+      <c r="B32">
+        <v>764497</v>
+      </c>
+      <c r="C32">
+        <v>922.48159003257695</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>289</v>
+      </c>
+      <c r="B33">
+        <v>764393</v>
+      </c>
+      <c r="C33">
+        <v>923.70001530647198</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>290</v>
+      </c>
+      <c r="B34">
+        <v>764683</v>
+      </c>
+      <c r="C34">
+        <v>922.49204611778202</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>291</v>
+      </c>
+      <c r="B35">
+        <v>765003</v>
+      </c>
+      <c r="C35">
+        <v>967.331067085266</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>292</v>
+      </c>
+      <c r="B36">
+        <v>764839</v>
+      </c>
+      <c r="C36">
+        <v>922.35739517211903</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>293</v>
+      </c>
+      <c r="B37">
+        <v>804333</v>
+      </c>
+      <c r="C37">
+        <v>922.56556200981095</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>294</v>
+      </c>
+      <c r="B38">
+        <v>803382</v>
+      </c>
+      <c r="C38">
+        <v>922.20214200019802</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>295</v>
+      </c>
+      <c r="B39">
+        <v>804625</v>
+      </c>
+      <c r="C39">
+        <v>922.59399294853199</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>296</v>
+      </c>
+      <c r="B40">
+        <v>806073</v>
+      </c>
+      <c r="C40">
+        <v>922.38513612747101</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>297</v>
+      </c>
+      <c r="B41">
+        <v>804822</v>
+      </c>
+      <c r="C41">
+        <v>922.39462590217499</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>298</v>
+      </c>
+      <c r="B42">
+        <v>8314623</v>
+      </c>
+      <c r="C42">
+        <v>922.52507877349797</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>299</v>
+      </c>
+      <c r="B43">
+        <v>8238967</v>
+      </c>
+      <c r="C43">
+        <v>922.15382504463196</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>300</v>
+      </c>
+      <c r="B44">
+        <v>8272022</v>
+      </c>
+      <c r="C44">
+        <v>922.41212320327702</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>301</v>
+      </c>
+      <c r="B45">
+        <v>8293624</v>
+      </c>
+      <c r="C45">
+        <v>922.37150001525799</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>302</v>
+      </c>
+      <c r="B46">
+        <v>8113598</v>
+      </c>
+      <c r="C46">
+        <v>922.51200389862004</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>303</v>
+      </c>
+      <c r="B47">
+        <v>257982</v>
+      </c>
+      <c r="C47">
+        <v>902.45427799224797</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>304</v>
+      </c>
+      <c r="B48">
+        <v>257573</v>
+      </c>
+      <c r="C48">
+        <v>902.71455574035599</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>305</v>
+      </c>
+      <c r="B49">
+        <v>257637</v>
+      </c>
+      <c r="C49">
+        <v>902.45287489890995</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>306</v>
+      </c>
+      <c r="B50">
+        <v>258002</v>
+      </c>
+      <c r="C50">
+        <v>902.86888289451599</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>307</v>
+      </c>
+      <c r="B51">
+        <v>257947</v>
+      </c>
+      <c r="C51">
+        <v>902.55648112297001</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>308</v>
+      </c>
+      <c r="B52">
+        <v>277963</v>
+      </c>
+      <c r="C52">
+        <v>902.70880317687897</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>309</v>
+      </c>
+      <c r="B53">
+        <v>277186</v>
+      </c>
+      <c r="C53">
+        <v>902.76570177078202</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>310</v>
+      </c>
+      <c r="B54">
+        <v>277318</v>
+      </c>
+      <c r="C54">
+        <v>903.03716206550598</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>311</v>
+      </c>
+      <c r="B55">
+        <v>277503</v>
+      </c>
+      <c r="C55">
+        <v>903.02846908569302</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>312</v>
+      </c>
+      <c r="B56">
+        <v>277660</v>
+      </c>
+      <c r="C56">
+        <v>902.86114811897198</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>313</v>
+      </c>
+      <c r="B57">
+        <v>335250</v>
+      </c>
+      <c r="C57">
+        <v>902.81879806518498</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>314</v>
+      </c>
+      <c r="B58">
+        <v>337978</v>
+      </c>
+      <c r="C58">
+        <v>902.66474580764702</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>315</v>
+      </c>
+      <c r="B59">
+        <v>334568</v>
+      </c>
+      <c r="C59">
+        <v>902.43451786041203</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>316</v>
+      </c>
+      <c r="B60">
+        <v>336775</v>
+      </c>
+      <c r="C60">
+        <v>902.83008790016095</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>317</v>
+      </c>
+      <c r="B61">
+        <v>336807</v>
+      </c>
+      <c r="C61">
+        <v>902.78700304031304</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>318</v>
+      </c>
+      <c r="B62">
+        <v>511596</v>
+      </c>
+      <c r="C62">
+        <v>911.28729915618896</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>319</v>
+      </c>
+      <c r="B63">
+        <v>511543</v>
+      </c>
+      <c r="C63">
+        <v>911.35703802108696</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>320</v>
+      </c>
+      <c r="B64">
+        <v>511820</v>
+      </c>
+      <c r="C64">
+        <v>910.53267502784695</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>321</v>
+      </c>
+      <c r="B65">
+        <v>511720</v>
+      </c>
+      <c r="C65">
+        <v>911.17584109306301</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>322</v>
+      </c>
+      <c r="B66">
+        <v>511896</v>
+      </c>
+      <c r="C66">
+        <v>911.82793593406598</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>323</v>
+      </c>
+      <c r="B67">
+        <v>543113</v>
+      </c>
+      <c r="C67">
+        <v>910.08405399322498</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>324</v>
+      </c>
+      <c r="B68">
+        <v>544757</v>
+      </c>
+      <c r="C68">
+        <v>910.17574715614296</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>325</v>
+      </c>
+      <c r="B69">
+        <v>545082</v>
+      </c>
+      <c r="C69">
+        <v>910.02588105201698</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>326</v>
+      </c>
+      <c r="B70">
+        <v>544587</v>
+      </c>
+      <c r="C70">
+        <v>910.35155200958195</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>327</v>
+      </c>
+      <c r="B71">
+        <v>543683</v>
+      </c>
+      <c r="C71">
+        <v>910.50993108749299</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>328</v>
+      </c>
+      <c r="B72">
+        <v>650774</v>
+      </c>
+      <c r="C72">
+        <v>911.23421382903996</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>329</v>
+      </c>
+      <c r="B73">
+        <v>652789</v>
+      </c>
+      <c r="C73">
+        <v>911.64885783195496</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>330</v>
+      </c>
+      <c r="B74">
+        <v>651278</v>
+      </c>
+      <c r="C74">
+        <v>911.36014986038197</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>331</v>
+      </c>
+      <c r="B75">
+        <v>650240</v>
+      </c>
+      <c r="C75">
+        <v>911.308551073074</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>332</v>
+      </c>
+      <c r="B76">
+        <v>653596</v>
+      </c>
+      <c r="C76">
+        <v>910.14066624641396</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>333</v>
+      </c>
+      <c r="B77">
+        <v>764489</v>
+      </c>
+      <c r="C77">
+        <v>925.529658079147</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>334</v>
+      </c>
+      <c r="B78">
+        <v>764323</v>
+      </c>
+      <c r="C78">
+        <v>922.64379024505604</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>335</v>
+      </c>
+      <c r="B79">
+        <v>764514</v>
+      </c>
+      <c r="C79">
+        <v>943.27610707282997</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>336</v>
+      </c>
+      <c r="B80">
+        <v>764778</v>
+      </c>
+      <c r="C80">
+        <v>1000.9630742073</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>337</v>
+      </c>
+      <c r="B81">
+        <v>764518</v>
+      </c>
+      <c r="C81">
+        <v>923.41966295242298</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>338</v>
+      </c>
+      <c r="B82">
+        <v>805705</v>
+      </c>
+      <c r="C82">
+        <v>923.70170497894196</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>339</v>
+      </c>
+      <c r="B83">
+        <v>804801</v>
+      </c>
+      <c r="C83">
+        <v>925.14163589477505</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>340</v>
+      </c>
+      <c r="B84">
+        <v>806007</v>
+      </c>
+      <c r="C84">
+        <v>926.23342895507801</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>341</v>
+      </c>
+      <c r="B85">
+        <v>804453</v>
+      </c>
+      <c r="C85">
+        <v>925.72512578964199</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>342</v>
+      </c>
+      <c r="B86">
+        <v>805745</v>
+      </c>
+      <c r="C86">
+        <v>926.446646928787</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>343</v>
+      </c>
+      <c r="B87">
+        <v>8243622</v>
+      </c>
+      <c r="C87">
+        <v>926.22148108482304</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>344</v>
+      </c>
+      <c r="B88">
+        <v>8373748</v>
+      </c>
+      <c r="C88">
+        <v>925.34666800498906</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>345</v>
+      </c>
+      <c r="B89">
+        <v>8264997</v>
+      </c>
+      <c r="C89">
+        <v>925.06150794029202</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>346</v>
+      </c>
+      <c r="B90">
+        <v>8320376</v>
+      </c>
+      <c r="C90">
+        <v>927.86582994461003</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>347</v>
+      </c>
+      <c r="B91">
+        <v>8384003</v>
+      </c>
+      <c r="C91">
+        <v>924.673907995224</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ1096"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="111" workbookViewId="0">
+      <selection activeCell="H252" sqref="H252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1770,58 +3351,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="23"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="23"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="23"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="22" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="23"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
       <c r="T1" s="15"/>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="V1" s="23"/>
       <c r="W1" s="1"/>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="22" t="s">
         <v>2</v>
       </c>
       <c r="Y1" s="23"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="AB1" s="28"/>
+      <c r="AB1" s="27"/>
       <c r="AC1" s="23"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="27" t="s">
+      <c r="AE1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="AF1" s="23"/>
       <c r="AG1" s="1"/>
-      <c r="AH1" s="27" t="s">
+      <c r="AH1" s="22" t="s">
         <v>2</v>
       </c>
       <c r="AI1" s="23"/>
@@ -21589,7 +23170,7 @@
         <v>20898</v>
       </c>
       <c r="AF195" s="8">
-        <f t="shared" ref="AF195:AF242" si="48">AE195/B195</f>
+        <f t="shared" ref="AF195:AF241" si="48">AE195/B195</f>
         <v>0.58454308970378455</v>
       </c>
       <c r="AG195" s="1"/>
@@ -26289,11 +27870,33 @@
       <c r="AI242" s="8"/>
       <c r="AJ242" s="1"/>
     </row>
+    <row r="243" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B243" s="10">
+        <v>257988</v>
+      </c>
+      <c r="C243" s="10">
+        <v>905.518512010574</v>
+      </c>
+      <c r="D243" s="10">
+        <v>0</v>
+      </c>
+    </row>
     <row r="244" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A244" s="1"/>
-      <c r="B244" s="1"/>
-      <c r="C244" s="1"/>
-      <c r="D244" s="1"/>
+      <c r="A244" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B244" s="10">
+        <v>257502</v>
+      </c>
+      <c r="C244" s="10">
+        <v>902.75716519355694</v>
+      </c>
+      <c r="D244" s="10">
+        <v>0</v>
+      </c>
       <c r="E244" s="1"/>
       <c r="F244" s="1"/>
       <c r="G244" s="1"/>
@@ -26328,17 +27931,20 @@
       <c r="AJ244" s="1"/>
     </row>
     <row r="245" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A245" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="B245" s="23"/>
-      <c r="C245" s="7">
-        <f>SUM(C3:C242)</f>
-        <v>11757.668949604795</v>
-      </c>
-      <c r="D245" s="1"/>
+      <c r="A245" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="B245" s="10">
+        <v>258182</v>
+      </c>
+      <c r="C245" s="10">
+        <v>903.18458223342896</v>
+      </c>
+      <c r="D245" s="10">
+        <v>0</v>
+      </c>
       <c r="E245" s="1"/>
-      <c r="F245" s="22" t="s">
+      <c r="F245" s="24" t="s">
         <v>244</v>
       </c>
       <c r="G245" s="23"/>
@@ -26349,20 +27955,20 @@
       <c r="I245" s="1"/>
       <c r="J245" s="1"/>
       <c r="K245" s="1"/>
-      <c r="L245" s="22" t="s">
+      <c r="L245" s="24" t="s">
         <v>245</v>
       </c>
       <c r="M245" s="23"/>
       <c r="N245" s="7">
-        <f>H245-C245</f>
+        <f>H245-C335</f>
         <v>-11315.203019142911</v>
       </c>
-      <c r="O245" s="24">
-        <f>N245/C245</f>
+      <c r="O245" s="25">
+        <f>N245/C335</f>
         <v>-0.96236788666542994</v>
       </c>
       <c r="P245" s="1"/>
-      <c r="Q245" s="22" t="s">
+      <c r="Q245" s="24" t="s">
         <v>244</v>
       </c>
       <c r="R245" s="23"/>
@@ -26372,20 +27978,20 @@
       </c>
       <c r="T245" s="1"/>
       <c r="U245" s="1"/>
-      <c r="V245" s="22" t="s">
+      <c r="V245" s="24" t="s">
         <v>245</v>
       </c>
       <c r="W245" s="23"/>
       <c r="X245" s="7">
-        <f>S245-C245</f>
+        <f>S245-C335</f>
         <v>-10758.029428244399</v>
       </c>
-      <c r="Y245" s="24">
-        <f>X245/C245</f>
+      <c r="Y245" s="25">
+        <f>X245/C335</f>
         <v>-0.91497978675492508</v>
       </c>
       <c r="Z245" s="1"/>
-      <c r="AA245" s="22" t="s">
+      <c r="AA245" s="24" t="s">
         <v>244</v>
       </c>
       <c r="AB245" s="23"/>
@@ -26395,32 +28001,35 @@
       </c>
       <c r="AD245" s="1"/>
       <c r="AE245" s="1"/>
-      <c r="AF245" s="22" t="s">
+      <c r="AF245" s="24" t="s">
         <v>245</v>
       </c>
       <c r="AG245" s="23"/>
       <c r="AH245" s="7">
-        <f>AC245-C245</f>
+        <f>AC245-C335</f>
         <v>-5312.7672976047943</v>
       </c>
-      <c r="AI245" s="24">
-        <f>AH245/C245</f>
+      <c r="AI245" s="25">
+        <f>AH245/C335</f>
         <v>-0.45185549281716847</v>
       </c>
       <c r="AJ245" s="1"/>
     </row>
     <row r="246" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A246" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="B246" s="23"/>
-      <c r="C246" s="7">
-        <f>C245/60</f>
-        <v>195.96114916007991</v>
-      </c>
-      <c r="D246" s="1"/>
+      <c r="A246" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B246" s="10">
+        <v>257987</v>
+      </c>
+      <c r="C246" s="10">
+        <v>902.67631506919804</v>
+      </c>
+      <c r="D246" s="10">
+        <v>0</v>
+      </c>
       <c r="E246" s="1"/>
-      <c r="F246" s="22" t="s">
+      <c r="F246" s="24" t="s">
         <v>246</v>
       </c>
       <c r="G246" s="23"/>
@@ -26431,17 +28040,17 @@
       <c r="I246" s="1"/>
       <c r="J246" s="1"/>
       <c r="K246" s="1"/>
-      <c r="L246" s="22" t="s">
+      <c r="L246" s="24" t="s">
         <v>247</v>
       </c>
       <c r="M246" s="23"/>
       <c r="N246" s="7">
-        <f>H246-C246</f>
+        <f>H246-C336</f>
         <v>-188.58671698571519</v>
       </c>
-      <c r="O246" s="25"/>
+      <c r="O246" s="26"/>
       <c r="P246" s="1"/>
-      <c r="Q246" s="22" t="s">
+      <c r="Q246" s="24" t="s">
         <v>246</v>
       </c>
       <c r="R246" s="23"/>
@@ -26451,17 +28060,17 @@
       </c>
       <c r="T246" s="1"/>
       <c r="U246" s="1"/>
-      <c r="V246" s="22" t="s">
+      <c r="V246" s="24" t="s">
         <v>247</v>
       </c>
       <c r="W246" s="23"/>
       <c r="X246" s="7">
-        <f>S246-C246</f>
+        <f>S246-C336</f>
         <v>-179.30049047073999</v>
       </c>
-      <c r="Y246" s="25"/>
+      <c r="Y246" s="26"/>
       <c r="Z246" s="1"/>
-      <c r="AA246" s="22" t="s">
+      <c r="AA246" s="24" t="s">
         <v>246</v>
       </c>
       <c r="AB246" s="23"/>
@@ -26471,22 +28080,30 @@
       </c>
       <c r="AD246" s="1"/>
       <c r="AE246" s="1"/>
-      <c r="AF246" s="22" t="s">
+      <c r="AF246" s="24" t="s">
         <v>247</v>
       </c>
       <c r="AG246" s="23"/>
       <c r="AH246" s="7">
-        <f>AC246-C246</f>
+        <f>AC246-C336</f>
         <v>-88.546121626746569</v>
       </c>
-      <c r="AI246" s="25"/>
+      <c r="AI246" s="26"/>
       <c r="AJ246" s="1"/>
     </row>
     <row r="247" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A247" s="1"/>
-      <c r="B247" s="1"/>
-      <c r="C247" s="1"/>
-      <c r="D247" s="1"/>
+      <c r="A247" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="B247" s="10">
+        <v>258280</v>
+      </c>
+      <c r="C247" s="10">
+        <v>902.95274996757496</v>
+      </c>
+      <c r="D247" s="10">
+        <v>0</v>
+      </c>
       <c r="E247" s="1"/>
       <c r="F247" s="1"/>
       <c r="G247" s="1"/>
@@ -26521,10 +28138,18 @@
       <c r="AJ247" s="1"/>
     </row>
     <row r="248" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A248" s="1"/>
-      <c r="B248" s="1"/>
-      <c r="C248" s="1"/>
-      <c r="D248" s="1"/>
+      <c r="A248" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B248" s="10">
+        <v>277387</v>
+      </c>
+      <c r="C248" s="10">
+        <v>902.45952630042996</v>
+      </c>
+      <c r="D248" s="10">
+        <v>0</v>
+      </c>
       <c r="E248" s="1"/>
       <c r="F248" s="1"/>
       <c r="G248" s="1"/>
@@ -26559,10 +28184,18 @@
       <c r="AJ248" s="1"/>
     </row>
     <row r="249" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A249" s="1"/>
-      <c r="B249" s="1"/>
-      <c r="C249" s="1"/>
-      <c r="D249" s="1"/>
+      <c r="A249" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B249" s="10">
+        <v>276108</v>
+      </c>
+      <c r="C249" s="10">
+        <v>902.45691275596596</v>
+      </c>
+      <c r="D249" s="10">
+        <v>0</v>
+      </c>
       <c r="E249" s="1"/>
       <c r="F249" s="1"/>
       <c r="G249" s="1"/>
@@ -26597,10 +28230,18 @@
       <c r="AJ249" s="1"/>
     </row>
     <row r="250" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A250" s="1"/>
-      <c r="B250" s="1"/>
-      <c r="C250" s="1"/>
-      <c r="D250" s="1"/>
+      <c r="A250" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B250" s="10">
+        <v>277320</v>
+      </c>
+      <c r="C250" s="10">
+        <v>902.72219800949097</v>
+      </c>
+      <c r="D250" s="10">
+        <v>0</v>
+      </c>
       <c r="E250" s="1"/>
       <c r="F250" s="1"/>
       <c r="G250" s="1"/>
@@ -26635,10 +28276,18 @@
       <c r="AJ250" s="1"/>
     </row>
     <row r="251" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A251" s="1"/>
-      <c r="B251" s="1"/>
-      <c r="C251" s="1"/>
-      <c r="D251" s="1"/>
+      <c r="A251" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B251" s="10">
+        <v>278647</v>
+      </c>
+      <c r="C251" s="10">
+        <v>902.727436780929</v>
+      </c>
+      <c r="D251" s="10">
+        <v>0</v>
+      </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1"/>
       <c r="G251" s="1"/>
@@ -26673,10 +28322,18 @@
       <c r="AJ251" s="1"/>
     </row>
     <row r="252" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A252" s="1"/>
-      <c r="B252" s="1"/>
-      <c r="C252" s="1"/>
-      <c r="D252" s="1"/>
+      <c r="A252" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B252" s="10">
+        <v>277579</v>
+      </c>
+      <c r="C252" s="10">
+        <v>902.81754302978504</v>
+      </c>
+      <c r="D252" s="10">
+        <v>0</v>
+      </c>
       <c r="E252" s="1"/>
       <c r="F252" s="1"/>
       <c r="G252" s="1"/>
@@ -26711,10 +28368,18 @@
       <c r="AJ252" s="1"/>
     </row>
     <row r="253" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A253" s="1"/>
-      <c r="B253" s="1"/>
-      <c r="C253" s="1"/>
-      <c r="D253" s="1"/>
+      <c r="A253" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B253" s="10">
+        <v>341259</v>
+      </c>
+      <c r="C253" s="10">
+        <v>902.71302103996197</v>
+      </c>
+      <c r="D253" s="10">
+        <v>0</v>
+      </c>
       <c r="E253" s="1"/>
       <c r="F253" s="1"/>
       <c r="G253" s="1"/>
@@ -26749,10 +28414,18 @@
       <c r="AJ253" s="1"/>
     </row>
     <row r="254" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A254" s="1"/>
-      <c r="B254" s="1"/>
-      <c r="C254" s="1"/>
-      <c r="D254" s="1"/>
+      <c r="A254" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B254" s="10">
+        <v>334500</v>
+      </c>
+      <c r="C254" s="10">
+        <v>902.76530218124299</v>
+      </c>
+      <c r="D254" s="10">
+        <v>0</v>
+      </c>
       <c r="E254" s="1"/>
       <c r="F254" s="1"/>
       <c r="G254" s="1"/>
@@ -26787,10 +28460,18 @@
       <c r="AJ254" s="1"/>
     </row>
     <row r="255" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A255" s="1"/>
-      <c r="B255" s="1"/>
-      <c r="C255" s="1"/>
-      <c r="D255" s="1"/>
+      <c r="A255" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B255" s="10">
+        <v>336912</v>
+      </c>
+      <c r="C255" s="10">
+        <v>902.78485202789295</v>
+      </c>
+      <c r="D255" s="10">
+        <v>0</v>
+      </c>
       <c r="E255" s="1"/>
       <c r="F255" s="1"/>
       <c r="G255" s="1"/>
@@ -26825,10 +28506,18 @@
       <c r="AJ255" s="1"/>
     </row>
     <row r="256" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A256" s="1"/>
-      <c r="B256" s="1"/>
-      <c r="C256" s="1"/>
-      <c r="D256" s="1"/>
+      <c r="A256" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B256" s="10">
+        <v>333923</v>
+      </c>
+      <c r="C256" s="10">
+        <v>902.75450706481899</v>
+      </c>
+      <c r="D256" s="10">
+        <v>0</v>
+      </c>
       <c r="E256" s="1"/>
       <c r="F256" s="1"/>
       <c r="G256" s="1"/>
@@ -26863,10 +28552,18 @@
       <c r="AJ256" s="1"/>
     </row>
     <row r="257" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A257" s="1"/>
-      <c r="B257" s="1"/>
-      <c r="C257" s="1"/>
-      <c r="D257" s="1"/>
+      <c r="A257" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B257" s="10">
+        <v>337657</v>
+      </c>
+      <c r="C257" s="10">
+        <v>902.712965011596</v>
+      </c>
+      <c r="D257" s="10">
+        <v>0</v>
+      </c>
       <c r="E257" s="1"/>
       <c r="F257" s="1"/>
       <c r="G257" s="1"/>
@@ -26901,10 +28598,18 @@
       <c r="AJ257" s="1"/>
     </row>
     <row r="258" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A258" s="1"/>
-      <c r="B258" s="1"/>
-      <c r="C258" s="1"/>
-      <c r="D258" s="1"/>
+      <c r="A258" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B258" s="10">
+        <v>511857</v>
+      </c>
+      <c r="C258" s="10">
+        <v>911.37733507156304</v>
+      </c>
+      <c r="D258" s="10">
+        <v>0</v>
+      </c>
       <c r="E258" s="1"/>
       <c r="F258" s="1"/>
       <c r="G258" s="1"/>
@@ -26939,10 +28644,18 @@
       <c r="AJ258" s="1"/>
     </row>
     <row r="259" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A259" s="1"/>
-      <c r="B259" s="1"/>
-      <c r="C259" s="1"/>
-      <c r="D259" s="1"/>
+      <c r="A259" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B259" s="10">
+        <v>511692</v>
+      </c>
+      <c r="C259" s="10">
+        <v>911.29974985122601</v>
+      </c>
+      <c r="D259" s="10">
+        <v>0</v>
+      </c>
       <c r="E259" s="1"/>
       <c r="F259" s="1"/>
       <c r="G259" s="1"/>
@@ -26977,10 +28690,18 @@
       <c r="AJ259" s="1"/>
     </row>
     <row r="260" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A260" s="1"/>
-      <c r="B260" s="1"/>
-      <c r="C260" s="1"/>
-      <c r="D260" s="1"/>
+      <c r="A260" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B260" s="10">
+        <v>511164</v>
+      </c>
+      <c r="C260" s="10">
+        <v>909.99310088157597</v>
+      </c>
+      <c r="D260" s="10">
+        <v>0</v>
+      </c>
       <c r="E260" s="1"/>
       <c r="F260" s="1"/>
       <c r="G260" s="1"/>
@@ -27015,10 +28736,18 @@
       <c r="AJ260" s="1"/>
     </row>
     <row r="261" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A261" s="1"/>
-      <c r="B261" s="1"/>
-      <c r="C261" s="1"/>
-      <c r="D261" s="1"/>
+      <c r="A261" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B261" s="10">
+        <v>511333</v>
+      </c>
+      <c r="C261" s="10">
+        <v>909.94816899299599</v>
+      </c>
+      <c r="D261" s="10">
+        <v>0</v>
+      </c>
       <c r="E261" s="1"/>
       <c r="F261" s="1"/>
       <c r="G261" s="1"/>
@@ -27053,10 +28782,18 @@
       <c r="AJ261" s="1"/>
     </row>
     <row r="262" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A262" s="1"/>
-      <c r="B262" s="1"/>
-      <c r="C262" s="1"/>
-      <c r="D262" s="1"/>
+      <c r="A262" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B262" s="10">
+        <v>511659</v>
+      </c>
+      <c r="C262" s="10">
+        <v>909.94293403625397</v>
+      </c>
+      <c r="D262" s="10">
+        <v>0</v>
+      </c>
       <c r="E262" s="1"/>
       <c r="F262" s="1"/>
       <c r="G262" s="1"/>
@@ -27091,10 +28828,18 @@
       <c r="AJ262" s="1"/>
     </row>
     <row r="263" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A263" s="1"/>
-      <c r="B263" s="1"/>
-      <c r="C263" s="1"/>
-      <c r="D263" s="1"/>
+      <c r="A263" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="B263" s="10">
+        <v>544990</v>
+      </c>
+      <c r="C263" s="10">
+        <v>909.91394376754704</v>
+      </c>
+      <c r="D263" s="10">
+        <v>0</v>
+      </c>
       <c r="E263" s="1"/>
       <c r="F263" s="1"/>
       <c r="G263" s="1"/>
@@ -27129,10 +28874,18 @@
       <c r="AJ263" s="1"/>
     </row>
     <row r="264" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A264" s="1"/>
-      <c r="B264" s="1"/>
-      <c r="C264" s="1"/>
-      <c r="D264" s="1"/>
+      <c r="A264" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B264" s="10">
+        <v>543833</v>
+      </c>
+      <c r="C264" s="10">
+        <v>909.87025308608997</v>
+      </c>
+      <c r="D264" s="10">
+        <v>0</v>
+      </c>
       <c r="E264" s="1"/>
       <c r="F264" s="1"/>
       <c r="G264" s="1"/>
@@ -27167,10 +28920,18 @@
       <c r="AJ264" s="1"/>
     </row>
     <row r="265" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A265" s="1"/>
-      <c r="B265" s="1"/>
-      <c r="C265" s="1"/>
-      <c r="D265" s="1"/>
+      <c r="A265" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B265" s="10">
+        <v>544177</v>
+      </c>
+      <c r="C265" s="10">
+        <v>910.11111402511597</v>
+      </c>
+      <c r="D265" s="10">
+        <v>0</v>
+      </c>
       <c r="E265" s="1"/>
       <c r="F265" s="1"/>
       <c r="G265" s="1"/>
@@ -27205,10 +28966,18 @@
       <c r="AJ265" s="1"/>
     </row>
     <row r="266" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A266" s="1"/>
-      <c r="B266" s="1"/>
-      <c r="C266" s="1"/>
-      <c r="D266" s="1"/>
+      <c r="A266" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B266" s="10">
+        <v>544017</v>
+      </c>
+      <c r="C266" s="10">
+        <v>909.91126084327698</v>
+      </c>
+      <c r="D266" s="10">
+        <v>0</v>
+      </c>
       <c r="E266" s="1"/>
       <c r="F266" s="1"/>
       <c r="G266" s="1"/>
@@ -27243,10 +29012,18 @@
       <c r="AJ266" s="1"/>
     </row>
     <row r="267" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A267" s="1"/>
-      <c r="B267" s="1"/>
-      <c r="C267" s="1"/>
-      <c r="D267" s="1"/>
+      <c r="A267" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B267" s="10">
+        <v>542311</v>
+      </c>
+      <c r="C267" s="10">
+        <v>910.70027804374695</v>
+      </c>
+      <c r="D267" s="10">
+        <v>0</v>
+      </c>
       <c r="E267" s="1"/>
       <c r="F267" s="1"/>
       <c r="G267" s="1"/>
@@ -27281,10 +29058,18 @@
       <c r="AJ267" s="1"/>
     </row>
     <row r="268" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A268" s="1"/>
-      <c r="B268" s="1"/>
-      <c r="C268" s="1"/>
-      <c r="D268" s="1"/>
+      <c r="A268" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B268" s="10">
+        <v>651242</v>
+      </c>
+      <c r="C268" s="10">
+        <v>909.854112148284</v>
+      </c>
+      <c r="D268" s="10">
+        <v>0</v>
+      </c>
       <c r="E268" s="1"/>
       <c r="F268" s="1"/>
       <c r="G268" s="1"/>
@@ -27319,10 +29104,18 @@
       <c r="AJ268" s="1"/>
     </row>
     <row r="269" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A269" s="1"/>
-      <c r="B269" s="1"/>
-      <c r="C269" s="1"/>
-      <c r="D269" s="1"/>
+      <c r="A269" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B269" s="10">
+        <v>650678</v>
+      </c>
+      <c r="C269" s="10">
+        <v>909.89395713806096</v>
+      </c>
+      <c r="D269" s="10">
+        <v>0</v>
+      </c>
       <c r="E269" s="1"/>
       <c r="F269" s="1"/>
       <c r="G269" s="1"/>
@@ -27357,10 +29150,18 @@
       <c r="AJ269" s="1"/>
     </row>
     <row r="270" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A270" s="1"/>
-      <c r="B270" s="1"/>
-      <c r="C270" s="1"/>
-      <c r="D270" s="1"/>
+      <c r="A270" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B270" s="10">
+        <v>635921</v>
+      </c>
+      <c r="C270" s="10">
+        <v>917.24749302863995</v>
+      </c>
+      <c r="D270" s="10">
+        <v>0</v>
+      </c>
       <c r="E270" s="1"/>
       <c r="F270" s="1"/>
       <c r="G270" s="1"/>
@@ -27395,10 +29196,18 @@
       <c r="AJ270" s="1"/>
     </row>
     <row r="271" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A271" s="1"/>
-      <c r="B271" s="1"/>
-      <c r="C271" s="1"/>
-      <c r="D271" s="1"/>
+      <c r="A271" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B271" s="10">
+        <v>653109</v>
+      </c>
+      <c r="C271" s="10">
+        <v>914.40007305145195</v>
+      </c>
+      <c r="D271" s="10">
+        <v>0</v>
+      </c>
       <c r="E271" s="1"/>
       <c r="F271" s="1"/>
       <c r="G271" s="1"/>
@@ -27433,10 +29242,18 @@
       <c r="AJ271" s="1"/>
     </row>
     <row r="272" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A272" s="1"/>
-      <c r="B272" s="1"/>
-      <c r="C272" s="1"/>
-      <c r="D272" s="1"/>
+      <c r="A272" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="B272" s="10">
+        <v>656085</v>
+      </c>
+      <c r="C272" s="10">
+        <v>909.84456491470303</v>
+      </c>
+      <c r="D272" s="10">
+        <v>0</v>
+      </c>
       <c r="E272" s="1"/>
       <c r="F272" s="1"/>
       <c r="G272" s="1"/>
@@ -27471,10 +29288,18 @@
       <c r="AJ272" s="1"/>
     </row>
     <row r="273" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A273" s="1"/>
-      <c r="B273" s="1"/>
-      <c r="C273" s="1"/>
-      <c r="D273" s="1"/>
+      <c r="A273" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B273" s="10">
+        <v>764497</v>
+      </c>
+      <c r="C273" s="10">
+        <v>922.48159003257695</v>
+      </c>
+      <c r="D273" s="10">
+        <v>0</v>
+      </c>
       <c r="E273" s="1"/>
       <c r="F273" s="1"/>
       <c r="G273" s="1"/>
@@ -27509,10 +29334,18 @@
       <c r="AJ273" s="1"/>
     </row>
     <row r="274" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A274" s="1"/>
-      <c r="B274" s="1"/>
-      <c r="C274" s="1"/>
-      <c r="D274" s="1"/>
+      <c r="A274" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B274" s="10">
+        <v>764393</v>
+      </c>
+      <c r="C274" s="10">
+        <v>923.70001530647198</v>
+      </c>
+      <c r="D274" s="10">
+        <v>0</v>
+      </c>
       <c r="E274" s="1"/>
       <c r="F274" s="1"/>
       <c r="G274" s="1"/>
@@ -27547,10 +29380,18 @@
       <c r="AJ274" s="1"/>
     </row>
     <row r="275" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A275" s="1"/>
-      <c r="B275" s="1"/>
-      <c r="C275" s="1"/>
-      <c r="D275" s="1"/>
+      <c r="A275" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B275" s="10">
+        <v>764683</v>
+      </c>
+      <c r="C275" s="10">
+        <v>922.49204611778202</v>
+      </c>
+      <c r="D275" s="10">
+        <v>0</v>
+      </c>
       <c r="E275" s="1"/>
       <c r="F275" s="1"/>
       <c r="G275" s="1"/>
@@ -27585,10 +29426,18 @@
       <c r="AJ275" s="1"/>
     </row>
     <row r="276" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A276" s="1"/>
-      <c r="B276" s="1"/>
-      <c r="C276" s="1"/>
-      <c r="D276" s="1"/>
+      <c r="A276" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="B276" s="10">
+        <v>765003</v>
+      </c>
+      <c r="C276" s="10">
+        <v>967.331067085266</v>
+      </c>
+      <c r="D276" s="10">
+        <v>0</v>
+      </c>
       <c r="E276" s="1"/>
       <c r="F276" s="1"/>
       <c r="G276" s="1"/>
@@ -27623,10 +29472,18 @@
       <c r="AJ276" s="1"/>
     </row>
     <row r="277" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A277" s="1"/>
-      <c r="B277" s="1"/>
-      <c r="C277" s="1"/>
-      <c r="D277" s="1"/>
+      <c r="A277" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B277" s="10">
+        <v>764839</v>
+      </c>
+      <c r="C277" s="10">
+        <v>922.35739517211903</v>
+      </c>
+      <c r="D277" s="10">
+        <v>0</v>
+      </c>
       <c r="E277" s="1"/>
       <c r="F277" s="1"/>
       <c r="G277" s="1"/>
@@ -27661,10 +29518,18 @@
       <c r="AJ277" s="1"/>
     </row>
     <row r="278" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A278" s="1"/>
-      <c r="B278" s="1"/>
-      <c r="C278" s="1"/>
-      <c r="D278" s="1"/>
+      <c r="A278" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B278" s="10">
+        <v>804333</v>
+      </c>
+      <c r="C278" s="10">
+        <v>922.56556200981095</v>
+      </c>
+      <c r="D278" s="10">
+        <v>0</v>
+      </c>
       <c r="E278" s="1"/>
       <c r="F278" s="1"/>
       <c r="G278" s="1"/>
@@ -27699,10 +29564,18 @@
       <c r="AJ278" s="1"/>
     </row>
     <row r="279" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A279" s="1"/>
-      <c r="B279" s="1"/>
-      <c r="C279" s="1"/>
-      <c r="D279" s="1"/>
+      <c r="A279" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B279" s="10">
+        <v>803382</v>
+      </c>
+      <c r="C279" s="10">
+        <v>922.20214200019802</v>
+      </c>
+      <c r="D279" s="10">
+        <v>0</v>
+      </c>
       <c r="E279" s="1"/>
       <c r="F279" s="1"/>
       <c r="G279" s="1"/>
@@ -27737,10 +29610,18 @@
       <c r="AJ279" s="1"/>
     </row>
     <row r="280" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A280" s="1"/>
-      <c r="B280" s="1"/>
-      <c r="C280" s="1"/>
-      <c r="D280" s="1"/>
+      <c r="A280" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B280" s="10">
+        <v>804625</v>
+      </c>
+      <c r="C280" s="10">
+        <v>922.59399294853199</v>
+      </c>
+      <c r="D280" s="10">
+        <v>0</v>
+      </c>
       <c r="E280" s="1"/>
       <c r="F280" s="1"/>
       <c r="G280" s="1"/>
@@ -27775,10 +29656,18 @@
       <c r="AJ280" s="1"/>
     </row>
     <row r="281" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A281" s="1"/>
-      <c r="B281" s="1"/>
-      <c r="C281" s="1"/>
-      <c r="D281" s="1"/>
+      <c r="A281" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B281" s="10">
+        <v>806073</v>
+      </c>
+      <c r="C281" s="10">
+        <v>922.38513612747101</v>
+      </c>
+      <c r="D281" s="10">
+        <v>0</v>
+      </c>
       <c r="E281" s="1"/>
       <c r="F281" s="1"/>
       <c r="G281" s="1"/>
@@ -27813,10 +29702,18 @@
       <c r="AJ281" s="1"/>
     </row>
     <row r="282" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A282" s="1"/>
-      <c r="B282" s="1"/>
-      <c r="C282" s="1"/>
-      <c r="D282" s="1"/>
+      <c r="A282" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B282" s="10">
+        <v>804822</v>
+      </c>
+      <c r="C282" s="10">
+        <v>922.39462590217499</v>
+      </c>
+      <c r="D282" s="10">
+        <v>0</v>
+      </c>
       <c r="E282" s="1"/>
       <c r="F282" s="1"/>
       <c r="G282" s="1"/>
@@ -27851,10 +29748,18 @@
       <c r="AJ282" s="1"/>
     </row>
     <row r="283" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A283" s="1"/>
-      <c r="B283" s="1"/>
-      <c r="C283" s="1"/>
-      <c r="D283" s="1"/>
+      <c r="A283" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B283" s="10">
+        <v>8314623</v>
+      </c>
+      <c r="C283" s="10">
+        <v>922.52507877349797</v>
+      </c>
+      <c r="D283" s="10">
+        <v>0</v>
+      </c>
       <c r="E283" s="1"/>
       <c r="F283" s="1"/>
       <c r="G283" s="1"/>
@@ -27889,10 +29794,18 @@
       <c r="AJ283" s="1"/>
     </row>
     <row r="284" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A284" s="1"/>
-      <c r="B284" s="1"/>
-      <c r="C284" s="1"/>
-      <c r="D284" s="1"/>
+      <c r="A284" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B284" s="10">
+        <v>8238967</v>
+      </c>
+      <c r="C284" s="10">
+        <v>922.15382504463196</v>
+      </c>
+      <c r="D284" s="10">
+        <v>0</v>
+      </c>
       <c r="E284" s="1"/>
       <c r="F284" s="1"/>
       <c r="G284" s="1"/>
@@ -27927,10 +29840,18 @@
       <c r="AJ284" s="1"/>
     </row>
     <row r="285" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A285" s="1"/>
-      <c r="B285" s="1"/>
-      <c r="C285" s="1"/>
-      <c r="D285" s="1"/>
+      <c r="A285" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B285" s="10">
+        <v>8272022</v>
+      </c>
+      <c r="C285" s="10">
+        <v>922.41212320327702</v>
+      </c>
+      <c r="D285" s="10">
+        <v>0</v>
+      </c>
       <c r="E285" s="1"/>
       <c r="F285" s="1"/>
       <c r="G285" s="1"/>
@@ -27965,10 +29886,18 @@
       <c r="AJ285" s="1"/>
     </row>
     <row r="286" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A286" s="1"/>
-      <c r="B286" s="1"/>
-      <c r="C286" s="1"/>
-      <c r="D286" s="1"/>
+      <c r="A286" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B286" s="10">
+        <v>8293624</v>
+      </c>
+      <c r="C286" s="10">
+        <v>922.37150001525799</v>
+      </c>
+      <c r="D286" s="10">
+        <v>0</v>
+      </c>
       <c r="E286" s="1"/>
       <c r="F286" s="1"/>
       <c r="G286" s="1"/>
@@ -28003,10 +29932,18 @@
       <c r="AJ286" s="1"/>
     </row>
     <row r="287" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A287" s="1"/>
-      <c r="B287" s="1"/>
-      <c r="C287" s="1"/>
-      <c r="D287" s="1"/>
+      <c r="A287" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B287" s="10">
+        <v>8113598</v>
+      </c>
+      <c r="C287" s="10">
+        <v>922.51200389862004</v>
+      </c>
+      <c r="D287" s="10">
+        <v>0</v>
+      </c>
       <c r="E287" s="1"/>
       <c r="F287" s="1"/>
       <c r="G287" s="1"/>
@@ -28041,10 +29978,18 @@
       <c r="AJ287" s="1"/>
     </row>
     <row r="288" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A288" s="1"/>
-      <c r="B288" s="1"/>
-      <c r="C288" s="1"/>
-      <c r="D288" s="1"/>
+      <c r="A288" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B288" s="10">
+        <v>257982</v>
+      </c>
+      <c r="C288" s="10">
+        <v>902.45427799224797</v>
+      </c>
+      <c r="D288" s="10">
+        <v>0</v>
+      </c>
       <c r="E288" s="1"/>
       <c r="F288" s="1"/>
       <c r="G288" s="1"/>
@@ -28079,10 +30024,18 @@
       <c r="AJ288" s="1"/>
     </row>
     <row r="289" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A289" s="1"/>
-      <c r="B289" s="1"/>
-      <c r="C289" s="1"/>
-      <c r="D289" s="1"/>
+      <c r="A289" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B289" s="10">
+        <v>257573</v>
+      </c>
+      <c r="C289" s="10">
+        <v>902.71455574035599</v>
+      </c>
+      <c r="D289" s="10">
+        <v>0</v>
+      </c>
       <c r="E289" s="1"/>
       <c r="F289" s="1"/>
       <c r="G289" s="1"/>
@@ -28117,10 +30070,18 @@
       <c r="AJ289" s="1"/>
     </row>
     <row r="290" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A290" s="1"/>
-      <c r="B290" s="1"/>
-      <c r="C290" s="1"/>
-      <c r="D290" s="1"/>
+      <c r="A290" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="B290" s="10">
+        <v>257637</v>
+      </c>
+      <c r="C290" s="10">
+        <v>902.45287489890995</v>
+      </c>
+      <c r="D290" s="10">
+        <v>0</v>
+      </c>
       <c r="E290" s="1"/>
       <c r="F290" s="1"/>
       <c r="G290" s="1"/>
@@ -28155,10 +30116,18 @@
       <c r="AJ290" s="1"/>
     </row>
     <row r="291" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A291" s="1"/>
-      <c r="B291" s="1"/>
-      <c r="C291" s="1"/>
-      <c r="D291" s="1"/>
+      <c r="A291" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="B291" s="10">
+        <v>258002</v>
+      </c>
+      <c r="C291" s="10">
+        <v>902.86888289451599</v>
+      </c>
+      <c r="D291" s="10">
+        <v>0</v>
+      </c>
       <c r="E291" s="1"/>
       <c r="F291" s="1"/>
       <c r="G291" s="1"/>
@@ -28193,10 +30162,18 @@
       <c r="AJ291" s="1"/>
     </row>
     <row r="292" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A292" s="1"/>
-      <c r="B292" s="1"/>
-      <c r="C292" s="1"/>
-      <c r="D292" s="1"/>
+      <c r="A292" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="B292" s="10">
+        <v>257947</v>
+      </c>
+      <c r="C292" s="10">
+        <v>902.55648112297001</v>
+      </c>
+      <c r="D292" s="10">
+        <v>0</v>
+      </c>
       <c r="E292" s="1"/>
       <c r="F292" s="1"/>
       <c r="G292" s="1"/>
@@ -28231,10 +30208,18 @@
       <c r="AJ292" s="1"/>
     </row>
     <row r="293" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A293" s="1"/>
-      <c r="B293" s="1"/>
-      <c r="C293" s="1"/>
-      <c r="D293" s="1"/>
+      <c r="A293" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B293" s="10">
+        <v>277963</v>
+      </c>
+      <c r="C293" s="10">
+        <v>902.70880317687897</v>
+      </c>
+      <c r="D293" s="10">
+        <v>0</v>
+      </c>
       <c r="E293" s="1"/>
       <c r="F293" s="1"/>
       <c r="G293" s="1"/>
@@ -28269,10 +30254,18 @@
       <c r="AJ293" s="1"/>
     </row>
     <row r="294" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A294" s="1"/>
-      <c r="B294" s="1"/>
-      <c r="C294" s="1"/>
-      <c r="D294" s="1"/>
+      <c r="A294" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="B294" s="10">
+        <v>277186</v>
+      </c>
+      <c r="C294" s="10">
+        <v>902.76570177078202</v>
+      </c>
+      <c r="D294" s="10">
+        <v>0</v>
+      </c>
       <c r="E294" s="1"/>
       <c r="F294" s="1"/>
       <c r="G294" s="1"/>
@@ -28307,10 +30300,18 @@
       <c r="AJ294" s="1"/>
     </row>
     <row r="295" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A295" s="1"/>
-      <c r="B295" s="1"/>
-      <c r="C295" s="1"/>
-      <c r="D295" s="1"/>
+      <c r="A295" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B295" s="10">
+        <v>277318</v>
+      </c>
+      <c r="C295" s="10">
+        <v>903.03716206550598</v>
+      </c>
+      <c r="D295" s="10">
+        <v>0</v>
+      </c>
       <c r="E295" s="1"/>
       <c r="F295" s="1"/>
       <c r="G295" s="1"/>
@@ -28345,10 +30346,18 @@
       <c r="AJ295" s="1"/>
     </row>
     <row r="296" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A296" s="1"/>
-      <c r="B296" s="1"/>
-      <c r="C296" s="1"/>
-      <c r="D296" s="1"/>
+      <c r="A296" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B296" s="10">
+        <v>277503</v>
+      </c>
+      <c r="C296" s="10">
+        <v>903.02846908569302</v>
+      </c>
+      <c r="D296" s="10">
+        <v>0</v>
+      </c>
       <c r="E296" s="1"/>
       <c r="F296" s="1"/>
       <c r="G296" s="1"/>
@@ -28383,10 +30392,18 @@
       <c r="AJ296" s="1"/>
     </row>
     <row r="297" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A297" s="1"/>
-      <c r="B297" s="1"/>
-      <c r="C297" s="1"/>
-      <c r="D297" s="1"/>
+      <c r="A297" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B297" s="10">
+        <v>277660</v>
+      </c>
+      <c r="C297" s="10">
+        <v>902.86114811897198</v>
+      </c>
+      <c r="D297" s="10">
+        <v>0</v>
+      </c>
       <c r="E297" s="1"/>
       <c r="F297" s="1"/>
       <c r="G297" s="1"/>
@@ -28421,10 +30438,18 @@
       <c r="AJ297" s="1"/>
     </row>
     <row r="298" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A298" s="1"/>
-      <c r="B298" s="1"/>
-      <c r="C298" s="1"/>
-      <c r="D298" s="1"/>
+      <c r="A298" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B298" s="10">
+        <v>335250</v>
+      </c>
+      <c r="C298" s="10">
+        <v>902.81879806518498</v>
+      </c>
+      <c r="D298" s="10">
+        <v>0</v>
+      </c>
       <c r="E298" s="1"/>
       <c r="F298" s="1"/>
       <c r="G298" s="1"/>
@@ -28459,10 +30484,18 @@
       <c r="AJ298" s="1"/>
     </row>
     <row r="299" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A299" s="1"/>
-      <c r="B299" s="1"/>
-      <c r="C299" s="1"/>
-      <c r="D299" s="1"/>
+      <c r="A299" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="B299" s="10">
+        <v>337978</v>
+      </c>
+      <c r="C299" s="10">
+        <v>902.66474580764702</v>
+      </c>
+      <c r="D299" s="10">
+        <v>0</v>
+      </c>
       <c r="E299" s="1"/>
       <c r="F299" s="1"/>
       <c r="G299" s="1"/>
@@ -28497,10 +30530,18 @@
       <c r="AJ299" s="1"/>
     </row>
     <row r="300" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A300" s="1"/>
-      <c r="B300" s="1"/>
-      <c r="C300" s="1"/>
-      <c r="D300" s="1"/>
+      <c r="A300" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B300" s="10">
+        <v>334568</v>
+      </c>
+      <c r="C300" s="10">
+        <v>902.43451786041203</v>
+      </c>
+      <c r="D300" s="10">
+        <v>0</v>
+      </c>
       <c r="E300" s="1"/>
       <c r="F300" s="1"/>
       <c r="G300" s="1"/>
@@ -28535,10 +30576,18 @@
       <c r="AJ300" s="1"/>
     </row>
     <row r="301" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A301" s="1"/>
-      <c r="B301" s="1"/>
-      <c r="C301" s="1"/>
-      <c r="D301" s="1"/>
+      <c r="A301" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="B301" s="10">
+        <v>336775</v>
+      </c>
+      <c r="C301" s="10">
+        <v>902.83008790016095</v>
+      </c>
+      <c r="D301" s="10">
+        <v>0</v>
+      </c>
       <c r="E301" s="1"/>
       <c r="F301" s="1"/>
       <c r="G301" s="1"/>
@@ -28573,10 +30622,18 @@
       <c r="AJ301" s="1"/>
     </row>
     <row r="302" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A302" s="1"/>
-      <c r="B302" s="1"/>
-      <c r="C302" s="1"/>
-      <c r="D302" s="1"/>
+      <c r="A302" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B302" s="10">
+        <v>336807</v>
+      </c>
+      <c r="C302" s="10">
+        <v>902.78700304031304</v>
+      </c>
+      <c r="D302" s="10">
+        <v>0</v>
+      </c>
       <c r="E302" s="1"/>
       <c r="F302" s="1"/>
       <c r="G302" s="1"/>
@@ -28611,10 +30668,18 @@
       <c r="AJ302" s="1"/>
     </row>
     <row r="303" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A303" s="1"/>
-      <c r="B303" s="1"/>
-      <c r="C303" s="1"/>
-      <c r="D303" s="1"/>
+      <c r="A303" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B303" s="10">
+        <v>511596</v>
+      </c>
+      <c r="C303" s="10">
+        <v>911.28729915618896</v>
+      </c>
+      <c r="D303" s="10">
+        <v>0</v>
+      </c>
       <c r="E303" s="1"/>
       <c r="F303" s="1"/>
       <c r="G303" s="1"/>
@@ -28649,10 +30714,18 @@
       <c r="AJ303" s="1"/>
     </row>
     <row r="304" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A304" s="1"/>
-      <c r="B304" s="1"/>
-      <c r="C304" s="1"/>
-      <c r="D304" s="1"/>
+      <c r="A304" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B304" s="10">
+        <v>511543</v>
+      </c>
+      <c r="C304" s="10">
+        <v>911.35703802108696</v>
+      </c>
+      <c r="D304" s="10">
+        <v>0</v>
+      </c>
       <c r="E304" s="1"/>
       <c r="F304" s="1"/>
       <c r="G304" s="1"/>
@@ -28687,10 +30760,18 @@
       <c r="AJ304" s="1"/>
     </row>
     <row r="305" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A305" s="1"/>
-      <c r="B305" s="1"/>
-      <c r="C305" s="1"/>
-      <c r="D305" s="1"/>
+      <c r="A305" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B305" s="10">
+        <v>511820</v>
+      </c>
+      <c r="C305" s="10">
+        <v>910.53267502784695</v>
+      </c>
+      <c r="D305" s="10">
+        <v>0</v>
+      </c>
       <c r="E305" s="1"/>
       <c r="F305" s="1"/>
       <c r="G305" s="1"/>
@@ -28725,10 +30806,18 @@
       <c r="AJ305" s="1"/>
     </row>
     <row r="306" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A306" s="1"/>
-      <c r="B306" s="1"/>
-      <c r="C306" s="1"/>
-      <c r="D306" s="1"/>
+      <c r="A306" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="B306" s="10">
+        <v>511720</v>
+      </c>
+      <c r="C306" s="10">
+        <v>911.17584109306301</v>
+      </c>
+      <c r="D306" s="10">
+        <v>0</v>
+      </c>
       <c r="E306" s="1"/>
       <c r="F306" s="1"/>
       <c r="G306" s="1"/>
@@ -28763,10 +30852,18 @@
       <c r="AJ306" s="1"/>
     </row>
     <row r="307" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A307" s="1"/>
-      <c r="B307" s="1"/>
-      <c r="C307" s="1"/>
-      <c r="D307" s="1"/>
+      <c r="A307" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="B307" s="10">
+        <v>511896</v>
+      </c>
+      <c r="C307" s="10">
+        <v>911.82793593406598</v>
+      </c>
+      <c r="D307" s="10">
+        <v>0</v>
+      </c>
       <c r="E307" s="1"/>
       <c r="F307" s="1"/>
       <c r="G307" s="1"/>
@@ -28801,10 +30898,18 @@
       <c r="AJ307" s="1"/>
     </row>
     <row r="308" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A308" s="1"/>
-      <c r="B308" s="1"/>
-      <c r="C308" s="1"/>
-      <c r="D308" s="1"/>
+      <c r="A308" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="B308" s="10">
+        <v>543113</v>
+      </c>
+      <c r="C308" s="10">
+        <v>910.08405399322498</v>
+      </c>
+      <c r="D308" s="10">
+        <v>0</v>
+      </c>
       <c r="E308" s="1"/>
       <c r="F308" s="1"/>
       <c r="G308" s="1"/>
@@ -28839,10 +30944,18 @@
       <c r="AJ308" s="1"/>
     </row>
     <row r="309" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A309" s="1"/>
-      <c r="B309" s="1"/>
-      <c r="C309" s="1"/>
-      <c r="D309" s="1"/>
+      <c r="A309" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="B309" s="10">
+        <v>544757</v>
+      </c>
+      <c r="C309" s="10">
+        <v>910.17574715614296</v>
+      </c>
+      <c r="D309" s="10">
+        <v>0</v>
+      </c>
       <c r="E309" s="1"/>
       <c r="F309" s="1"/>
       <c r="G309" s="1"/>
@@ -28877,10 +30990,18 @@
       <c r="AJ309" s="1"/>
     </row>
     <row r="310" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A310" s="1"/>
-      <c r="B310" s="1"/>
-      <c r="C310" s="1"/>
-      <c r="D310" s="1"/>
+      <c r="A310" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="B310" s="10">
+        <v>545082</v>
+      </c>
+      <c r="C310" s="10">
+        <v>910.02588105201698</v>
+      </c>
+      <c r="D310" s="10">
+        <v>0</v>
+      </c>
       <c r="E310" s="1"/>
       <c r="F310" s="1"/>
       <c r="G310" s="1"/>
@@ -28915,10 +31036,18 @@
       <c r="AJ310" s="1"/>
     </row>
     <row r="311" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A311" s="1"/>
-      <c r="B311" s="1"/>
-      <c r="C311" s="1"/>
-      <c r="D311" s="1"/>
+      <c r="A311" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="B311" s="10">
+        <v>544587</v>
+      </c>
+      <c r="C311" s="10">
+        <v>910.35155200958195</v>
+      </c>
+      <c r="D311" s="10">
+        <v>0</v>
+      </c>
       <c r="E311" s="1"/>
       <c r="F311" s="1"/>
       <c r="G311" s="1"/>
@@ -28953,10 +31082,18 @@
       <c r="AJ311" s="1"/>
     </row>
     <row r="312" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A312" s="1"/>
-      <c r="B312" s="1"/>
-      <c r="C312" s="1"/>
-      <c r="D312" s="1"/>
+      <c r="A312" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="B312" s="10">
+        <v>543683</v>
+      </c>
+      <c r="C312" s="10">
+        <v>910.50993108749299</v>
+      </c>
+      <c r="D312" s="10">
+        <v>0</v>
+      </c>
       <c r="E312" s="1"/>
       <c r="F312" s="1"/>
       <c r="G312" s="1"/>
@@ -28991,10 +31128,18 @@
       <c r="AJ312" s="1"/>
     </row>
     <row r="313" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A313" s="1"/>
-      <c r="B313" s="1"/>
-      <c r="C313" s="1"/>
-      <c r="D313" s="1"/>
+      <c r="A313" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="B313" s="10">
+        <v>650774</v>
+      </c>
+      <c r="C313" s="10">
+        <v>911.23421382903996</v>
+      </c>
+      <c r="D313" s="10">
+        <v>0</v>
+      </c>
       <c r="E313" s="1"/>
       <c r="F313" s="1"/>
       <c r="G313" s="1"/>
@@ -29029,10 +31174,18 @@
       <c r="AJ313" s="1"/>
     </row>
     <row r="314" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A314" s="1"/>
-      <c r="B314" s="1"/>
-      <c r="C314" s="1"/>
-      <c r="D314" s="1"/>
+      <c r="A314" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="B314" s="10">
+        <v>652789</v>
+      </c>
+      <c r="C314" s="10">
+        <v>911.64885783195496</v>
+      </c>
+      <c r="D314" s="10">
+        <v>0</v>
+      </c>
       <c r="E314" s="1"/>
       <c r="F314" s="1"/>
       <c r="G314" s="1"/>
@@ -29067,10 +31220,18 @@
       <c r="AJ314" s="1"/>
     </row>
     <row r="315" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A315" s="1"/>
-      <c r="B315" s="1"/>
-      <c r="C315" s="1"/>
-      <c r="D315" s="1"/>
+      <c r="A315" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B315" s="10">
+        <v>651278</v>
+      </c>
+      <c r="C315" s="10">
+        <v>911.36014986038197</v>
+      </c>
+      <c r="D315" s="10">
+        <v>0</v>
+      </c>
       <c r="E315" s="1"/>
       <c r="F315" s="1"/>
       <c r="G315" s="1"/>
@@ -29105,10 +31266,18 @@
       <c r="AJ315" s="1"/>
     </row>
     <row r="316" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A316" s="1"/>
-      <c r="B316" s="1"/>
-      <c r="C316" s="1"/>
-      <c r="D316" s="1"/>
+      <c r="A316" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="B316" s="10">
+        <v>650240</v>
+      </c>
+      <c r="C316" s="10">
+        <v>911.308551073074</v>
+      </c>
+      <c r="D316" s="10">
+        <v>0</v>
+      </c>
       <c r="E316" s="1"/>
       <c r="F316" s="1"/>
       <c r="G316" s="1"/>
@@ -29143,10 +31312,18 @@
       <c r="AJ316" s="1"/>
     </row>
     <row r="317" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A317" s="1"/>
-      <c r="B317" s="1"/>
-      <c r="C317" s="1"/>
-      <c r="D317" s="1"/>
+      <c r="A317" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="B317" s="10">
+        <v>653596</v>
+      </c>
+      <c r="C317" s="10">
+        <v>910.14066624641396</v>
+      </c>
+      <c r="D317" s="10">
+        <v>0</v>
+      </c>
       <c r="E317" s="1"/>
       <c r="F317" s="1"/>
       <c r="G317" s="1"/>
@@ -29181,10 +31358,18 @@
       <c r="AJ317" s="1"/>
     </row>
     <row r="318" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A318" s="1"/>
-      <c r="B318" s="1"/>
-      <c r="C318" s="1"/>
-      <c r="D318" s="1"/>
+      <c r="A318" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="B318" s="10">
+        <v>764489</v>
+      </c>
+      <c r="C318" s="10">
+        <v>925.529658079147</v>
+      </c>
+      <c r="D318" s="10">
+        <v>0</v>
+      </c>
       <c r="E318" s="1"/>
       <c r="F318" s="1"/>
       <c r="G318" s="1"/>
@@ -29219,10 +31404,18 @@
       <c r="AJ318" s="1"/>
     </row>
     <row r="319" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A319" s="1"/>
-      <c r="B319" s="1"/>
-      <c r="C319" s="1"/>
-      <c r="D319" s="1"/>
+      <c r="A319" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="B319" s="10">
+        <v>764323</v>
+      </c>
+      <c r="C319" s="10">
+        <v>922.64379024505604</v>
+      </c>
+      <c r="D319" s="10">
+        <v>0</v>
+      </c>
       <c r="E319" s="1"/>
       <c r="F319" s="1"/>
       <c r="G319" s="1"/>
@@ -29257,10 +31450,18 @@
       <c r="AJ319" s="1"/>
     </row>
     <row r="320" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A320" s="1"/>
-      <c r="B320" s="1"/>
-      <c r="C320" s="1"/>
-      <c r="D320" s="1"/>
+      <c r="A320" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="B320" s="10">
+        <v>764514</v>
+      </c>
+      <c r="C320" s="10">
+        <v>943.27610707282997</v>
+      </c>
+      <c r="D320" s="10">
+        <v>0</v>
+      </c>
       <c r="E320" s="1"/>
       <c r="F320" s="1"/>
       <c r="G320" s="1"/>
@@ -29295,10 +31496,18 @@
       <c r="AJ320" s="1"/>
     </row>
     <row r="321" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A321" s="1"/>
-      <c r="B321" s="1"/>
-      <c r="C321" s="1"/>
-      <c r="D321" s="1"/>
+      <c r="A321" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="B321" s="10">
+        <v>764778</v>
+      </c>
+      <c r="C321" s="10">
+        <v>1000.9630742073</v>
+      </c>
+      <c r="D321" s="10">
+        <v>0</v>
+      </c>
       <c r="E321" s="1"/>
       <c r="F321" s="1"/>
       <c r="G321" s="1"/>
@@ -29333,10 +31542,18 @@
       <c r="AJ321" s="1"/>
     </row>
     <row r="322" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A322" s="1"/>
-      <c r="B322" s="1"/>
-      <c r="C322" s="1"/>
-      <c r="D322" s="1"/>
+      <c r="A322" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="B322" s="10">
+        <v>764518</v>
+      </c>
+      <c r="C322" s="10">
+        <v>923.41966295242298</v>
+      </c>
+      <c r="D322" s="10">
+        <v>0</v>
+      </c>
       <c r="E322" s="1"/>
       <c r="F322" s="1"/>
       <c r="G322" s="1"/>
@@ -29371,10 +31588,18 @@
       <c r="AJ322" s="1"/>
     </row>
     <row r="323" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A323" s="1"/>
-      <c r="B323" s="1"/>
-      <c r="C323" s="1"/>
-      <c r="D323" s="1"/>
+      <c r="A323" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="B323" s="10">
+        <v>805705</v>
+      </c>
+      <c r="C323" s="10">
+        <v>923.70170497894196</v>
+      </c>
+      <c r="D323" s="10">
+        <v>0</v>
+      </c>
       <c r="E323" s="1"/>
       <c r="F323" s="1"/>
       <c r="G323" s="1"/>
@@ -29409,10 +31634,18 @@
       <c r="AJ323" s="1"/>
     </row>
     <row r="324" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A324" s="1"/>
-      <c r="B324" s="1"/>
-      <c r="C324" s="1"/>
-      <c r="D324" s="1"/>
+      <c r="A324" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="B324" s="10">
+        <v>804801</v>
+      </c>
+      <c r="C324" s="10">
+        <v>925.14163589477505</v>
+      </c>
+      <c r="D324" s="10">
+        <v>0</v>
+      </c>
       <c r="E324" s="1"/>
       <c r="F324" s="1"/>
       <c r="G324" s="1"/>
@@ -29447,10 +31680,18 @@
       <c r="AJ324" s="1"/>
     </row>
     <row r="325" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A325" s="1"/>
-      <c r="B325" s="1"/>
-      <c r="C325" s="1"/>
-      <c r="D325" s="1"/>
+      <c r="A325" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B325" s="10">
+        <v>806007</v>
+      </c>
+      <c r="C325" s="10">
+        <v>926.23342895507801</v>
+      </c>
+      <c r="D325" s="10">
+        <v>0</v>
+      </c>
       <c r="E325" s="1"/>
       <c r="F325" s="1"/>
       <c r="G325" s="1"/>
@@ -29485,10 +31726,18 @@
       <c r="AJ325" s="1"/>
     </row>
     <row r="326" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A326" s="1"/>
-      <c r="B326" s="1"/>
-      <c r="C326" s="1"/>
-      <c r="D326" s="1"/>
+      <c r="A326" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="B326" s="10">
+        <v>804453</v>
+      </c>
+      <c r="C326" s="10">
+        <v>925.72512578964199</v>
+      </c>
+      <c r="D326" s="10">
+        <v>0</v>
+      </c>
       <c r="E326" s="1"/>
       <c r="F326" s="1"/>
       <c r="G326" s="1"/>
@@ -29523,10 +31772,18 @@
       <c r="AJ326" s="1"/>
     </row>
     <row r="327" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A327" s="1"/>
-      <c r="B327" s="1"/>
-      <c r="C327" s="1"/>
-      <c r="D327" s="1"/>
+      <c r="A327" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B327" s="10">
+        <v>805745</v>
+      </c>
+      <c r="C327" s="10">
+        <v>926.446646928787</v>
+      </c>
+      <c r="D327" s="10">
+        <v>0</v>
+      </c>
       <c r="E327" s="1"/>
       <c r="F327" s="1"/>
       <c r="G327" s="1"/>
@@ -29561,10 +31818,18 @@
       <c r="AJ327" s="1"/>
     </row>
     <row r="328" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A328" s="1"/>
-      <c r="B328" s="1"/>
-      <c r="C328" s="1"/>
-      <c r="D328" s="1"/>
+      <c r="A328" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="B328" s="10">
+        <v>8243622</v>
+      </c>
+      <c r="C328" s="10">
+        <v>926.22148108482304</v>
+      </c>
+      <c r="D328" s="10">
+        <v>0</v>
+      </c>
       <c r="E328" s="1"/>
       <c r="F328" s="1"/>
       <c r="G328" s="1"/>
@@ -29599,10 +31864,18 @@
       <c r="AJ328" s="1"/>
     </row>
     <row r="329" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A329" s="1"/>
-      <c r="B329" s="1"/>
-      <c r="C329" s="1"/>
-      <c r="D329" s="1"/>
+      <c r="A329" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="B329" s="10">
+        <v>8373748</v>
+      </c>
+      <c r="C329" s="10">
+        <v>925.34666800498906</v>
+      </c>
+      <c r="D329" s="10">
+        <v>0</v>
+      </c>
       <c r="E329" s="1"/>
       <c r="F329" s="1"/>
       <c r="G329" s="1"/>
@@ -29637,10 +31910,18 @@
       <c r="AJ329" s="1"/>
     </row>
     <row r="330" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A330" s="1"/>
-      <c r="B330" s="1"/>
-      <c r="C330" s="1"/>
-      <c r="D330" s="1"/>
+      <c r="A330" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="B330" s="10">
+        <v>8264997</v>
+      </c>
+      <c r="C330" s="10">
+        <v>925.06150794029202</v>
+      </c>
+      <c r="D330" s="10">
+        <v>0</v>
+      </c>
       <c r="E330" s="1"/>
       <c r="F330" s="1"/>
       <c r="G330" s="1"/>
@@ -29675,10 +31956,18 @@
       <c r="AJ330" s="1"/>
     </row>
     <row r="331" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A331" s="1"/>
-      <c r="B331" s="1"/>
-      <c r="C331" s="1"/>
-      <c r="D331" s="1"/>
+      <c r="A331" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="B331" s="10">
+        <v>8320376</v>
+      </c>
+      <c r="C331" s="10">
+        <v>927.86582994461003</v>
+      </c>
+      <c r="D331" s="10">
+        <v>0</v>
+      </c>
       <c r="E331" s="1"/>
       <c r="F331" s="1"/>
       <c r="G331" s="1"/>
@@ -29713,10 +32002,18 @@
       <c r="AJ331" s="1"/>
     </row>
     <row r="332" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A332" s="1"/>
-      <c r="B332" s="1"/>
-      <c r="C332" s="1"/>
-      <c r="D332" s="1"/>
+      <c r="A332" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="B332" s="10">
+        <v>8384003</v>
+      </c>
+      <c r="C332" s="10">
+        <v>924.673907995224</v>
+      </c>
+      <c r="D332" s="10">
+        <v>0</v>
+      </c>
       <c r="E332" s="1"/>
       <c r="F332" s="1"/>
       <c r="G332" s="1"/>
@@ -29751,10 +32048,6 @@
       <c r="AJ332" s="1"/>
     </row>
     <row r="333" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A333" s="1"/>
-      <c r="B333" s="1"/>
-      <c r="C333" s="1"/>
-      <c r="D333" s="1"/>
       <c r="E333" s="1"/>
       <c r="F333" s="1"/>
       <c r="G333" s="1"/>
@@ -29827,9 +32120,14 @@
       <c r="AJ334" s="1"/>
     </row>
     <row r="335" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A335" s="1"/>
-      <c r="B335" s="1"/>
-      <c r="C335" s="1"/>
+      <c r="A335" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="B335" s="23"/>
+      <c r="C335" s="7">
+        <f>SUM(C3:C242)</f>
+        <v>11757.668949604795</v>
+      </c>
       <c r="D335" s="1"/>
       <c r="E335" s="1"/>
       <c r="F335" s="1"/>
@@ -29865,9 +32163,14 @@
       <c r="AJ335" s="1"/>
     </row>
     <row r="336" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A336" s="1"/>
-      <c r="B336" s="1"/>
-      <c r="C336" s="1"/>
+      <c r="A336" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="B336" s="23"/>
+      <c r="C336" s="7">
+        <f>C335/60</f>
+        <v>195.96114916007991</v>
+      </c>
       <c r="D336" s="1"/>
       <c r="E336" s="1"/>
       <c r="F336" s="1"/>
@@ -55362,16 +57665,555 @@
       <c r="AI1006" s="1"/>
       <c r="AJ1006" s="1"/>
     </row>
+    <row r="1007" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="1"/>
+    </row>
+    <row r="1008" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+      <c r="D1008" s="1"/>
+    </row>
+    <row r="1009" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="1"/>
+      <c r="C1009" s="1"/>
+      <c r="D1009" s="1"/>
+    </row>
+    <row r="1010" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1010" s="1"/>
+      <c r="B1010" s="1"/>
+      <c r="C1010" s="1"/>
+      <c r="D1010" s="1"/>
+    </row>
+    <row r="1011" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1011" s="1"/>
+      <c r="B1011" s="1"/>
+      <c r="C1011" s="1"/>
+      <c r="D1011" s="1"/>
+    </row>
+    <row r="1012" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1012" s="1"/>
+      <c r="B1012" s="1"/>
+      <c r="C1012" s="1"/>
+      <c r="D1012" s="1"/>
+    </row>
+    <row r="1013" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1013" s="1"/>
+      <c r="B1013" s="1"/>
+      <c r="C1013" s="1"/>
+      <c r="D1013" s="1"/>
+    </row>
+    <row r="1014" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1014" s="1"/>
+      <c r="B1014" s="1"/>
+      <c r="C1014" s="1"/>
+      <c r="D1014" s="1"/>
+    </row>
+    <row r="1015" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1015" s="1"/>
+      <c r="B1015" s="1"/>
+      <c r="C1015" s="1"/>
+      <c r="D1015" s="1"/>
+    </row>
+    <row r="1016" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1016" s="1"/>
+      <c r="B1016" s="1"/>
+      <c r="C1016" s="1"/>
+      <c r="D1016" s="1"/>
+    </row>
+    <row r="1017" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1017" s="1"/>
+      <c r="B1017" s="1"/>
+      <c r="C1017" s="1"/>
+      <c r="D1017" s="1"/>
+    </row>
+    <row r="1018" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1018" s="1"/>
+      <c r="B1018" s="1"/>
+      <c r="C1018" s="1"/>
+      <c r="D1018" s="1"/>
+    </row>
+    <row r="1019" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1019" s="1"/>
+      <c r="B1019" s="1"/>
+      <c r="C1019" s="1"/>
+      <c r="D1019" s="1"/>
+    </row>
+    <row r="1020" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1020" s="1"/>
+      <c r="B1020" s="1"/>
+      <c r="C1020" s="1"/>
+      <c r="D1020" s="1"/>
+    </row>
+    <row r="1021" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1021" s="1"/>
+      <c r="B1021" s="1"/>
+      <c r="C1021" s="1"/>
+      <c r="D1021" s="1"/>
+    </row>
+    <row r="1022" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1022" s="1"/>
+      <c r="B1022" s="1"/>
+      <c r="C1022" s="1"/>
+      <c r="D1022" s="1"/>
+    </row>
+    <row r="1023" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1023" s="1"/>
+      <c r="B1023" s="1"/>
+      <c r="C1023" s="1"/>
+      <c r="D1023" s="1"/>
+    </row>
+    <row r="1024" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1024" s="1"/>
+      <c r="B1024" s="1"/>
+      <c r="C1024" s="1"/>
+      <c r="D1024" s="1"/>
+    </row>
+    <row r="1025" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1025" s="1"/>
+      <c r="B1025" s="1"/>
+      <c r="C1025" s="1"/>
+      <c r="D1025" s="1"/>
+    </row>
+    <row r="1026" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1026" s="1"/>
+      <c r="B1026" s="1"/>
+      <c r="C1026" s="1"/>
+      <c r="D1026" s="1"/>
+    </row>
+    <row r="1027" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1027" s="1"/>
+      <c r="B1027" s="1"/>
+      <c r="C1027" s="1"/>
+      <c r="D1027" s="1"/>
+    </row>
+    <row r="1028" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1028" s="1"/>
+      <c r="B1028" s="1"/>
+      <c r="C1028" s="1"/>
+      <c r="D1028" s="1"/>
+    </row>
+    <row r="1029" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1029" s="1"/>
+      <c r="B1029" s="1"/>
+      <c r="C1029" s="1"/>
+      <c r="D1029" s="1"/>
+    </row>
+    <row r="1030" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1030" s="1"/>
+      <c r="B1030" s="1"/>
+      <c r="C1030" s="1"/>
+      <c r="D1030" s="1"/>
+    </row>
+    <row r="1031" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1031" s="1"/>
+      <c r="B1031" s="1"/>
+      <c r="C1031" s="1"/>
+      <c r="D1031" s="1"/>
+    </row>
+    <row r="1032" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1032" s="1"/>
+      <c r="B1032" s="1"/>
+      <c r="C1032" s="1"/>
+      <c r="D1032" s="1"/>
+    </row>
+    <row r="1033" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1033" s="1"/>
+      <c r="B1033" s="1"/>
+      <c r="C1033" s="1"/>
+      <c r="D1033" s="1"/>
+    </row>
+    <row r="1034" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1034" s="1"/>
+      <c r="B1034" s="1"/>
+      <c r="C1034" s="1"/>
+      <c r="D1034" s="1"/>
+    </row>
+    <row r="1035" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1035" s="1"/>
+      <c r="B1035" s="1"/>
+      <c r="C1035" s="1"/>
+      <c r="D1035" s="1"/>
+    </row>
+    <row r="1036" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1036" s="1"/>
+      <c r="B1036" s="1"/>
+      <c r="C1036" s="1"/>
+      <c r="D1036" s="1"/>
+    </row>
+    <row r="1037" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1037" s="1"/>
+      <c r="B1037" s="1"/>
+      <c r="C1037" s="1"/>
+      <c r="D1037" s="1"/>
+    </row>
+    <row r="1038" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1038" s="1"/>
+      <c r="B1038" s="1"/>
+      <c r="C1038" s="1"/>
+      <c r="D1038" s="1"/>
+    </row>
+    <row r="1039" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1039" s="1"/>
+      <c r="B1039" s="1"/>
+      <c r="C1039" s="1"/>
+      <c r="D1039" s="1"/>
+    </row>
+    <row r="1040" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1040" s="1"/>
+      <c r="B1040" s="1"/>
+      <c r="C1040" s="1"/>
+      <c r="D1040" s="1"/>
+    </row>
+    <row r="1041" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1041" s="1"/>
+      <c r="B1041" s="1"/>
+      <c r="C1041" s="1"/>
+      <c r="D1041" s="1"/>
+    </row>
+    <row r="1042" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1042" s="1"/>
+      <c r="B1042" s="1"/>
+      <c r="C1042" s="1"/>
+      <c r="D1042" s="1"/>
+    </row>
+    <row r="1043" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1043" s="1"/>
+      <c r="B1043" s="1"/>
+      <c r="C1043" s="1"/>
+      <c r="D1043" s="1"/>
+    </row>
+    <row r="1044" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1044" s="1"/>
+      <c r="B1044" s="1"/>
+      <c r="C1044" s="1"/>
+      <c r="D1044" s="1"/>
+    </row>
+    <row r="1045" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1045" s="1"/>
+      <c r="B1045" s="1"/>
+      <c r="C1045" s="1"/>
+      <c r="D1045" s="1"/>
+    </row>
+    <row r="1046" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1046" s="1"/>
+      <c r="B1046" s="1"/>
+      <c r="C1046" s="1"/>
+      <c r="D1046" s="1"/>
+    </row>
+    <row r="1047" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1047" s="1"/>
+      <c r="B1047" s="1"/>
+      <c r="C1047" s="1"/>
+      <c r="D1047" s="1"/>
+    </row>
+    <row r="1048" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1048" s="1"/>
+      <c r="B1048" s="1"/>
+      <c r="C1048" s="1"/>
+      <c r="D1048" s="1"/>
+    </row>
+    <row r="1049" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1049" s="1"/>
+      <c r="B1049" s="1"/>
+      <c r="C1049" s="1"/>
+      <c r="D1049" s="1"/>
+    </row>
+    <row r="1050" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1050" s="1"/>
+      <c r="B1050" s="1"/>
+      <c r="C1050" s="1"/>
+      <c r="D1050" s="1"/>
+    </row>
+    <row r="1051" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1051" s="1"/>
+      <c r="B1051" s="1"/>
+      <c r="C1051" s="1"/>
+      <c r="D1051" s="1"/>
+    </row>
+    <row r="1052" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1052" s="1"/>
+      <c r="B1052" s="1"/>
+      <c r="C1052" s="1"/>
+      <c r="D1052" s="1"/>
+    </row>
+    <row r="1053" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1053" s="1"/>
+      <c r="B1053" s="1"/>
+      <c r="C1053" s="1"/>
+      <c r="D1053" s="1"/>
+    </row>
+    <row r="1054" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1054" s="1"/>
+      <c r="B1054" s="1"/>
+      <c r="C1054" s="1"/>
+      <c r="D1054" s="1"/>
+    </row>
+    <row r="1055" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1055" s="1"/>
+      <c r="B1055" s="1"/>
+      <c r="C1055" s="1"/>
+      <c r="D1055" s="1"/>
+    </row>
+    <row r="1056" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1056" s="1"/>
+      <c r="B1056" s="1"/>
+      <c r="C1056" s="1"/>
+      <c r="D1056" s="1"/>
+    </row>
+    <row r="1057" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1057" s="1"/>
+      <c r="B1057" s="1"/>
+      <c r="C1057" s="1"/>
+      <c r="D1057" s="1"/>
+    </row>
+    <row r="1058" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1058" s="1"/>
+      <c r="B1058" s="1"/>
+      <c r="C1058" s="1"/>
+      <c r="D1058" s="1"/>
+    </row>
+    <row r="1059" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1059" s="1"/>
+      <c r="B1059" s="1"/>
+      <c r="C1059" s="1"/>
+      <c r="D1059" s="1"/>
+    </row>
+    <row r="1060" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1060" s="1"/>
+      <c r="B1060" s="1"/>
+      <c r="C1060" s="1"/>
+      <c r="D1060" s="1"/>
+    </row>
+    <row r="1061" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1061" s="1"/>
+      <c r="B1061" s="1"/>
+      <c r="C1061" s="1"/>
+      <c r="D1061" s="1"/>
+    </row>
+    <row r="1062" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1062" s="1"/>
+      <c r="B1062" s="1"/>
+      <c r="C1062" s="1"/>
+      <c r="D1062" s="1"/>
+    </row>
+    <row r="1063" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1063" s="1"/>
+      <c r="B1063" s="1"/>
+      <c r="C1063" s="1"/>
+      <c r="D1063" s="1"/>
+    </row>
+    <row r="1064" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1064" s="1"/>
+      <c r="B1064" s="1"/>
+      <c r="C1064" s="1"/>
+      <c r="D1064" s="1"/>
+    </row>
+    <row r="1065" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1065" s="1"/>
+      <c r="B1065" s="1"/>
+      <c r="C1065" s="1"/>
+      <c r="D1065" s="1"/>
+    </row>
+    <row r="1066" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1066" s="1"/>
+      <c r="B1066" s="1"/>
+      <c r="C1066" s="1"/>
+      <c r="D1066" s="1"/>
+    </row>
+    <row r="1067" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1067" s="1"/>
+      <c r="B1067" s="1"/>
+      <c r="C1067" s="1"/>
+      <c r="D1067" s="1"/>
+    </row>
+    <row r="1068" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1068" s="1"/>
+      <c r="B1068" s="1"/>
+      <c r="C1068" s="1"/>
+      <c r="D1068" s="1"/>
+    </row>
+    <row r="1069" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1069" s="1"/>
+      <c r="B1069" s="1"/>
+      <c r="C1069" s="1"/>
+      <c r="D1069" s="1"/>
+    </row>
+    <row r="1070" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1070" s="1"/>
+      <c r="B1070" s="1"/>
+      <c r="C1070" s="1"/>
+      <c r="D1070" s="1"/>
+    </row>
+    <row r="1071" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1071" s="1"/>
+      <c r="B1071" s="1"/>
+      <c r="C1071" s="1"/>
+      <c r="D1071" s="1"/>
+    </row>
+    <row r="1072" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1072" s="1"/>
+      <c r="B1072" s="1"/>
+      <c r="C1072" s="1"/>
+      <c r="D1072" s="1"/>
+    </row>
+    <row r="1073" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1073" s="1"/>
+      <c r="B1073" s="1"/>
+      <c r="C1073" s="1"/>
+      <c r="D1073" s="1"/>
+    </row>
+    <row r="1074" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1074" s="1"/>
+      <c r="B1074" s="1"/>
+      <c r="C1074" s="1"/>
+      <c r="D1074" s="1"/>
+    </row>
+    <row r="1075" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1075" s="1"/>
+      <c r="B1075" s="1"/>
+      <c r="C1075" s="1"/>
+      <c r="D1075" s="1"/>
+    </row>
+    <row r="1076" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1076" s="1"/>
+      <c r="B1076" s="1"/>
+      <c r="C1076" s="1"/>
+      <c r="D1076" s="1"/>
+    </row>
+    <row r="1077" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1077" s="1"/>
+      <c r="B1077" s="1"/>
+      <c r="C1077" s="1"/>
+      <c r="D1077" s="1"/>
+    </row>
+    <row r="1078" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1078" s="1"/>
+      <c r="B1078" s="1"/>
+      <c r="C1078" s="1"/>
+      <c r="D1078" s="1"/>
+    </row>
+    <row r="1079" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1079" s="1"/>
+      <c r="B1079" s="1"/>
+      <c r="C1079" s="1"/>
+      <c r="D1079" s="1"/>
+    </row>
+    <row r="1080" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1080" s="1"/>
+      <c r="B1080" s="1"/>
+      <c r="C1080" s="1"/>
+      <c r="D1080" s="1"/>
+    </row>
+    <row r="1081" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1081" s="1"/>
+      <c r="B1081" s="1"/>
+      <c r="C1081" s="1"/>
+      <c r="D1081" s="1"/>
+    </row>
+    <row r="1082" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1082" s="1"/>
+      <c r="B1082" s="1"/>
+      <c r="C1082" s="1"/>
+      <c r="D1082" s="1"/>
+    </row>
+    <row r="1083" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1083" s="1"/>
+      <c r="B1083" s="1"/>
+      <c r="C1083" s="1"/>
+      <c r="D1083" s="1"/>
+    </row>
+    <row r="1084" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1084" s="1"/>
+      <c r="B1084" s="1"/>
+      <c r="C1084" s="1"/>
+      <c r="D1084" s="1"/>
+    </row>
+    <row r="1085" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1085" s="1"/>
+      <c r="B1085" s="1"/>
+      <c r="C1085" s="1"/>
+      <c r="D1085" s="1"/>
+    </row>
+    <row r="1086" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1086" s="1"/>
+      <c r="B1086" s="1"/>
+      <c r="C1086" s="1"/>
+      <c r="D1086" s="1"/>
+    </row>
+    <row r="1087" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1087" s="1"/>
+      <c r="B1087" s="1"/>
+      <c r="C1087" s="1"/>
+      <c r="D1087" s="1"/>
+    </row>
+    <row r="1088" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1088" s="1"/>
+      <c r="B1088" s="1"/>
+      <c r="C1088" s="1"/>
+      <c r="D1088" s="1"/>
+    </row>
+    <row r="1089" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1089" s="1"/>
+      <c r="B1089" s="1"/>
+      <c r="C1089" s="1"/>
+      <c r="D1089" s="1"/>
+    </row>
+    <row r="1090" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1090" s="1"/>
+      <c r="B1090" s="1"/>
+      <c r="C1090" s="1"/>
+      <c r="D1090" s="1"/>
+    </row>
+    <row r="1091" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1091" s="1"/>
+      <c r="B1091" s="1"/>
+      <c r="C1091" s="1"/>
+      <c r="D1091" s="1"/>
+    </row>
+    <row r="1092" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1092" s="1"/>
+      <c r="B1092" s="1"/>
+      <c r="C1092" s="1"/>
+      <c r="D1092" s="1"/>
+    </row>
+    <row r="1093" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1093" s="1"/>
+      <c r="B1093" s="1"/>
+      <c r="C1093" s="1"/>
+      <c r="D1093" s="1"/>
+    </row>
+    <row r="1094" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1094" s="1"/>
+      <c r="B1094" s="1"/>
+      <c r="C1094" s="1"/>
+      <c r="D1094" s="1"/>
+    </row>
+    <row r="1095" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1095" s="1"/>
+      <c r="B1095" s="1"/>
+      <c r="C1095" s="1"/>
+      <c r="D1095" s="1"/>
+    </row>
+    <row r="1096" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1096" s="1"/>
+      <c r="B1096" s="1"/>
+      <c r="C1096" s="1"/>
+      <c r="D1096" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="F245:G245"/>
-    <mergeCell ref="F246:G246"/>
-    <mergeCell ref="L245:M245"/>
-    <mergeCell ref="O245:O246"/>
-    <mergeCell ref="L246:M246"/>
-    <mergeCell ref="A245:B245"/>
-    <mergeCell ref="A246:B246"/>
+    <mergeCell ref="V245:W245"/>
+    <mergeCell ref="Y245:Y246"/>
+    <mergeCell ref="Q246:R246"/>
+    <mergeCell ref="V246:W246"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="A335:B335"/>
+    <mergeCell ref="A336:B336"/>
     <mergeCell ref="AI245:AI246"/>
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="AH1:AI1"/>
@@ -55386,18 +58228,19 @@
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="Q245:R245"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="V245:W245"/>
-    <mergeCell ref="Y245:Y246"/>
-    <mergeCell ref="Q246:R246"/>
-    <mergeCell ref="V246:W246"/>
-    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="F245:G245"/>
+    <mergeCell ref="F246:G246"/>
+    <mergeCell ref="L245:M245"/>
+    <mergeCell ref="O245:O246"/>
+    <mergeCell ref="L246:M246"/>
   </mergeCells>
   <conditionalFormatting sqref="AF3:AF242">
-    <cfRule type="cellIs" dxfId="42" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="49" operator="greaterThan">
       <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="lessThan">
-      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3:AF242">
@@ -55553,7 +58396,7 @@
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D242">
+  <conditionalFormatting sqref="D3:D332">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Comecando a parte do ganho na troca de instalacao
</commit_message>
<xml_diff>
--- a/solutions.xlsx
+++ b/solutions.xlsx
@@ -9,19 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan2" sheetId="2" r:id="rId1"/>
-    <sheet name="Plan1" sheetId="1" r:id="rId2"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solutions1" localSheetId="1">Plan1!$F$2:$I$17</definedName>
-    <definedName name="solutions1_1" localSheetId="1">Plan1!$AA$3:$AC$17</definedName>
-    <definedName name="solutions1_2" localSheetId="1">Plan1!$Q$2:$S$17</definedName>
-    <definedName name="solutions2" localSheetId="1">Plan1!$Z$4:$AC$224</definedName>
-    <definedName name="solutions2_1" localSheetId="1">Plan1!$AA$18:$AC$237</definedName>
-    <definedName name="solutions2_2" localSheetId="0">Plan2!$A$1:$D$91</definedName>
+    <definedName name="solutions1" localSheetId="0">Plan1!$F$2:$I$17</definedName>
+    <definedName name="solutions1_1" localSheetId="0">Plan1!$AA$3:$AC$17</definedName>
+    <definedName name="solutions1_2" localSheetId="0">Plan1!$Q$2:$S$17</definedName>
+    <definedName name="solutions2" localSheetId="0">Plan1!$Z$4:$AC$224</definedName>
+    <definedName name="solutions2_1" localSheetId="0">Plan1!$AA$18:$AC$237</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -57,21 +55,11 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="solutions2" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Macbook/Documents/GitKraken_Projects/ICAlgoritmos/gurobi/solutions2.csv" comma="1">
-      <textFields count="4">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="348">
   <si>
     <t>ILP</t>
   </si>
@@ -1323,26 +1311,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
@@ -1613,6 +1581,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
@@ -1750,15 +1738,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions2_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2024,1305 +2008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D91"/>
-  <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D91"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B2">
-        <v>257988</v>
-      </c>
-      <c r="C2">
-        <v>905.518512010574</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B3">
-        <v>257502</v>
-      </c>
-      <c r="C3">
-        <v>902.75716519355694</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>260</v>
-      </c>
-      <c r="B4">
-        <v>258182</v>
-      </c>
-      <c r="C4">
-        <v>903.18458223342896</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B5">
-        <v>257987</v>
-      </c>
-      <c r="C5">
-        <v>902.67631506919804</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>262</v>
-      </c>
-      <c r="B6">
-        <v>258280</v>
-      </c>
-      <c r="C6">
-        <v>902.95274996757496</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>263</v>
-      </c>
-      <c r="B7">
-        <v>277387</v>
-      </c>
-      <c r="C7">
-        <v>902.45952630042996</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>264</v>
-      </c>
-      <c r="B8">
-        <v>276108</v>
-      </c>
-      <c r="C8">
-        <v>902.45691275596596</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B9">
-        <v>277320</v>
-      </c>
-      <c r="C9">
-        <v>902.72219800949097</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>266</v>
-      </c>
-      <c r="B10">
-        <v>278647</v>
-      </c>
-      <c r="C10">
-        <v>902.727436780929</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>267</v>
-      </c>
-      <c r="B11">
-        <v>277579</v>
-      </c>
-      <c r="C11">
-        <v>902.81754302978504</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>268</v>
-      </c>
-      <c r="B12">
-        <v>341259</v>
-      </c>
-      <c r="C12">
-        <v>902.71302103996197</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>269</v>
-      </c>
-      <c r="B13">
-        <v>334500</v>
-      </c>
-      <c r="C13">
-        <v>902.76530218124299</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>270</v>
-      </c>
-      <c r="B14">
-        <v>336912</v>
-      </c>
-      <c r="C14">
-        <v>902.78485202789295</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>271</v>
-      </c>
-      <c r="B15">
-        <v>333923</v>
-      </c>
-      <c r="C15">
-        <v>902.75450706481899</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>272</v>
-      </c>
-      <c r="B16">
-        <v>337657</v>
-      </c>
-      <c r="C16">
-        <v>902.712965011596</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>273</v>
-      </c>
-      <c r="B17">
-        <v>511857</v>
-      </c>
-      <c r="C17">
-        <v>911.37733507156304</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>274</v>
-      </c>
-      <c r="B18">
-        <v>511692</v>
-      </c>
-      <c r="C18">
-        <v>911.29974985122601</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>275</v>
-      </c>
-      <c r="B19">
-        <v>511164</v>
-      </c>
-      <c r="C19">
-        <v>909.99310088157597</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>276</v>
-      </c>
-      <c r="B20">
-        <v>511333</v>
-      </c>
-      <c r="C20">
-        <v>909.94816899299599</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>277</v>
-      </c>
-      <c r="B21">
-        <v>511659</v>
-      </c>
-      <c r="C21">
-        <v>909.94293403625397</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>278</v>
-      </c>
-      <c r="B22">
-        <v>544990</v>
-      </c>
-      <c r="C22">
-        <v>909.91394376754704</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>279</v>
-      </c>
-      <c r="B23">
-        <v>543833</v>
-      </c>
-      <c r="C23">
-        <v>909.87025308608997</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>280</v>
-      </c>
-      <c r="B24">
-        <v>544177</v>
-      </c>
-      <c r="C24">
-        <v>910.11111402511597</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>281</v>
-      </c>
-      <c r="B25">
-        <v>544017</v>
-      </c>
-      <c r="C25">
-        <v>909.91126084327698</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>282</v>
-      </c>
-      <c r="B26">
-        <v>542311</v>
-      </c>
-      <c r="C26">
-        <v>910.70027804374695</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>283</v>
-      </c>
-      <c r="B27">
-        <v>651242</v>
-      </c>
-      <c r="C27">
-        <v>909.854112148284</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>284</v>
-      </c>
-      <c r="B28">
-        <v>650678</v>
-      </c>
-      <c r="C28">
-        <v>909.89395713806096</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>285</v>
-      </c>
-      <c r="B29">
-        <v>635921</v>
-      </c>
-      <c r="C29">
-        <v>917.24749302863995</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>286</v>
-      </c>
-      <c r="B30">
-        <v>653109</v>
-      </c>
-      <c r="C30">
-        <v>914.40007305145195</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>287</v>
-      </c>
-      <c r="B31">
-        <v>656085</v>
-      </c>
-      <c r="C31">
-        <v>909.84456491470303</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>288</v>
-      </c>
-      <c r="B32">
-        <v>764497</v>
-      </c>
-      <c r="C32">
-        <v>922.48159003257695</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>289</v>
-      </c>
-      <c r="B33">
-        <v>764393</v>
-      </c>
-      <c r="C33">
-        <v>923.70001530647198</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>290</v>
-      </c>
-      <c r="B34">
-        <v>764683</v>
-      </c>
-      <c r="C34">
-        <v>922.49204611778202</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>291</v>
-      </c>
-      <c r="B35">
-        <v>765003</v>
-      </c>
-      <c r="C35">
-        <v>967.331067085266</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>292</v>
-      </c>
-      <c r="B36">
-        <v>764839</v>
-      </c>
-      <c r="C36">
-        <v>922.35739517211903</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>293</v>
-      </c>
-      <c r="B37">
-        <v>804333</v>
-      </c>
-      <c r="C37">
-        <v>922.56556200981095</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>294</v>
-      </c>
-      <c r="B38">
-        <v>803382</v>
-      </c>
-      <c r="C38">
-        <v>922.20214200019802</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>295</v>
-      </c>
-      <c r="B39">
-        <v>804625</v>
-      </c>
-      <c r="C39">
-        <v>922.59399294853199</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>296</v>
-      </c>
-      <c r="B40">
-        <v>806073</v>
-      </c>
-      <c r="C40">
-        <v>922.38513612747101</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>297</v>
-      </c>
-      <c r="B41">
-        <v>804822</v>
-      </c>
-      <c r="C41">
-        <v>922.39462590217499</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>298</v>
-      </c>
-      <c r="B42">
-        <v>8314623</v>
-      </c>
-      <c r="C42">
-        <v>922.52507877349797</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>299</v>
-      </c>
-      <c r="B43">
-        <v>8238967</v>
-      </c>
-      <c r="C43">
-        <v>922.15382504463196</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>300</v>
-      </c>
-      <c r="B44">
-        <v>8272022</v>
-      </c>
-      <c r="C44">
-        <v>922.41212320327702</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>301</v>
-      </c>
-      <c r="B45">
-        <v>8293624</v>
-      </c>
-      <c r="C45">
-        <v>922.37150001525799</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>302</v>
-      </c>
-      <c r="B46">
-        <v>8113598</v>
-      </c>
-      <c r="C46">
-        <v>922.51200389862004</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>303</v>
-      </c>
-      <c r="B47">
-        <v>257982</v>
-      </c>
-      <c r="C47">
-        <v>902.45427799224797</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>304</v>
-      </c>
-      <c r="B48">
-        <v>257573</v>
-      </c>
-      <c r="C48">
-        <v>902.71455574035599</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>305</v>
-      </c>
-      <c r="B49">
-        <v>257637</v>
-      </c>
-      <c r="C49">
-        <v>902.45287489890995</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>306</v>
-      </c>
-      <c r="B50">
-        <v>258002</v>
-      </c>
-      <c r="C50">
-        <v>902.86888289451599</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>307</v>
-      </c>
-      <c r="B51">
-        <v>257947</v>
-      </c>
-      <c r="C51">
-        <v>902.55648112297001</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>308</v>
-      </c>
-      <c r="B52">
-        <v>277963</v>
-      </c>
-      <c r="C52">
-        <v>902.70880317687897</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>309</v>
-      </c>
-      <c r="B53">
-        <v>277186</v>
-      </c>
-      <c r="C53">
-        <v>902.76570177078202</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>310</v>
-      </c>
-      <c r="B54">
-        <v>277318</v>
-      </c>
-      <c r="C54">
-        <v>903.03716206550598</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>311</v>
-      </c>
-      <c r="B55">
-        <v>277503</v>
-      </c>
-      <c r="C55">
-        <v>903.02846908569302</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>312</v>
-      </c>
-      <c r="B56">
-        <v>277660</v>
-      </c>
-      <c r="C56">
-        <v>902.86114811897198</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>313</v>
-      </c>
-      <c r="B57">
-        <v>335250</v>
-      </c>
-      <c r="C57">
-        <v>902.81879806518498</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>314</v>
-      </c>
-      <c r="B58">
-        <v>337978</v>
-      </c>
-      <c r="C58">
-        <v>902.66474580764702</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>315</v>
-      </c>
-      <c r="B59">
-        <v>334568</v>
-      </c>
-      <c r="C59">
-        <v>902.43451786041203</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>316</v>
-      </c>
-      <c r="B60">
-        <v>336775</v>
-      </c>
-      <c r="C60">
-        <v>902.83008790016095</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>317</v>
-      </c>
-      <c r="B61">
-        <v>336807</v>
-      </c>
-      <c r="C61">
-        <v>902.78700304031304</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>318</v>
-      </c>
-      <c r="B62">
-        <v>511596</v>
-      </c>
-      <c r="C62">
-        <v>911.28729915618896</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>319</v>
-      </c>
-      <c r="B63">
-        <v>511543</v>
-      </c>
-      <c r="C63">
-        <v>911.35703802108696</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>320</v>
-      </c>
-      <c r="B64">
-        <v>511820</v>
-      </c>
-      <c r="C64">
-        <v>910.53267502784695</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>321</v>
-      </c>
-      <c r="B65">
-        <v>511720</v>
-      </c>
-      <c r="C65">
-        <v>911.17584109306301</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>322</v>
-      </c>
-      <c r="B66">
-        <v>511896</v>
-      </c>
-      <c r="C66">
-        <v>911.82793593406598</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>323</v>
-      </c>
-      <c r="B67">
-        <v>543113</v>
-      </c>
-      <c r="C67">
-        <v>910.08405399322498</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>324</v>
-      </c>
-      <c r="B68">
-        <v>544757</v>
-      </c>
-      <c r="C68">
-        <v>910.17574715614296</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>325</v>
-      </c>
-      <c r="B69">
-        <v>545082</v>
-      </c>
-      <c r="C69">
-        <v>910.02588105201698</v>
-      </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>326</v>
-      </c>
-      <c r="B70">
-        <v>544587</v>
-      </c>
-      <c r="C70">
-        <v>910.35155200958195</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>327</v>
-      </c>
-      <c r="B71">
-        <v>543683</v>
-      </c>
-      <c r="C71">
-        <v>910.50993108749299</v>
-      </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>328</v>
-      </c>
-      <c r="B72">
-        <v>650774</v>
-      </c>
-      <c r="C72">
-        <v>911.23421382903996</v>
-      </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>329</v>
-      </c>
-      <c r="B73">
-        <v>652789</v>
-      </c>
-      <c r="C73">
-        <v>911.64885783195496</v>
-      </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>330</v>
-      </c>
-      <c r="B74">
-        <v>651278</v>
-      </c>
-      <c r="C74">
-        <v>911.36014986038197</v>
-      </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>331</v>
-      </c>
-      <c r="B75">
-        <v>650240</v>
-      </c>
-      <c r="C75">
-        <v>911.308551073074</v>
-      </c>
-      <c r="D75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>332</v>
-      </c>
-      <c r="B76">
-        <v>653596</v>
-      </c>
-      <c r="C76">
-        <v>910.14066624641396</v>
-      </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>333</v>
-      </c>
-      <c r="B77">
-        <v>764489</v>
-      </c>
-      <c r="C77">
-        <v>925.529658079147</v>
-      </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>334</v>
-      </c>
-      <c r="B78">
-        <v>764323</v>
-      </c>
-      <c r="C78">
-        <v>922.64379024505604</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>335</v>
-      </c>
-      <c r="B79">
-        <v>764514</v>
-      </c>
-      <c r="C79">
-        <v>943.27610707282997</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>336</v>
-      </c>
-      <c r="B80">
-        <v>764778</v>
-      </c>
-      <c r="C80">
-        <v>1000.9630742073</v>
-      </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>337</v>
-      </c>
-      <c r="B81">
-        <v>764518</v>
-      </c>
-      <c r="C81">
-        <v>923.41966295242298</v>
-      </c>
-      <c r="D81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>338</v>
-      </c>
-      <c r="B82">
-        <v>805705</v>
-      </c>
-      <c r="C82">
-        <v>923.70170497894196</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>339</v>
-      </c>
-      <c r="B83">
-        <v>804801</v>
-      </c>
-      <c r="C83">
-        <v>925.14163589477505</v>
-      </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>340</v>
-      </c>
-      <c r="B84">
-        <v>806007</v>
-      </c>
-      <c r="C84">
-        <v>926.23342895507801</v>
-      </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>341</v>
-      </c>
-      <c r="B85">
-        <v>804453</v>
-      </c>
-      <c r="C85">
-        <v>925.72512578964199</v>
-      </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>342</v>
-      </c>
-      <c r="B86">
-        <v>805745</v>
-      </c>
-      <c r="C86">
-        <v>926.446646928787</v>
-      </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>343</v>
-      </c>
-      <c r="B87">
-        <v>8243622</v>
-      </c>
-      <c r="C87">
-        <v>926.22148108482304</v>
-      </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>344</v>
-      </c>
-      <c r="B88">
-        <v>8373748</v>
-      </c>
-      <c r="C88">
-        <v>925.34666800498906</v>
-      </c>
-      <c r="D88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>345</v>
-      </c>
-      <c r="B89">
-        <v>8264997</v>
-      </c>
-      <c r="C89">
-        <v>925.06150794029202</v>
-      </c>
-      <c r="D89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>346</v>
-      </c>
-      <c r="B90">
-        <v>8320376</v>
-      </c>
-      <c r="C90">
-        <v>927.86582994461003</v>
-      </c>
-      <c r="D90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>347</v>
-      </c>
-      <c r="B91">
-        <v>8384003</v>
-      </c>
-      <c r="C91">
-        <v>924.673907995224</v>
-      </c>
-      <c r="D91">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1096"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="111" workbookViewId="0">
-      <selection activeCell="H252" sqref="H252"/>
+    <sheetView tabSelected="1" topLeftCell="L228" zoomScale="111" workbookViewId="0">
+      <selection activeCell="M234" sqref="M234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23142,7 +21831,7 @@
         <v>0</v>
       </c>
       <c r="V195" s="17">
-        <f t="shared" ref="V195:V238" si="45">U195/B195</f>
+        <f t="shared" ref="V195:V254" si="45">U195/B195</f>
         <v>0</v>
       </c>
       <c r="W195" s="1"/>
@@ -27635,7 +26324,7 @@
       </c>
       <c r="W239" s="1"/>
       <c r="X239" s="10">
-        <f t="shared" ref="X239" si="65">S239-C239</f>
+        <f t="shared" ref="X239:X241" si="65">S239-C239</f>
         <v>-28.54945516586298</v>
       </c>
       <c r="Y239" s="17">
@@ -27705,11 +26394,23 @@
       <c r="R240" s="10"/>
       <c r="S240" s="10"/>
       <c r="T240" s="1"/>
-      <c r="U240" s="10"/>
-      <c r="V240" s="17"/>
+      <c r="U240" s="10">
+        <f t="shared" ref="U240:U264" si="66">R240-B240</f>
+        <v>-55342977</v>
+      </c>
+      <c r="V240" s="17">
+        <f t="shared" ref="V240:V264" si="67">U240/B240</f>
+        <v>-1</v>
+      </c>
       <c r="W240" s="1"/>
-      <c r="X240" s="10"/>
-      <c r="Y240" s="17"/>
+      <c r="X240" s="10">
+        <f t="shared" si="65"/>
+        <v>-1606.694</v>
+      </c>
+      <c r="Y240" s="17">
+        <f t="shared" ref="Y240:Y264" si="68">X240/C240</f>
+        <v>-1</v>
+      </c>
       <c r="Z240" s="1"/>
       <c r="AA240" s="3" t="s">
         <v>254</v>
@@ -27773,11 +26474,23 @@
       <c r="R241" s="10"/>
       <c r="S241" s="10"/>
       <c r="T241" s="1"/>
-      <c r="U241" s="10"/>
-      <c r="V241" s="17"/>
+      <c r="U241" s="10">
+        <f t="shared" si="66"/>
+        <v>-39631404</v>
+      </c>
+      <c r="V241" s="17">
+        <f t="shared" si="67"/>
+        <v>-1</v>
+      </c>
       <c r="W241" s="1"/>
-      <c r="X241" s="10"/>
-      <c r="Y241" s="17"/>
+      <c r="X241" s="10">
+        <f t="shared" si="65"/>
+        <v>-1903.46</v>
+      </c>
+      <c r="Y241" s="17">
+        <f t="shared" si="68"/>
+        <v>-1</v>
+      </c>
       <c r="Z241" s="1"/>
       <c r="AA241" s="3" t="s">
         <v>255</v>
@@ -27841,11 +26554,23 @@
       <c r="R242" s="10"/>
       <c r="S242" s="10"/>
       <c r="T242" s="1"/>
-      <c r="U242" s="10"/>
-      <c r="V242" s="17"/>
+      <c r="U242" s="10">
+        <f t="shared" si="66"/>
+        <v>-64172666</v>
+      </c>
+      <c r="V242" s="17">
+        <f t="shared" si="67"/>
+        <v>-1</v>
+      </c>
       <c r="W242" s="1"/>
-      <c r="X242" s="10"/>
-      <c r="Y242" s="17"/>
+      <c r="X242" s="10">
+        <f t="shared" ref="X242:X264" si="69">S242-C242</f>
+        <v>-5842.8617999999997</v>
+      </c>
+      <c r="Y242" s="17">
+        <f t="shared" si="68"/>
+        <v>-1</v>
+      </c>
       <c r="Z242" s="1"/>
       <c r="AA242" s="3" t="s">
         <v>256</v>
@@ -27862,7 +26587,7 @@
         <v>-61744226</v>
       </c>
       <c r="AF242" s="8">
-        <f t="shared" ref="AF242" si="66">AE242/B242</f>
+        <f t="shared" ref="AF242" si="70">AE242/B242</f>
         <v>-0.96215771992393151</v>
       </c>
       <c r="AG242" s="1"/>
@@ -27882,6 +26607,31 @@
       </c>
       <c r="D243" s="10">
         <v>0</v>
+      </c>
+      <c r="Q243" t="s">
+        <v>258</v>
+      </c>
+      <c r="R243">
+        <v>257957</v>
+      </c>
+      <c r="S243">
+        <v>902.94870400428704</v>
+      </c>
+      <c r="U243" s="10">
+        <f t="shared" si="66"/>
+        <v>-31</v>
+      </c>
+      <c r="V243" s="17">
+        <f t="shared" si="67"/>
+        <v>-1.2016062762609114E-4</v>
+      </c>
+      <c r="X243" s="10">
+        <f t="shared" si="69"/>
+        <v>-2.5698080062869622</v>
+      </c>
+      <c r="Y243" s="17">
+        <f t="shared" si="68"/>
+        <v>-2.8379408838159169E-3</v>
       </c>
     </row>
     <row r="244" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27909,15 +26659,33 @@
       <c r="N244" s="1"/>
       <c r="O244" s="1"/>
       <c r="P244" s="1"/>
-      <c r="Q244" s="1"/>
-      <c r="R244" s="1"/>
-      <c r="S244" s="1"/>
+      <c r="Q244" t="s">
+        <v>259</v>
+      </c>
+      <c r="R244">
+        <v>257502</v>
+      </c>
+      <c r="S244">
+        <v>646.22315716743401</v>
+      </c>
       <c r="T244" s="1"/>
-      <c r="U244" s="1"/>
-      <c r="V244" s="1"/>
+      <c r="U244" s="10">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="V244" s="17">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
       <c r="W244" s="1"/>
-      <c r="X244" s="1"/>
-      <c r="Y244" s="1"/>
+      <c r="X244" s="10">
+        <f t="shared" si="69"/>
+        <v>-256.53400802612293</v>
+      </c>
+      <c r="Y244" s="17">
+        <f t="shared" si="68"/>
+        <v>-0.28416723557228196</v>
+      </c>
       <c r="Z244" s="1"/>
       <c r="AA244" s="1"/>
       <c r="AB244" s="1"/>
@@ -27968,27 +26736,31 @@
         <v>-0.96236788666542994</v>
       </c>
       <c r="P245" s="1"/>
-      <c r="Q245" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="R245" s="23"/>
-      <c r="S245" s="7">
-        <f>SUM(S3:S242)</f>
-        <v>999.63952136039632</v>
+      <c r="Q245" t="s">
+        <v>260</v>
+      </c>
+      <c r="R245">
+        <v>257966</v>
+      </c>
+      <c r="S245">
+        <v>903.84508395194996</v>
       </c>
       <c r="T245" s="1"/>
-      <c r="U245" s="1"/>
-      <c r="V245" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="W245" s="23"/>
-      <c r="X245" s="7">
-        <f>S245-C335</f>
-        <v>-10758.029428244399</v>
-      </c>
-      <c r="Y245" s="25">
-        <f>X245/C335</f>
-        <v>-0.91497978675492508</v>
+      <c r="U245" s="10">
+        <f t="shared" si="66"/>
+        <v>-216</v>
+      </c>
+      <c r="V245" s="17">
+        <f t="shared" si="67"/>
+        <v>-8.366191291414583E-4</v>
+      </c>
+      <c r="X245" s="10">
+        <f t="shared" si="69"/>
+        <v>0.66050171852100448</v>
+      </c>
+      <c r="Y245" s="17">
+        <f t="shared" si="68"/>
+        <v>7.3130313726978255E-4</v>
       </c>
       <c r="Z245" s="1"/>
       <c r="AA245" s="24" t="s">
@@ -28050,25 +26822,32 @@
       </c>
       <c r="O246" s="26"/>
       <c r="P246" s="1"/>
-      <c r="Q246" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="R246" s="23"/>
-      <c r="S246" s="7">
-        <f>S245/60</f>
-        <v>16.66065868933994</v>
+      <c r="Q246" t="s">
+        <v>261</v>
+      </c>
+      <c r="R246">
+        <v>258005</v>
+      </c>
+      <c r="S246">
+        <v>904.08771204948403</v>
       </c>
       <c r="T246" s="1"/>
-      <c r="U246" s="1"/>
-      <c r="V246" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="W246" s="23"/>
-      <c r="X246" s="7">
-        <f>S246-C336</f>
-        <v>-179.30049047073999</v>
-      </c>
-      <c r="Y246" s="26"/>
+      <c r="U246" s="10">
+        <f t="shared" si="66"/>
+        <v>18</v>
+      </c>
+      <c r="V246" s="17">
+        <f t="shared" si="67"/>
+        <v>6.9770957451344449E-5</v>
+      </c>
+      <c r="X246" s="10">
+        <f t="shared" si="69"/>
+        <v>1.4113969802859856</v>
+      </c>
+      <c r="Y246" s="17">
+        <f t="shared" si="68"/>
+        <v>1.5635693068758426E-3</v>
+      </c>
       <c r="Z246" s="1"/>
       <c r="AA246" s="24" t="s">
         <v>246</v>
@@ -28116,15 +26895,33 @@
       <c r="N247" s="1"/>
       <c r="O247" s="1"/>
       <c r="P247" s="1"/>
-      <c r="Q247" s="1"/>
-      <c r="R247" s="1"/>
-      <c r="S247" s="1"/>
+      <c r="Q247" t="s">
+        <v>262</v>
+      </c>
+      <c r="R247">
+        <v>258190</v>
+      </c>
+      <c r="S247">
+        <v>904.72833204269398</v>
+      </c>
       <c r="T247" s="1"/>
-      <c r="U247" s="1"/>
-      <c r="V247" s="1"/>
+      <c r="U247" s="10">
+        <f t="shared" si="66"/>
+        <v>-90</v>
+      </c>
+      <c r="V247" s="17">
+        <f t="shared" si="67"/>
+        <v>-3.4845903670435187E-4</v>
+      </c>
       <c r="W247" s="1"/>
-      <c r="X247" s="1"/>
-      <c r="Y247" s="1"/>
+      <c r="X247" s="10">
+        <f t="shared" si="69"/>
+        <v>1.7755820751190186</v>
+      </c>
+      <c r="Y247" s="17">
+        <f t="shared" si="68"/>
+        <v>1.9664174843952572E-3</v>
+      </c>
       <c r="Z247" s="1"/>
       <c r="AA247" s="1"/>
       <c r="AB247" s="1"/>
@@ -28162,15 +26959,33 @@
       <c r="N248" s="1"/>
       <c r="O248" s="1"/>
       <c r="P248" s="1"/>
-      <c r="Q248" s="1"/>
-      <c r="R248" s="1"/>
-      <c r="S248" s="1"/>
+      <c r="Q248" t="s">
+        <v>263</v>
+      </c>
+      <c r="R248">
+        <v>276296</v>
+      </c>
+      <c r="S248">
+        <v>904.17506408691395</v>
+      </c>
       <c r="T248" s="1"/>
-      <c r="U248" s="1"/>
-      <c r="V248" s="1"/>
+      <c r="U248" s="10">
+        <f t="shared" si="66"/>
+        <v>-1091</v>
+      </c>
+      <c r="V248" s="17">
+        <f t="shared" si="67"/>
+        <v>-3.933133131689661E-3</v>
+      </c>
       <c r="W248" s="1"/>
-      <c r="X248" s="1"/>
-      <c r="Y248" s="1"/>
+      <c r="X248" s="10">
+        <f t="shared" si="69"/>
+        <v>1.715537786483992</v>
+      </c>
+      <c r="Y248" s="17">
+        <f t="shared" si="68"/>
+        <v>1.9009581443687783E-3</v>
+      </c>
       <c r="Z248" s="1"/>
       <c r="AA248" s="1"/>
       <c r="AB248" s="1"/>
@@ -28208,15 +27023,33 @@
       <c r="N249" s="1"/>
       <c r="O249" s="1"/>
       <c r="P249" s="1"/>
-      <c r="Q249" s="1"/>
-      <c r="R249" s="1"/>
-      <c r="S249" s="1"/>
+      <c r="Q249" t="s">
+        <v>264</v>
+      </c>
+      <c r="R249">
+        <v>275150</v>
+      </c>
+      <c r="S249">
+        <v>905.37515091896</v>
+      </c>
       <c r="T249" s="1"/>
-      <c r="U249" s="1"/>
-      <c r="V249" s="1"/>
+      <c r="U249" s="10">
+        <f t="shared" si="66"/>
+        <v>-958</v>
+      </c>
+      <c r="V249" s="17">
+        <f t="shared" si="67"/>
+        <v>-3.4696568009619424E-3</v>
+      </c>
       <c r="W249" s="1"/>
-      <c r="X249" s="1"/>
-      <c r="Y249" s="1"/>
+      <c r="X249" s="10">
+        <f t="shared" si="69"/>
+        <v>2.9182381629940437</v>
+      </c>
+      <c r="Y249" s="17">
+        <f t="shared" si="68"/>
+        <v>3.233659271424038E-3</v>
+      </c>
       <c r="Z249" s="1"/>
       <c r="AA249" s="1"/>
       <c r="AB249" s="1"/>
@@ -28254,15 +27087,33 @@
       <c r="N250" s="1"/>
       <c r="O250" s="1"/>
       <c r="P250" s="1"/>
-      <c r="Q250" s="1"/>
-      <c r="R250" s="1"/>
-      <c r="S250" s="1"/>
+      <c r="Q250" t="s">
+        <v>265</v>
+      </c>
+      <c r="R250">
+        <v>276252</v>
+      </c>
+      <c r="S250">
+        <v>903.11568903923001</v>
+      </c>
       <c r="T250" s="1"/>
-      <c r="U250" s="1"/>
-      <c r="V250" s="1"/>
+      <c r="U250" s="10">
+        <f t="shared" si="66"/>
+        <v>-1068</v>
+      </c>
+      <c r="V250" s="17">
+        <f t="shared" si="67"/>
+        <v>-3.8511466897446995E-3</v>
+      </c>
       <c r="W250" s="1"/>
-      <c r="X250" s="1"/>
-      <c r="Y250" s="1"/>
+      <c r="X250" s="10">
+        <f t="shared" si="69"/>
+        <v>0.39349102973903882</v>
+      </c>
+      <c r="Y250" s="17">
+        <f t="shared" si="68"/>
+        <v>4.358938227138863E-4</v>
+      </c>
       <c r="Z250" s="1"/>
       <c r="AA250" s="1"/>
       <c r="AB250" s="1"/>
@@ -28300,15 +27151,33 @@
       <c r="N251" s="1"/>
       <c r="O251" s="1"/>
       <c r="P251" s="1"/>
-      <c r="Q251" s="1"/>
-      <c r="R251" s="1"/>
-      <c r="S251" s="1"/>
+      <c r="Q251" t="s">
+        <v>266</v>
+      </c>
+      <c r="R251">
+        <v>276403</v>
+      </c>
+      <c r="S251">
+        <v>905.14797997474602</v>
+      </c>
       <c r="T251" s="1"/>
-      <c r="U251" s="1"/>
-      <c r="V251" s="1"/>
+      <c r="U251" s="10">
+        <f t="shared" si="66"/>
+        <v>-2244</v>
+      </c>
+      <c r="V251" s="17">
+        <f t="shared" si="67"/>
+        <v>-8.0531999267890921E-3</v>
+      </c>
       <c r="W251" s="1"/>
-      <c r="X251" s="1"/>
-      <c r="Y251" s="1"/>
+      <c r="X251" s="10">
+        <f t="shared" si="69"/>
+        <v>2.420543193817025</v>
+      </c>
+      <c r="Y251" s="17">
+        <f t="shared" si="68"/>
+        <v>2.6813665954903668E-3</v>
+      </c>
       <c r="Z251" s="1"/>
       <c r="AA251" s="1"/>
       <c r="AB251" s="1"/>
@@ -28346,15 +27215,33 @@
       <c r="N252" s="1"/>
       <c r="O252" s="1"/>
       <c r="P252" s="1"/>
-      <c r="Q252" s="1"/>
-      <c r="R252" s="1"/>
-      <c r="S252" s="1"/>
+      <c r="Q252" t="s">
+        <v>267</v>
+      </c>
+      <c r="R252">
+        <v>276404</v>
+      </c>
+      <c r="S252">
+        <v>905.19020795822098</v>
+      </c>
       <c r="T252" s="1"/>
-      <c r="U252" s="1"/>
-      <c r="V252" s="1"/>
+      <c r="U252" s="10">
+        <f t="shared" si="66"/>
+        <v>-1175</v>
+      </c>
+      <c r="V252" s="17">
+        <f t="shared" si="67"/>
+        <v>-4.2330291556637928E-3</v>
+      </c>
       <c r="W252" s="1"/>
-      <c r="X252" s="1"/>
-      <c r="Y252" s="1"/>
+      <c r="X252" s="10">
+        <f t="shared" si="69"/>
+        <v>2.3726649284359382</v>
+      </c>
+      <c r="Y252" s="17">
+        <f t="shared" si="68"/>
+        <v>2.6280669297513433E-3</v>
+      </c>
       <c r="Z252" s="1"/>
       <c r="AA252" s="1"/>
       <c r="AB252" s="1"/>
@@ -28392,15 +27279,33 @@
       <c r="N253" s="1"/>
       <c r="O253" s="1"/>
       <c r="P253" s="1"/>
-      <c r="Q253" s="1"/>
-      <c r="R253" s="1"/>
-      <c r="S253" s="1"/>
+      <c r="Q253" t="s">
+        <v>268</v>
+      </c>
+      <c r="R253">
+        <v>334694</v>
+      </c>
+      <c r="S253">
+        <v>904.03681874275196</v>
+      </c>
       <c r="T253" s="1"/>
-      <c r="U253" s="1"/>
-      <c r="V253" s="1"/>
+      <c r="U253" s="10">
+        <f t="shared" si="66"/>
+        <v>-6565</v>
+      </c>
+      <c r="V253" s="17">
+        <f t="shared" si="67"/>
+        <v>-1.9237587873140342E-2</v>
+      </c>
       <c r="W253" s="1"/>
-      <c r="X253" s="1"/>
-      <c r="Y253" s="1"/>
+      <c r="X253" s="10">
+        <f t="shared" si="69"/>
+        <v>1.3237977027899888</v>
+      </c>
+      <c r="Y253" s="17">
+        <f t="shared" si="68"/>
+        <v>1.466465722699912E-3</v>
+      </c>
       <c r="Z253" s="1"/>
       <c r="AA253" s="1"/>
       <c r="AB253" s="1"/>
@@ -28438,15 +27343,33 @@
       <c r="N254" s="1"/>
       <c r="O254" s="1"/>
       <c r="P254" s="1"/>
-      <c r="Q254" s="1"/>
-      <c r="R254" s="1"/>
-      <c r="S254" s="1"/>
+      <c r="Q254" t="s">
+        <v>269</v>
+      </c>
+      <c r="R254">
+        <v>333782</v>
+      </c>
+      <c r="S254">
+        <v>904.95290088653496</v>
+      </c>
       <c r="T254" s="1"/>
-      <c r="U254" s="1"/>
-      <c r="V254" s="1"/>
+      <c r="U254" s="10">
+        <f t="shared" si="66"/>
+        <v>-718</v>
+      </c>
+      <c r="V254" s="17">
+        <f t="shared" si="67"/>
+        <v>-2.1464872944693572E-3</v>
+      </c>
       <c r="W254" s="1"/>
-      <c r="X254" s="1"/>
-      <c r="Y254" s="1"/>
+      <c r="X254" s="10">
+        <f t="shared" si="69"/>
+        <v>2.1875987052919754</v>
+      </c>
+      <c r="Y254" s="17">
+        <f t="shared" si="68"/>
+        <v>2.4232197449396255E-3</v>
+      </c>
       <c r="Z254" s="1"/>
       <c r="AA254" s="1"/>
       <c r="AB254" s="1"/>
@@ -28484,15 +27407,33 @@
       <c r="N255" s="1"/>
       <c r="O255" s="1"/>
       <c r="P255" s="1"/>
-      <c r="Q255" s="1"/>
-      <c r="R255" s="1"/>
-      <c r="S255" s="1"/>
+      <c r="Q255" t="s">
+        <v>270</v>
+      </c>
+      <c r="R255">
+        <v>334151</v>
+      </c>
+      <c r="S255">
+        <v>903.62970805168095</v>
+      </c>
       <c r="T255" s="1"/>
-      <c r="U255" s="1"/>
-      <c r="V255" s="1"/>
+      <c r="U255" s="10">
+        <f t="shared" si="66"/>
+        <v>-2761</v>
+      </c>
+      <c r="V255" s="17">
+        <f t="shared" si="67"/>
+        <v>-8.1950182837061316E-3</v>
+      </c>
       <c r="W255" s="1"/>
-      <c r="X255" s="1"/>
-      <c r="Y255" s="1"/>
+      <c r="X255" s="10">
+        <f t="shared" si="69"/>
+        <v>0.8448560237879974</v>
+      </c>
+      <c r="Y255" s="17">
+        <f t="shared" si="68"/>
+        <v>9.3583318538212942E-4</v>
+      </c>
       <c r="Z255" s="1"/>
       <c r="AA255" s="1"/>
       <c r="AB255" s="1"/>
@@ -28530,15 +27471,33 @@
       <c r="N256" s="1"/>
       <c r="O256" s="1"/>
       <c r="P256" s="1"/>
-      <c r="Q256" s="1"/>
-      <c r="R256" s="1"/>
-      <c r="S256" s="1"/>
+      <c r="Q256" t="s">
+        <v>271</v>
+      </c>
+      <c r="R256">
+        <v>332423</v>
+      </c>
+      <c r="S256">
+        <v>902.60521602630604</v>
+      </c>
       <c r="T256" s="1"/>
-      <c r="U256" s="1"/>
-      <c r="V256" s="1"/>
+      <c r="U256" s="10">
+        <f t="shared" si="66"/>
+        <v>-1500</v>
+      </c>
+      <c r="V256" s="17">
+        <f t="shared" si="67"/>
+        <v>-4.4920535572572119E-3</v>
+      </c>
       <c r="W256" s="1"/>
-      <c r="X256" s="1"/>
-      <c r="Y256" s="1"/>
+      <c r="X256" s="10">
+        <f t="shared" si="69"/>
+        <v>-0.14929103851295622</v>
+      </c>
+      <c r="Y256" s="17">
+        <f t="shared" si="68"/>
+        <v>-1.6537279774803376E-4</v>
+      </c>
       <c r="Z256" s="1"/>
       <c r="AA256" s="1"/>
       <c r="AB256" s="1"/>
@@ -28576,15 +27535,33 @@
       <c r="N257" s="1"/>
       <c r="O257" s="1"/>
       <c r="P257" s="1"/>
-      <c r="Q257" s="1"/>
-      <c r="R257" s="1"/>
-      <c r="S257" s="1"/>
+      <c r="Q257" t="s">
+        <v>272</v>
+      </c>
+      <c r="R257">
+        <v>333944</v>
+      </c>
+      <c r="S257">
+        <v>902.54419922828595</v>
+      </c>
       <c r="T257" s="1"/>
-      <c r="U257" s="1"/>
-      <c r="V257" s="1"/>
+      <c r="U257" s="10">
+        <f t="shared" si="66"/>
+        <v>-3713</v>
+      </c>
+      <c r="V257" s="17">
+        <f t="shared" si="67"/>
+        <v>-1.099636613486467E-2</v>
+      </c>
       <c r="W257" s="1"/>
-      <c r="X257" s="1"/>
-      <c r="Y257" s="1"/>
+      <c r="X257" s="10">
+        <f t="shared" si="69"/>
+        <v>-0.16876578331005021</v>
+      </c>
+      <c r="Y257" s="17">
+        <f t="shared" si="68"/>
+        <v>-1.8695398188712433E-4</v>
+      </c>
       <c r="Z257" s="1"/>
       <c r="AA257" s="1"/>
       <c r="AB257" s="1"/>
@@ -28622,15 +27599,33 @@
       <c r="N258" s="1"/>
       <c r="O258" s="1"/>
       <c r="P258" s="1"/>
-      <c r="Q258" s="1"/>
-      <c r="R258" s="1"/>
-      <c r="S258" s="1"/>
+      <c r="Q258" t="s">
+        <v>273</v>
+      </c>
+      <c r="R258">
+        <v>511635</v>
+      </c>
+      <c r="S258">
+        <v>910.73574590682904</v>
+      </c>
       <c r="T258" s="1"/>
-      <c r="U258" s="1"/>
-      <c r="V258" s="1"/>
+      <c r="U258" s="10">
+        <f t="shared" si="66"/>
+        <v>-222</v>
+      </c>
+      <c r="V258" s="17">
+        <f t="shared" si="67"/>
+        <v>-4.3371488521208069E-4</v>
+      </c>
       <c r="W258" s="1"/>
-      <c r="X258" s="1"/>
-      <c r="Y258" s="1"/>
+      <c r="X258" s="10">
+        <f t="shared" si="69"/>
+        <v>-0.64158916473400041</v>
+      </c>
+      <c r="Y258" s="17">
+        <f t="shared" si="68"/>
+        <v>-7.03977529442974E-4</v>
+      </c>
       <c r="Z258" s="1"/>
       <c r="AA258" s="1"/>
       <c r="AB258" s="1"/>
@@ -28668,15 +27663,33 @@
       <c r="N259" s="1"/>
       <c r="O259" s="1"/>
       <c r="P259" s="1"/>
-      <c r="Q259" s="1"/>
-      <c r="R259" s="1"/>
-      <c r="S259" s="1"/>
+      <c r="Q259" t="s">
+        <v>274</v>
+      </c>
+      <c r="R259">
+        <v>511533</v>
+      </c>
+      <c r="S259">
+        <v>910.28540015220597</v>
+      </c>
       <c r="T259" s="1"/>
-      <c r="U259" s="1"/>
-      <c r="V259" s="1"/>
+      <c r="U259" s="10">
+        <f t="shared" si="66"/>
+        <v>-159</v>
+      </c>
+      <c r="V259" s="17">
+        <f t="shared" si="67"/>
+        <v>-3.10733800802045E-4</v>
+      </c>
       <c r="W259" s="1"/>
-      <c r="X259" s="1"/>
-      <c r="Y259" s="1"/>
+      <c r="X259" s="10">
+        <f t="shared" si="69"/>
+        <v>-1.0143496990200447</v>
+      </c>
+      <c r="Y259" s="17">
+        <f t="shared" si="68"/>
+        <v>-1.1130801903387355E-3</v>
+      </c>
       <c r="Z259" s="1"/>
       <c r="AA259" s="1"/>
       <c r="AB259" s="1"/>
@@ -28714,15 +27727,33 @@
       <c r="N260" s="1"/>
       <c r="O260" s="1"/>
       <c r="P260" s="1"/>
-      <c r="Q260" s="1"/>
-      <c r="R260" s="1"/>
-      <c r="S260" s="1"/>
+      <c r="Q260" t="s">
+        <v>275</v>
+      </c>
+      <c r="R260">
+        <v>510959</v>
+      </c>
+      <c r="S260">
+        <v>911.58185696601799</v>
+      </c>
       <c r="T260" s="1"/>
-      <c r="U260" s="1"/>
-      <c r="V260" s="1"/>
+      <c r="U260" s="10">
+        <f t="shared" si="66"/>
+        <v>-205</v>
+      </c>
+      <c r="V260" s="17">
+        <f t="shared" si="67"/>
+        <v>-4.0104545703531546E-4</v>
+      </c>
       <c r="W260" s="1"/>
-      <c r="X260" s="1"/>
-      <c r="Y260" s="1"/>
+      <c r="X260" s="10">
+        <f t="shared" si="69"/>
+        <v>1.588756084442025</v>
+      </c>
+      <c r="Y260" s="17">
+        <f t="shared" si="68"/>
+        <v>1.7458990435233876E-3</v>
+      </c>
       <c r="Z260" s="1"/>
       <c r="AA260" s="1"/>
       <c r="AB260" s="1"/>
@@ -28760,15 +27791,33 @@
       <c r="N261" s="1"/>
       <c r="O261" s="1"/>
       <c r="P261" s="1"/>
-      <c r="Q261" s="1"/>
-      <c r="R261" s="1"/>
-      <c r="S261" s="1"/>
+      <c r="Q261" t="s">
+        <v>276</v>
+      </c>
+      <c r="R261">
+        <v>511169</v>
+      </c>
+      <c r="S261">
+        <v>911.33941793441704</v>
+      </c>
       <c r="T261" s="1"/>
-      <c r="U261" s="1"/>
-      <c r="V261" s="1"/>
+      <c r="U261" s="10">
+        <f t="shared" si="66"/>
+        <v>-164</v>
+      </c>
+      <c r="V261" s="17">
+        <f t="shared" si="67"/>
+        <v>-3.2073032642133405E-4</v>
+      </c>
       <c r="W261" s="1"/>
-      <c r="X261" s="1"/>
-      <c r="Y261" s="1"/>
+      <c r="X261" s="10">
+        <f t="shared" si="69"/>
+        <v>1.391248941421054</v>
+      </c>
+      <c r="Y261" s="17">
+        <f t="shared" si="68"/>
+        <v>1.5289320741869229E-3</v>
+      </c>
       <c r="Z261" s="1"/>
       <c r="AA261" s="1"/>
       <c r="AB261" s="1"/>
@@ -28806,15 +27855,33 @@
       <c r="N262" s="1"/>
       <c r="O262" s="1"/>
       <c r="P262" s="1"/>
-      <c r="Q262" s="1"/>
-      <c r="R262" s="1"/>
-      <c r="S262" s="1"/>
+      <c r="Q262" t="s">
+        <v>277</v>
+      </c>
+      <c r="R262">
+        <v>511769</v>
+      </c>
+      <c r="S262">
+        <v>911.565459012985</v>
+      </c>
       <c r="T262" s="1"/>
-      <c r="U262" s="1"/>
-      <c r="V262" s="1"/>
+      <c r="U262" s="10">
+        <f t="shared" si="66"/>
+        <v>110</v>
+      </c>
+      <c r="V262" s="17">
+        <f t="shared" si="67"/>
+        <v>2.1498693465765286E-4</v>
+      </c>
       <c r="W262" s="1"/>
-      <c r="X262" s="1"/>
-      <c r="Y262" s="1"/>
+      <c r="X262" s="10">
+        <f t="shared" si="69"/>
+        <v>1.6225249767310288</v>
+      </c>
+      <c r="Y262" s="17">
+        <f t="shared" si="68"/>
+        <v>1.7831062982531871E-3</v>
+      </c>
       <c r="Z262" s="1"/>
       <c r="AA262" s="1"/>
       <c r="AB262" s="1"/>
@@ -28852,15 +27919,33 @@
       <c r="N263" s="1"/>
       <c r="O263" s="1"/>
       <c r="P263" s="1"/>
-      <c r="Q263" s="1"/>
-      <c r="R263" s="1"/>
-      <c r="S263" s="1"/>
+      <c r="Q263" t="s">
+        <v>278</v>
+      </c>
+      <c r="R263">
+        <v>539108</v>
+      </c>
+      <c r="S263">
+        <v>911.63480806350697</v>
+      </c>
       <c r="T263" s="1"/>
-      <c r="U263" s="1"/>
-      <c r="V263" s="1"/>
+      <c r="U263" s="10">
+        <f t="shared" si="66"/>
+        <v>-5882</v>
+      </c>
+      <c r="V263" s="17">
+        <f t="shared" si="67"/>
+        <v>-1.0792858584561185E-2</v>
+      </c>
       <c r="W263" s="1"/>
-      <c r="X263" s="1"/>
-      <c r="Y263" s="1"/>
+      <c r="X263" s="10">
+        <f t="shared" si="69"/>
+        <v>1.7208642959599274</v>
+      </c>
+      <c r="Y263" s="17">
+        <f t="shared" si="68"/>
+        <v>1.8912385151881477E-3</v>
+      </c>
       <c r="Z263" s="1"/>
       <c r="AA263" s="1"/>
       <c r="AB263" s="1"/>
@@ -28898,15 +27983,33 @@
       <c r="N264" s="1"/>
       <c r="O264" s="1"/>
       <c r="P264" s="1"/>
-      <c r="Q264" s="1"/>
-      <c r="R264" s="1"/>
-      <c r="S264" s="1"/>
+      <c r="Q264" t="s">
+        <v>279</v>
+      </c>
+      <c r="R264">
+        <v>538454</v>
+      </c>
+      <c r="S264">
+        <v>911.56484103202797</v>
+      </c>
       <c r="T264" s="1"/>
-      <c r="U264" s="1"/>
-      <c r="V264" s="1"/>
+      <c r="U264" s="10">
+        <f t="shared" si="66"/>
+        <v>-5379</v>
+      </c>
+      <c r="V264" s="17">
+        <f t="shared" si="67"/>
+        <v>-9.8909040091351569E-3</v>
+      </c>
       <c r="W264" s="1"/>
-      <c r="X264" s="1"/>
-      <c r="Y264" s="1"/>
+      <c r="X264" s="10">
+        <f t="shared" si="69"/>
+        <v>1.6945879459379967</v>
+      </c>
+      <c r="Y264" s="17">
+        <f t="shared" si="68"/>
+        <v>1.8624501022978914E-3</v>
+      </c>
       <c r="Z264" s="1"/>
       <c r="AA264" s="1"/>
       <c r="AB264" s="1"/>
@@ -28944,9 +28047,6 @@
       <c r="N265" s="1"/>
       <c r="O265" s="1"/>
       <c r="P265" s="1"/>
-      <c r="Q265" s="1"/>
-      <c r="R265" s="1"/>
-      <c r="S265" s="1"/>
       <c r="T265" s="1"/>
       <c r="U265" s="1"/>
       <c r="V265" s="1"/>
@@ -29036,15 +28136,28 @@
       <c r="N267" s="1"/>
       <c r="O267" s="1"/>
       <c r="P267" s="1"/>
-      <c r="Q267" s="1"/>
-      <c r="R267" s="1"/>
-      <c r="S267" s="1"/>
+      <c r="Q267" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="R267" s="23"/>
+      <c r="S267" s="7">
+        <f>SUM(S3:S242)</f>
+        <v>999.63952136039632</v>
+      </c>
       <c r="T267" s="1"/>
       <c r="U267" s="1"/>
-      <c r="V267" s="1"/>
-      <c r="W267" s="1"/>
-      <c r="X267" s="1"/>
-      <c r="Y267" s="1"/>
+      <c r="V267" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="W267" s="23"/>
+      <c r="X267" s="7">
+        <f>S267-C335</f>
+        <v>-10758.029428244399</v>
+      </c>
+      <c r="Y267" s="25">
+        <f>X267/C335</f>
+        <v>-0.91497978675492508</v>
+      </c>
       <c r="Z267" s="1"/>
       <c r="AA267" s="1"/>
       <c r="AB267" s="1"/>
@@ -29082,15 +28195,25 @@
       <c r="N268" s="1"/>
       <c r="O268" s="1"/>
       <c r="P268" s="1"/>
-      <c r="Q268" s="1"/>
-      <c r="R268" s="1"/>
-      <c r="S268" s="1"/>
+      <c r="Q268" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="R268" s="23"/>
+      <c r="S268" s="7">
+        <f>S267/60</f>
+        <v>16.66065868933994</v>
+      </c>
       <c r="T268" s="1"/>
       <c r="U268" s="1"/>
-      <c r="V268" s="1"/>
-      <c r="W268" s="1"/>
-      <c r="X268" s="1"/>
-      <c r="Y268" s="1"/>
+      <c r="V268" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="W268" s="23"/>
+      <c r="X268" s="7">
+        <f>S268-C336</f>
+        <v>-179.30049047073999</v>
+      </c>
+      <c r="Y268" s="26"/>
       <c r="Z268" s="1"/>
       <c r="AA268" s="1"/>
       <c r="AB268" s="1"/>
@@ -57670,200 +56793,266 @@
       <c r="B1007" s="1"/>
       <c r="C1007" s="1"/>
       <c r="D1007" s="1"/>
+      <c r="Q1007" s="1"/>
+      <c r="R1007" s="1"/>
+      <c r="S1007" s="1"/>
     </row>
     <row r="1008" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1008" s="1"/>
       <c r="B1008" s="1"/>
       <c r="C1008" s="1"/>
       <c r="D1008" s="1"/>
-    </row>
-    <row r="1009" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1008" s="1"/>
+      <c r="R1008" s="1"/>
+      <c r="S1008" s="1"/>
+    </row>
+    <row r="1009" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1009" s="1"/>
       <c r="B1009" s="1"/>
       <c r="C1009" s="1"/>
       <c r="D1009" s="1"/>
-    </row>
-    <row r="1010" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1009" s="1"/>
+      <c r="R1009" s="1"/>
+      <c r="S1009" s="1"/>
+    </row>
+    <row r="1010" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1010" s="1"/>
       <c r="B1010" s="1"/>
       <c r="C1010" s="1"/>
       <c r="D1010" s="1"/>
-    </row>
-    <row r="1011" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1010" s="1"/>
+      <c r="R1010" s="1"/>
+      <c r="S1010" s="1"/>
+    </row>
+    <row r="1011" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1011" s="1"/>
       <c r="B1011" s="1"/>
       <c r="C1011" s="1"/>
       <c r="D1011" s="1"/>
-    </row>
-    <row r="1012" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1011" s="1"/>
+      <c r="R1011" s="1"/>
+      <c r="S1011" s="1"/>
+    </row>
+    <row r="1012" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1012" s="1"/>
       <c r="B1012" s="1"/>
       <c r="C1012" s="1"/>
       <c r="D1012" s="1"/>
-    </row>
-    <row r="1013" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1012" s="1"/>
+      <c r="R1012" s="1"/>
+      <c r="S1012" s="1"/>
+    </row>
+    <row r="1013" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1013" s="1"/>
       <c r="B1013" s="1"/>
       <c r="C1013" s="1"/>
       <c r="D1013" s="1"/>
-    </row>
-    <row r="1014" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1013" s="1"/>
+      <c r="R1013" s="1"/>
+      <c r="S1013" s="1"/>
+    </row>
+    <row r="1014" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1014" s="1"/>
       <c r="B1014" s="1"/>
       <c r="C1014" s="1"/>
       <c r="D1014" s="1"/>
-    </row>
-    <row r="1015" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1014" s="1"/>
+      <c r="R1014" s="1"/>
+      <c r="S1014" s="1"/>
+    </row>
+    <row r="1015" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1015" s="1"/>
       <c r="B1015" s="1"/>
       <c r="C1015" s="1"/>
       <c r="D1015" s="1"/>
-    </row>
-    <row r="1016" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1015" s="1"/>
+      <c r="R1015" s="1"/>
+      <c r="S1015" s="1"/>
+    </row>
+    <row r="1016" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1016" s="1"/>
       <c r="B1016" s="1"/>
       <c r="C1016" s="1"/>
       <c r="D1016" s="1"/>
-    </row>
-    <row r="1017" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1016" s="1"/>
+      <c r="R1016" s="1"/>
+      <c r="S1016" s="1"/>
+    </row>
+    <row r="1017" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1017" s="1"/>
       <c r="B1017" s="1"/>
       <c r="C1017" s="1"/>
       <c r="D1017" s="1"/>
-    </row>
-    <row r="1018" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1017" s="1"/>
+      <c r="R1017" s="1"/>
+      <c r="S1017" s="1"/>
+    </row>
+    <row r="1018" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1018" s="1"/>
       <c r="B1018" s="1"/>
       <c r="C1018" s="1"/>
       <c r="D1018" s="1"/>
-    </row>
-    <row r="1019" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1018" s="1"/>
+      <c r="R1018" s="1"/>
+      <c r="S1018" s="1"/>
+    </row>
+    <row r="1019" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1019" s="1"/>
       <c r="B1019" s="1"/>
       <c r="C1019" s="1"/>
       <c r="D1019" s="1"/>
-    </row>
-    <row r="1020" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1019" s="1"/>
+      <c r="R1019" s="1"/>
+      <c r="S1019" s="1"/>
+    </row>
+    <row r="1020" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1020" s="1"/>
       <c r="B1020" s="1"/>
       <c r="C1020" s="1"/>
       <c r="D1020" s="1"/>
-    </row>
-    <row r="1021" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1020" s="1"/>
+      <c r="R1020" s="1"/>
+      <c r="S1020" s="1"/>
+    </row>
+    <row r="1021" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1021" s="1"/>
       <c r="B1021" s="1"/>
       <c r="C1021" s="1"/>
       <c r="D1021" s="1"/>
-    </row>
-    <row r="1022" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1021" s="1"/>
+      <c r="R1021" s="1"/>
+      <c r="S1021" s="1"/>
+    </row>
+    <row r="1022" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1022" s="1"/>
       <c r="B1022" s="1"/>
       <c r="C1022" s="1"/>
       <c r="D1022" s="1"/>
-    </row>
-    <row r="1023" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1022" s="1"/>
+      <c r="R1022" s="1"/>
+      <c r="S1022" s="1"/>
+    </row>
+    <row r="1023" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1023" s="1"/>
       <c r="B1023" s="1"/>
       <c r="C1023" s="1"/>
       <c r="D1023" s="1"/>
-    </row>
-    <row r="1024" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1023" s="1"/>
+      <c r="R1023" s="1"/>
+      <c r="S1023" s="1"/>
+    </row>
+    <row r="1024" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1024" s="1"/>
       <c r="B1024" s="1"/>
       <c r="C1024" s="1"/>
       <c r="D1024" s="1"/>
-    </row>
-    <row r="1025" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1024" s="1"/>
+      <c r="R1024" s="1"/>
+      <c r="S1024" s="1"/>
+    </row>
+    <row r="1025" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1025" s="1"/>
       <c r="B1025" s="1"/>
       <c r="C1025" s="1"/>
       <c r="D1025" s="1"/>
-    </row>
-    <row r="1026" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1025" s="1"/>
+      <c r="R1025" s="1"/>
+      <c r="S1025" s="1"/>
+    </row>
+    <row r="1026" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1026" s="1"/>
       <c r="B1026" s="1"/>
       <c r="C1026" s="1"/>
       <c r="D1026" s="1"/>
-    </row>
-    <row r="1027" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1026" s="1"/>
+      <c r="R1026" s="1"/>
+      <c r="S1026" s="1"/>
+    </row>
+    <row r="1027" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1027" s="1"/>
       <c r="B1027" s="1"/>
       <c r="C1027" s="1"/>
       <c r="D1027" s="1"/>
-    </row>
-    <row r="1028" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1027" s="1"/>
+      <c r="R1027" s="1"/>
+      <c r="S1027" s="1"/>
+    </row>
+    <row r="1028" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1028" s="1"/>
       <c r="B1028" s="1"/>
       <c r="C1028" s="1"/>
       <c r="D1028" s="1"/>
-    </row>
-    <row r="1029" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1028" s="1"/>
+      <c r="R1028" s="1"/>
+      <c r="S1028" s="1"/>
+    </row>
+    <row r="1029" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1029" s="1"/>
       <c r="B1029" s="1"/>
       <c r="C1029" s="1"/>
       <c r="D1029" s="1"/>
     </row>
-    <row r="1030" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1030" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1030" s="1"/>
       <c r="B1030" s="1"/>
       <c r="C1030" s="1"/>
       <c r="D1030" s="1"/>
     </row>
-    <row r="1031" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1031" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1031" s="1"/>
       <c r="B1031" s="1"/>
       <c r="C1031" s="1"/>
       <c r="D1031" s="1"/>
     </row>
-    <row r="1032" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1032" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1032" s="1"/>
       <c r="B1032" s="1"/>
       <c r="C1032" s="1"/>
       <c r="D1032" s="1"/>
     </row>
-    <row r="1033" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1033" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1033" s="1"/>
       <c r="B1033" s="1"/>
       <c r="C1033" s="1"/>
       <c r="D1033" s="1"/>
     </row>
-    <row r="1034" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1034" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1034" s="1"/>
       <c r="B1034" s="1"/>
       <c r="C1034" s="1"/>
       <c r="D1034" s="1"/>
     </row>
-    <row r="1035" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1035" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1035" s="1"/>
       <c r="B1035" s="1"/>
       <c r="C1035" s="1"/>
       <c r="D1035" s="1"/>
     </row>
-    <row r="1036" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1036" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1036" s="1"/>
       <c r="B1036" s="1"/>
       <c r="C1036" s="1"/>
       <c r="D1036" s="1"/>
     </row>
-    <row r="1037" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1037" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1037" s="1"/>
       <c r="B1037" s="1"/>
       <c r="C1037" s="1"/>
       <c r="D1037" s="1"/>
     </row>
-    <row r="1038" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1038" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1038" s="1"/>
       <c r="B1038" s="1"/>
       <c r="C1038" s="1"/>
       <c r="D1038" s="1"/>
     </row>
-    <row r="1039" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1039" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1039" s="1"/>
       <c r="B1039" s="1"/>
       <c r="C1039" s="1"/>
       <c r="D1039" s="1"/>
     </row>
-    <row r="1040" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1040" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1040" s="1"/>
       <c r="B1040" s="1"/>
       <c r="C1040" s="1"/>
@@ -58207,10 +57396,10 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="V245:W245"/>
-    <mergeCell ref="Y245:Y246"/>
-    <mergeCell ref="Q246:R246"/>
-    <mergeCell ref="V246:W246"/>
+    <mergeCell ref="V267:W267"/>
+    <mergeCell ref="Y267:Y268"/>
+    <mergeCell ref="Q268:R268"/>
+    <mergeCell ref="V268:W268"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A335:B335"/>
     <mergeCell ref="A336:B336"/>
@@ -58226,7 +57415,7 @@
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Q245:R245"/>
+    <mergeCell ref="Q267:R267"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="F245:G245"/>
@@ -58293,7 +57482,7 @@
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y245:Y246">
+  <conditionalFormatting sqref="Y267:Y268">
     <cfRule type="cellIs" dxfId="28" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -58301,7 +57490,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y237">
+  <conditionalFormatting sqref="Y3:Y237 Y240 Y243 Y246 Y249 Y252 Y255 Y258 Y261 Y264">
     <cfRule type="cellIs" dxfId="26" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -58309,98 +57498,98 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V237">
-    <cfRule type="cellIs" dxfId="24" priority="32" operator="greaterThan">
+  <conditionalFormatting sqref="V3:V237 V240:V242 V245:V247 V250:V252 V255:V257 V260:V262">
+    <cfRule type="cellIs" dxfId="2" priority="32" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="34" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI238 O238 O240:O242 AI242">
-    <cfRule type="cellIs" dxfId="21" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L238 L240:L242">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y238 Y240:Y242">
-    <cfRule type="cellIs" dxfId="16" priority="21" operator="lessThan">
+  <conditionalFormatting sqref="Y238 Y241 Y244 Y247 Y250 Y253 Y256 Y259 Y262">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="22" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V238 V240:V242">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="greaterThan">
+  <conditionalFormatting sqref="V238 V243 V248 V253 V258 V263">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O239 AI239:AI241">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L239">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y239">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
+  <conditionalFormatting sqref="Y239 Y242 Y245 Y248 Y251 Y254 Y257 Y260 Y263">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V239">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="V239 V244 V249 V254 V259 V264">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D332">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Mais algumas analises do MIP executando
</commit_message>
<xml_diff>
--- a/solutions.xlsx
+++ b/solutions.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solutions1" localSheetId="0">Plan1!$F$2:$I$17</definedName>
-    <definedName name="solutions1_1" localSheetId="0">Plan1!$AA$3:$AC$17</definedName>
-    <definedName name="solutions1_2" localSheetId="0">Plan1!$Q$2:$S$17</definedName>
-    <definedName name="solutions2" localSheetId="0">Plan1!$Z$4:$AC$224</definedName>
-    <definedName name="solutions2_1" localSheetId="0">Plan1!$AA$18:$AC$237</definedName>
+    <definedName name="solutions1" localSheetId="1">Plan1!$F$2:$I$17</definedName>
+    <definedName name="solutions1_1" localSheetId="1">Plan1!$AA$3:$AC$17</definedName>
+    <definedName name="solutions1_2" localSheetId="1">Plan1!$Q$2:$S$17</definedName>
+    <definedName name="solutions2" localSheetId="1">Plan1!$Z$4:$AC$224</definedName>
+    <definedName name="solutions2_1" localSheetId="1">Plan1!$AA$18:$AC$237</definedName>
+    <definedName name="solutions2_2" localSheetId="0">Plan2!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -55,11 +57,21 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="solutions2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Macbook/Documents/GitKraken_Projects/ICAlgoritmos/gurobi/solutions2.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="348">
   <si>
     <t>ILP</t>
   </si>
@@ -1283,28 +1295,98 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -1581,26 +1663,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
@@ -1738,10 +1800,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions2_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -2008,10 +2074,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2">
+        <v>538945</v>
+      </c>
+      <c r="C2">
+        <v>919.36964797973599</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3">
+        <v>539381</v>
+      </c>
+      <c r="C3">
+        <v>911.516117811203</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4">
+        <v>538343</v>
+      </c>
+      <c r="C4">
+        <v>911.35817599296502</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5">
+        <v>626327</v>
+      </c>
+      <c r="C5">
+        <v>911.475837945938</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1096"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L228" zoomScale="111" workbookViewId="0">
-      <selection activeCell="M234" sqref="M234"/>
+    <sheetView tabSelected="1" topLeftCell="L260" zoomScale="111" workbookViewId="0">
+      <selection activeCell="U275" sqref="U275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2040,58 +2197,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="23"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
       <c r="I1" s="23"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="23"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="23"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="28" t="s">
+      <c r="Q1" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
       <c r="T1" s="15"/>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="V1" s="23"/>
       <c r="W1" s="1"/>
-      <c r="X1" s="22" t="s">
+      <c r="X1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="Y1" s="23"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="22" t="s">
+      <c r="AA1" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="AB1" s="27"/>
+      <c r="AB1" s="28"/>
       <c r="AC1" s="23"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="22" t="s">
+      <c r="AE1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="AF1" s="23"/>
       <c r="AG1" s="1"/>
-      <c r="AH1" s="22" t="s">
+      <c r="AH1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="AI1" s="23"/>
@@ -21831,7 +21988,7 @@
         <v>0</v>
       </c>
       <c r="V195" s="17">
-        <f t="shared" ref="V195:V254" si="45">U195/B195</f>
+        <f t="shared" ref="V195:V238" si="45">U195/B195</f>
         <v>0</v>
       </c>
       <c r="W195" s="1"/>
@@ -26712,7 +26869,7 @@
         <v>0</v>
       </c>
       <c r="E245" s="1"/>
-      <c r="F245" s="24" t="s">
+      <c r="F245" s="22" t="s">
         <v>244</v>
       </c>
       <c r="G245" s="23"/>
@@ -26723,7 +26880,7 @@
       <c r="I245" s="1"/>
       <c r="J245" s="1"/>
       <c r="K245" s="1"/>
-      <c r="L245" s="24" t="s">
+      <c r="L245" s="22" t="s">
         <v>245</v>
       </c>
       <c r="M245" s="23"/>
@@ -26731,7 +26888,7 @@
         <f>H245-C335</f>
         <v>-11315.203019142911</v>
       </c>
-      <c r="O245" s="25">
+      <c r="O245" s="24">
         <f>N245/C335</f>
         <v>-0.96236788666542994</v>
       </c>
@@ -26763,7 +26920,7 @@
         <v>7.3130313726978255E-4</v>
       </c>
       <c r="Z245" s="1"/>
-      <c r="AA245" s="24" t="s">
+      <c r="AA245" s="22" t="s">
         <v>244</v>
       </c>
       <c r="AB245" s="23"/>
@@ -26773,7 +26930,7 @@
       </c>
       <c r="AD245" s="1"/>
       <c r="AE245" s="1"/>
-      <c r="AF245" s="24" t="s">
+      <c r="AF245" s="22" t="s">
         <v>245</v>
       </c>
       <c r="AG245" s="23"/>
@@ -26781,7 +26938,7 @@
         <f>AC245-C335</f>
         <v>-5312.7672976047943</v>
       </c>
-      <c r="AI245" s="25">
+      <c r="AI245" s="24">
         <f>AH245/C335</f>
         <v>-0.45185549281716847</v>
       </c>
@@ -26801,7 +26958,7 @@
         <v>0</v>
       </c>
       <c r="E246" s="1"/>
-      <c r="F246" s="24" t="s">
+      <c r="F246" s="22" t="s">
         <v>246</v>
       </c>
       <c r="G246" s="23"/>
@@ -26812,7 +26969,7 @@
       <c r="I246" s="1"/>
       <c r="J246" s="1"/>
       <c r="K246" s="1"/>
-      <c r="L246" s="24" t="s">
+      <c r="L246" s="22" t="s">
         <v>247</v>
       </c>
       <c r="M246" s="23"/>
@@ -26820,7 +26977,7 @@
         <f>H246-C336</f>
         <v>-188.58671698571519</v>
       </c>
-      <c r="O246" s="26"/>
+      <c r="O246" s="25"/>
       <c r="P246" s="1"/>
       <c r="Q246" t="s">
         <v>261</v>
@@ -26849,7 +27006,7 @@
         <v>1.5635693068758426E-3</v>
       </c>
       <c r="Z246" s="1"/>
-      <c r="AA246" s="24" t="s">
+      <c r="AA246" s="22" t="s">
         <v>246</v>
       </c>
       <c r="AB246" s="23"/>
@@ -26859,7 +27016,7 @@
       </c>
       <c r="AD246" s="1"/>
       <c r="AE246" s="1"/>
-      <c r="AF246" s="24" t="s">
+      <c r="AF246" s="22" t="s">
         <v>247</v>
       </c>
       <c r="AG246" s="23"/>
@@ -26867,7 +27024,7 @@
         <f>AC246-C336</f>
         <v>-88.546121626746569</v>
       </c>
-      <c r="AI246" s="26"/>
+      <c r="AI246" s="25"/>
       <c r="AJ246" s="1"/>
     </row>
     <row r="247" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28047,12 +28204,33 @@
       <c r="N265" s="1"/>
       <c r="O265" s="1"/>
       <c r="P265" s="1"/>
+      <c r="Q265" t="s">
+        <v>280</v>
+      </c>
+      <c r="R265">
+        <v>538945</v>
+      </c>
+      <c r="S265">
+        <v>919.36964797973599</v>
+      </c>
       <c r="T265" s="1"/>
-      <c r="U265" s="1"/>
-      <c r="V265" s="1"/>
+      <c r="U265" s="10">
+        <f t="shared" ref="U265:U268" si="71">R265-B265</f>
+        <v>-5232</v>
+      </c>
+      <c r="V265" s="17">
+        <f t="shared" ref="V265:V268" si="72">U265/B265</f>
+        <v>-9.6145188054621942E-3</v>
+      </c>
       <c r="W265" s="1"/>
-      <c r="X265" s="1"/>
-      <c r="Y265" s="1"/>
+      <c r="X265" s="10">
+        <f t="shared" ref="X265:X268" si="73">S265-C265</f>
+        <v>9.2585339546200203</v>
+      </c>
+      <c r="Y265" s="17">
+        <f t="shared" ref="Y265:Y268" si="74">X265/C265</f>
+        <v>1.0172970983369967E-2</v>
+      </c>
       <c r="Z265" s="1"/>
       <c r="AA265" s="1"/>
       <c r="AB265" s="1"/>
@@ -28090,15 +28268,33 @@
       <c r="N266" s="1"/>
       <c r="O266" s="1"/>
       <c r="P266" s="1"/>
-      <c r="Q266" s="1"/>
-      <c r="R266" s="1"/>
-      <c r="S266" s="1"/>
+      <c r="Q266" t="s">
+        <v>281</v>
+      </c>
+      <c r="R266">
+        <v>539381</v>
+      </c>
+      <c r="S266">
+        <v>911.516117811203</v>
+      </c>
       <c r="T266" s="1"/>
-      <c r="U266" s="1"/>
-      <c r="V266" s="1"/>
+      <c r="U266" s="10">
+        <f t="shared" si="71"/>
+        <v>-4636</v>
+      </c>
+      <c r="V266" s="17">
+        <f t="shared" si="72"/>
+        <v>-8.5217925175132391E-3</v>
+      </c>
       <c r="W266" s="1"/>
-      <c r="X266" s="1"/>
-      <c r="Y266" s="1"/>
+      <c r="X266" s="10">
+        <f t="shared" si="73"/>
+        <v>1.6048569679260254</v>
+      </c>
+      <c r="Y266" s="17">
+        <f t="shared" si="74"/>
+        <v>1.7637510788015688E-3</v>
+      </c>
       <c r="Z266" s="1"/>
       <c r="AA266" s="1"/>
       <c r="AB266" s="1"/>
@@ -28136,27 +28332,31 @@
       <c r="N267" s="1"/>
       <c r="O267" s="1"/>
       <c r="P267" s="1"/>
-      <c r="Q267" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="R267" s="23"/>
-      <c r="S267" s="7">
-        <f>SUM(S3:S242)</f>
-        <v>999.63952136039632</v>
+      <c r="Q267" t="s">
+        <v>282</v>
+      </c>
+      <c r="R267">
+        <v>538343</v>
+      </c>
+      <c r="S267">
+        <v>911.35817599296502</v>
       </c>
       <c r="T267" s="1"/>
-      <c r="U267" s="1"/>
-      <c r="V267" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="W267" s="23"/>
-      <c r="X267" s="7">
-        <f>S267-C335</f>
-        <v>-10758.029428244399</v>
-      </c>
-      <c r="Y267" s="25">
-        <f>X267/C335</f>
-        <v>-0.91497978675492508</v>
+      <c r="U267" s="10">
+        <f t="shared" si="71"/>
+        <v>-3968</v>
+      </c>
+      <c r="V267" s="17">
+        <f t="shared" si="72"/>
+        <v>-7.3168348051210466E-3</v>
+      </c>
+      <c r="X267" s="10">
+        <f t="shared" si="73"/>
+        <v>0.65789794921806788</v>
+      </c>
+      <c r="Y267" s="17">
+        <f t="shared" si="74"/>
+        <v>7.2240885951114716E-4</v>
       </c>
       <c r="Z267" s="1"/>
       <c r="AA267" s="1"/>
@@ -28195,25 +28395,32 @@
       <c r="N268" s="1"/>
       <c r="O268" s="1"/>
       <c r="P268" s="1"/>
-      <c r="Q268" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="R268" s="23"/>
-      <c r="S268" s="7">
-        <f>S267/60</f>
-        <v>16.66065868933994</v>
+      <c r="Q268" t="s">
+        <v>283</v>
+      </c>
+      <c r="R268">
+        <v>626327</v>
+      </c>
+      <c r="S268">
+        <v>911.475837945938</v>
       </c>
       <c r="T268" s="1"/>
-      <c r="U268" s="1"/>
-      <c r="V268" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="W268" s="23"/>
-      <c r="X268" s="7">
-        <f>S268-C336</f>
-        <v>-179.30049047073999</v>
-      </c>
-      <c r="Y268" s="26"/>
+      <c r="U268" s="10">
+        <f t="shared" si="71"/>
+        <v>-24915</v>
+      </c>
+      <c r="V268" s="17">
+        <f t="shared" si="72"/>
+        <v>-3.8257667656570064E-2</v>
+      </c>
+      <c r="X268" s="10">
+        <f t="shared" si="73"/>
+        <v>1.6217257976539941</v>
+      </c>
+      <c r="Y268" s="17">
+        <f t="shared" si="74"/>
+        <v>1.7824020092901359E-3</v>
+      </c>
       <c r="Z268" s="1"/>
       <c r="AA268" s="1"/>
       <c r="AB268" s="1"/>
@@ -28251,9 +28458,6 @@
       <c r="N269" s="1"/>
       <c r="O269" s="1"/>
       <c r="P269" s="1"/>
-      <c r="Q269" s="1"/>
-      <c r="R269" s="1"/>
-      <c r="S269" s="1"/>
       <c r="T269" s="1"/>
       <c r="U269" s="1"/>
       <c r="V269" s="1"/>
@@ -28343,15 +28547,28 @@
       <c r="N271" s="1"/>
       <c r="O271" s="1"/>
       <c r="P271" s="1"/>
-      <c r="Q271" s="1"/>
-      <c r="R271" s="1"/>
-      <c r="S271" s="1"/>
+      <c r="Q271" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="R271" s="23"/>
+      <c r="S271" s="7">
+        <f>SUM(S3:S242)</f>
+        <v>999.63952136039632</v>
+      </c>
       <c r="T271" s="1"/>
       <c r="U271" s="1"/>
-      <c r="V271" s="1"/>
-      <c r="W271" s="1"/>
-      <c r="X271" s="1"/>
-      <c r="Y271" s="1"/>
+      <c r="V271" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="W271" s="23"/>
+      <c r="X271" s="7">
+        <f>S271-C335</f>
+        <v>-10758.029428244399</v>
+      </c>
+      <c r="Y271" s="24">
+        <f>X271/C335</f>
+        <v>-0.91497978675492508</v>
+      </c>
       <c r="Z271" s="1"/>
       <c r="AA271" s="1"/>
       <c r="AB271" s="1"/>
@@ -28389,15 +28606,25 @@
       <c r="N272" s="1"/>
       <c r="O272" s="1"/>
       <c r="P272" s="1"/>
-      <c r="Q272" s="1"/>
-      <c r="R272" s="1"/>
-      <c r="S272" s="1"/>
+      <c r="Q272" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="R272" s="23"/>
+      <c r="S272" s="7">
+        <f>S271/60</f>
+        <v>16.66065868933994</v>
+      </c>
       <c r="T272" s="1"/>
       <c r="U272" s="1"/>
-      <c r="V272" s="1"/>
-      <c r="W272" s="1"/>
-      <c r="X272" s="1"/>
-      <c r="Y272" s="1"/>
+      <c r="V272" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="W272" s="23"/>
+      <c r="X272" s="7">
+        <f>S272-C336</f>
+        <v>-179.30049047073999</v>
+      </c>
+      <c r="Y272" s="25"/>
       <c r="Z272" s="1"/>
       <c r="AA272" s="1"/>
       <c r="AB272" s="1"/>
@@ -31243,7 +31470,7 @@
       <c r="AJ334" s="1"/>
     </row>
     <row r="335" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A335" s="24" t="s">
+      <c r="A335" s="22" t="s">
         <v>244</v>
       </c>
       <c r="B335" s="23"/>
@@ -31286,7 +31513,7 @@
       <c r="AJ335" s="1"/>
     </row>
     <row r="336" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="22" t="s">
         <v>246</v>
       </c>
       <c r="B336" s="23"/>
@@ -56991,24 +57218,36 @@
       <c r="B1029" s="1"/>
       <c r="C1029" s="1"/>
       <c r="D1029" s="1"/>
+      <c r="Q1029" s="1"/>
+      <c r="R1029" s="1"/>
+      <c r="S1029" s="1"/>
     </row>
     <row r="1030" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1030" s="1"/>
       <c r="B1030" s="1"/>
       <c r="C1030" s="1"/>
       <c r="D1030" s="1"/>
+      <c r="Q1030" s="1"/>
+      <c r="R1030" s="1"/>
+      <c r="S1030" s="1"/>
     </row>
     <row r="1031" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1031" s="1"/>
       <c r="B1031" s="1"/>
       <c r="C1031" s="1"/>
       <c r="D1031" s="1"/>
+      <c r="Q1031" s="1"/>
+      <c r="R1031" s="1"/>
+      <c r="S1031" s="1"/>
     </row>
     <row r="1032" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1032" s="1"/>
       <c r="B1032" s="1"/>
       <c r="C1032" s="1"/>
       <c r="D1032" s="1"/>
+      <c r="Q1032" s="1"/>
+      <c r="R1032" s="1"/>
+      <c r="S1032" s="1"/>
     </row>
     <row r="1033" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1033" s="1"/>
@@ -57396,11 +57635,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="V267:W267"/>
-    <mergeCell ref="Y267:Y268"/>
-    <mergeCell ref="Q268:R268"/>
-    <mergeCell ref="V268:W268"/>
-    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="F245:G245"/>
+    <mergeCell ref="F246:G246"/>
+    <mergeCell ref="L245:M245"/>
+    <mergeCell ref="O245:O246"/>
+    <mergeCell ref="L246:M246"/>
     <mergeCell ref="A335:B335"/>
     <mergeCell ref="A336:B336"/>
     <mergeCell ref="AI245:AI246"/>
@@ -57415,181 +57655,180 @@
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Q267:R267"/>
+    <mergeCell ref="Q271:R271"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="F245:G245"/>
-    <mergeCell ref="F246:G246"/>
-    <mergeCell ref="L245:M245"/>
-    <mergeCell ref="O245:O246"/>
-    <mergeCell ref="L246:M246"/>
+    <mergeCell ref="V271:W271"/>
+    <mergeCell ref="Y271:Y272"/>
+    <mergeCell ref="Q272:R272"/>
+    <mergeCell ref="V272:W272"/>
+    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="AF3:AF242">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="49" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3:AF242">
-    <cfRule type="cellIs" dxfId="40" priority="50" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="50" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3:AF242">
-    <cfRule type="cellIs" dxfId="39" priority="51" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="51" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3:AF242">
-    <cfRule type="cellIs" dxfId="38" priority="52" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="43" priority="52" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI245:AI246">
-    <cfRule type="cellIs" dxfId="37" priority="44" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="45" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O245:O246">
-    <cfRule type="cellIs" dxfId="35" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="43" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="39" priority="43" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3:AI237 O3:O237">
-    <cfRule type="cellIs" dxfId="33" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="47" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="47" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L237">
-    <cfRule type="cellIs" dxfId="31" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="41" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y267:Y268">
-    <cfRule type="cellIs" dxfId="28" priority="35" operator="lessThan">
+  <conditionalFormatting sqref="Y271:Y272">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="36" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y237 Y240 Y243 Y246 Y249 Y252 Y255 Y258 Y261 Y264">
-    <cfRule type="cellIs" dxfId="26" priority="37" operator="lessThan">
+  <conditionalFormatting sqref="Y3:Y237 Y240 Y243 Y246 Y249 Y252 Y255 Y258 Y261 Y264 Y266 Y268">
+    <cfRule type="cellIs" dxfId="31" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="38" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V237 V240:V242 V245:V247 V250:V252 V255:V257 V260:V262">
-    <cfRule type="cellIs" dxfId="2" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="32" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="34" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI238 O238 O240:O242 AI242">
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L238 L240:L242">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y238 Y241 Y244 Y247 Y250 Y253 Y256 Y259 Y262">
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V238 V243 V248 V253 V258 V263">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
+  <conditionalFormatting sqref="V238 V243 V248 V253 V258 V263 V265 V267">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O239 AI239:AI241">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L239">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y239 Y242 Y245 Y248 Y251 Y254 Y257 Y260 Y263">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
+  <conditionalFormatting sqref="Y239 Y242 Y245 Y248 Y251 Y254 Y257 Y260 Y263 Y265 Y267">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V239 V244 V249 V254 V259 V264">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="V239 V244 V249 V254 V259 V264 V266 V268">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D332">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
As ultimas mudancas antes do meu computador morrer
</commit_message>
<xml_diff>
--- a/solutions.xlsx
+++ b/solutions.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15280" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan2" sheetId="2" r:id="rId1"/>
-    <sheet name="Plan1" sheetId="1" r:id="rId2"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId2"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solutions1" localSheetId="1">Plan1!$F$2:$I$17</definedName>
-    <definedName name="solutions1_1" localSheetId="1">Plan1!$AA$3:$AC$17</definedName>
-    <definedName name="solutions1_2" localSheetId="1">Plan1!$Q$2:$S$17</definedName>
-    <definedName name="solutions2" localSheetId="1">Plan1!$Z$4:$AC$224</definedName>
-    <definedName name="solutions2_1" localSheetId="1">Plan1!$AA$18:$AC$237</definedName>
+    <definedName name="solutions1" localSheetId="2">Plan1!$F$2:$I$17</definedName>
+    <definedName name="solutions1_1" localSheetId="2">Plan1!$AA$3:$AC$17</definedName>
+    <definedName name="solutions1_2" localSheetId="2">Plan1!$Q$2:$S$17</definedName>
+    <definedName name="solutions2" localSheetId="2">Plan1!$Z$4:$AC$224</definedName>
+    <definedName name="solutions2_1" localSheetId="2">Plan1!$AA$18:$AC$237</definedName>
     <definedName name="solutions2_2" localSheetId="0">Plan2!$A$1:$D$5</definedName>
+    <definedName name="solutions2_2" localSheetId="1">Plan3!$A$1:$D$20</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -58,6 +60,16 @@
     </textPr>
   </connection>
   <connection id="3" name="solutions2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/Macbook/Documents/GitKraken_Projects/ICAlgoritmos/gurobi/solutions2.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="solutions21" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Macbook/Documents/GitKraken_Projects/ICAlgoritmos/gurobi/solutions2.csv" comma="1">
       <textFields count="4">
         <textField/>
@@ -71,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="348">
   <si>
     <t>ILP</t>
   </si>
@@ -1295,23 +1307,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1804,11 +1816,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions2_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2165,10 +2181,311 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2">
+        <v>630039</v>
+      </c>
+      <c r="C2">
+        <v>911.932229042053</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3">
+        <v>627238</v>
+      </c>
+      <c r="C3">
+        <v>909.90097618103005</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4">
+        <v>630916</v>
+      </c>
+      <c r="C4">
+        <v>911.35412311553898</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5">
+        <v>629955</v>
+      </c>
+      <c r="C5">
+        <v>911.42725610732998</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B6">
+        <v>763842</v>
+      </c>
+      <c r="C6">
+        <v>925.18332099914505</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7">
+        <v>764165</v>
+      </c>
+      <c r="C7">
+        <v>925.12877488136201</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B8">
+        <v>763947</v>
+      </c>
+      <c r="C8">
+        <v>925.04690480232205</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9">
+        <v>764411</v>
+      </c>
+      <c r="C9">
+        <v>929.17364501953102</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10">
+        <v>764879</v>
+      </c>
+      <c r="C10">
+        <v>928.37262701988197</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B11">
+        <v>804158</v>
+      </c>
+      <c r="C11">
+        <v>925.19710779189995</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B12">
+        <v>803996</v>
+      </c>
+      <c r="C12">
+        <v>925.31088614463795</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B13">
+        <v>804650</v>
+      </c>
+      <c r="C13">
+        <v>925.21861290931702</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>296</v>
+      </c>
+      <c r="B14">
+        <v>798589</v>
+      </c>
+      <c r="C14">
+        <v>921.92955207824696</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>297</v>
+      </c>
+      <c r="B15">
+        <v>798211</v>
+      </c>
+      <c r="C15">
+        <v>921.955177307128</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>298</v>
+      </c>
+      <c r="B16">
+        <v>6297987</v>
+      </c>
+      <c r="C16">
+        <v>922.27863478660504</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>299</v>
+      </c>
+      <c r="B17">
+        <v>6202140</v>
+      </c>
+      <c r="C17">
+        <v>922.37359929084698</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>300</v>
+      </c>
+      <c r="B18">
+        <v>6483078</v>
+      </c>
+      <c r="C18">
+        <v>922.18164396285999</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B19">
+        <v>6588382</v>
+      </c>
+      <c r="C19">
+        <v>921.96937108039799</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>302</v>
+      </c>
+      <c r="B20">
+        <v>6337262</v>
+      </c>
+      <c r="C20">
+        <v>922.50565624237004</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1096"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L260" zoomScale="111" workbookViewId="0">
-      <selection activeCell="U275" sqref="U275"/>
+    <sheetView tabSelected="1" topLeftCell="O270" zoomScale="112" workbookViewId="0">
+      <selection activeCell="W284" sqref="W284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2197,58 +2514,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="23"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="23"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="23"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="22" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="23"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
       <c r="T1" s="15"/>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="V1" s="23"/>
       <c r="W1" s="1"/>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="22" t="s">
         <v>2</v>
       </c>
       <c r="Y1" s="23"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="AB1" s="28"/>
+      <c r="AB1" s="27"/>
       <c r="AC1" s="23"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="27" t="s">
+      <c r="AE1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="AF1" s="23"/>
       <c r="AG1" s="1"/>
-      <c r="AH1" s="27" t="s">
+      <c r="AH1" s="22" t="s">
         <v>2</v>
       </c>
       <c r="AI1" s="23"/>
@@ -26869,7 +27186,7 @@
         <v>0</v>
       </c>
       <c r="E245" s="1"/>
-      <c r="F245" s="22" t="s">
+      <c r="F245" s="24" t="s">
         <v>244</v>
       </c>
       <c r="G245" s="23"/>
@@ -26880,7 +27197,7 @@
       <c r="I245" s="1"/>
       <c r="J245" s="1"/>
       <c r="K245" s="1"/>
-      <c r="L245" s="22" t="s">
+      <c r="L245" s="24" t="s">
         <v>245</v>
       </c>
       <c r="M245" s="23"/>
@@ -26888,7 +27205,7 @@
         <f>H245-C335</f>
         <v>-11315.203019142911</v>
       </c>
-      <c r="O245" s="24">
+      <c r="O245" s="25">
         <f>N245/C335</f>
         <v>-0.96236788666542994</v>
       </c>
@@ -26920,7 +27237,7 @@
         <v>7.3130313726978255E-4</v>
       </c>
       <c r="Z245" s="1"/>
-      <c r="AA245" s="22" t="s">
+      <c r="AA245" s="24" t="s">
         <v>244</v>
       </c>
       <c r="AB245" s="23"/>
@@ -26930,7 +27247,7 @@
       </c>
       <c r="AD245" s="1"/>
       <c r="AE245" s="1"/>
-      <c r="AF245" s="22" t="s">
+      <c r="AF245" s="24" t="s">
         <v>245</v>
       </c>
       <c r="AG245" s="23"/>
@@ -26938,7 +27255,7 @@
         <f>AC245-C335</f>
         <v>-5312.7672976047943</v>
       </c>
-      <c r="AI245" s="24">
+      <c r="AI245" s="25">
         <f>AH245/C335</f>
         <v>-0.45185549281716847</v>
       </c>
@@ -26958,7 +27275,7 @@
         <v>0</v>
       </c>
       <c r="E246" s="1"/>
-      <c r="F246" s="22" t="s">
+      <c r="F246" s="24" t="s">
         <v>246</v>
       </c>
       <c r="G246" s="23"/>
@@ -26969,7 +27286,7 @@
       <c r="I246" s="1"/>
       <c r="J246" s="1"/>
       <c r="K246" s="1"/>
-      <c r="L246" s="22" t="s">
+      <c r="L246" s="24" t="s">
         <v>247</v>
       </c>
       <c r="M246" s="23"/>
@@ -26977,7 +27294,7 @@
         <f>H246-C336</f>
         <v>-188.58671698571519</v>
       </c>
-      <c r="O246" s="25"/>
+      <c r="O246" s="26"/>
       <c r="P246" s="1"/>
       <c r="Q246" t="s">
         <v>261</v>
@@ -27006,7 +27323,7 @@
         <v>1.5635693068758426E-3</v>
       </c>
       <c r="Z246" s="1"/>
-      <c r="AA246" s="22" t="s">
+      <c r="AA246" s="24" t="s">
         <v>246</v>
       </c>
       <c r="AB246" s="23"/>
@@ -27016,7 +27333,7 @@
       </c>
       <c r="AD246" s="1"/>
       <c r="AE246" s="1"/>
-      <c r="AF246" s="22" t="s">
+      <c r="AF246" s="24" t="s">
         <v>247</v>
       </c>
       <c r="AG246" s="23"/>
@@ -27024,7 +27341,7 @@
         <f>AC246-C336</f>
         <v>-88.546121626746569</v>
       </c>
-      <c r="AI246" s="25"/>
+      <c r="AI246" s="26"/>
       <c r="AJ246" s="1"/>
     </row>
     <row r="247" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -28458,12 +28775,33 @@
       <c r="N269" s="1"/>
       <c r="O269" s="1"/>
       <c r="P269" s="1"/>
+      <c r="Q269" t="s">
+        <v>284</v>
+      </c>
+      <c r="R269">
+        <v>630039</v>
+      </c>
+      <c r="S269">
+        <v>911.932229042053</v>
+      </c>
       <c r="T269" s="1"/>
-      <c r="U269" s="1"/>
-      <c r="V269" s="1"/>
+      <c r="U269" s="10">
+        <f t="shared" ref="U269:U287" si="75">R269-B269</f>
+        <v>-20639</v>
+      </c>
+      <c r="V269" s="17">
+        <f t="shared" ref="V269:V287" si="76">U269/B269</f>
+        <v>-3.1719222103713356E-2</v>
+      </c>
       <c r="W269" s="1"/>
-      <c r="X269" s="1"/>
-      <c r="Y269" s="1"/>
+      <c r="X269" s="10">
+        <f t="shared" ref="X269:X287" si="77">S269-C269</f>
+        <v>2.0382719039920403</v>
+      </c>
+      <c r="Y269" s="17">
+        <f t="shared" ref="Y269:Y287" si="78">X269/C269</f>
+        <v>2.2401202777553638E-3</v>
+      </c>
       <c r="Z269" s="1"/>
       <c r="AA269" s="1"/>
       <c r="AB269" s="1"/>
@@ -28501,15 +28839,33 @@
       <c r="N270" s="1"/>
       <c r="O270" s="1"/>
       <c r="P270" s="1"/>
-      <c r="Q270" s="1"/>
-      <c r="R270" s="1"/>
-      <c r="S270" s="1"/>
+      <c r="Q270" t="s">
+        <v>285</v>
+      </c>
+      <c r="R270">
+        <v>627238</v>
+      </c>
+      <c r="S270">
+        <v>909.90097618103005</v>
+      </c>
       <c r="T270" s="1"/>
-      <c r="U270" s="1"/>
-      <c r="V270" s="1"/>
+      <c r="U270" s="10">
+        <f t="shared" si="75"/>
+        <v>-8683</v>
+      </c>
+      <c r="V270" s="17">
+        <f t="shared" si="76"/>
+        <v>-1.365421176529789E-2</v>
+      </c>
       <c r="W270" s="1"/>
-      <c r="X270" s="1"/>
-      <c r="Y270" s="1"/>
+      <c r="X270" s="10">
+        <f t="shared" si="77"/>
+        <v>-7.3465168476099052</v>
+      </c>
+      <c r="Y270" s="17">
+        <f t="shared" si="78"/>
+        <v>-8.0093070882675272E-3</v>
+      </c>
       <c r="Z270" s="1"/>
       <c r="AA270" s="1"/>
       <c r="AB270" s="1"/>
@@ -28547,27 +28903,31 @@
       <c r="N271" s="1"/>
       <c r="O271" s="1"/>
       <c r="P271" s="1"/>
-      <c r="Q271" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="R271" s="23"/>
-      <c r="S271" s="7">
-        <f>SUM(S3:S242)</f>
-        <v>999.63952136039632</v>
+      <c r="Q271" t="s">
+        <v>286</v>
+      </c>
+      <c r="R271">
+        <v>630916</v>
+      </c>
+      <c r="S271">
+        <v>911.35412311553898</v>
       </c>
       <c r="T271" s="1"/>
-      <c r="U271" s="1"/>
-      <c r="V271" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="W271" s="23"/>
-      <c r="X271" s="7">
-        <f>S271-C335</f>
-        <v>-10758.029428244399</v>
-      </c>
-      <c r="Y271" s="24">
-        <f>X271/C335</f>
-        <v>-0.91497978675492508</v>
+      <c r="U271" s="10">
+        <f t="shared" si="75"/>
+        <v>-22193</v>
+      </c>
+      <c r="V271" s="17">
+        <f t="shared" si="76"/>
+        <v>-3.3980545360728455E-2</v>
+      </c>
+      <c r="X271" s="10">
+        <f t="shared" si="77"/>
+        <v>-3.0459499359129723</v>
+      </c>
+      <c r="Y271" s="17">
+        <f t="shared" si="78"/>
+        <v>-3.3310910898643169E-3</v>
       </c>
       <c r="Z271" s="1"/>
       <c r="AA271" s="1"/>
@@ -28606,25 +28966,32 @@
       <c r="N272" s="1"/>
       <c r="O272" s="1"/>
       <c r="P272" s="1"/>
-      <c r="Q272" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="R272" s="23"/>
-      <c r="S272" s="7">
-        <f>S271/60</f>
-        <v>16.66065868933994</v>
+      <c r="Q272" t="s">
+        <v>287</v>
+      </c>
+      <c r="R272">
+        <v>629955</v>
+      </c>
+      <c r="S272">
+        <v>911.42725610732998</v>
       </c>
       <c r="T272" s="1"/>
-      <c r="U272" s="1"/>
-      <c r="V272" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="W272" s="23"/>
-      <c r="X272" s="7">
-        <f>S272-C336</f>
-        <v>-179.30049047073999</v>
-      </c>
-      <c r="Y272" s="25"/>
+      <c r="U272" s="10">
+        <f t="shared" si="75"/>
+        <v>-26130</v>
+      </c>
+      <c r="V272" s="17">
+        <f t="shared" si="76"/>
+        <v>-3.982715654221633E-2</v>
+      </c>
+      <c r="X272" s="10">
+        <f t="shared" si="77"/>
+        <v>1.5826911926269531</v>
+      </c>
+      <c r="Y272" s="17">
+        <f t="shared" si="78"/>
+        <v>1.7395182140537695E-3</v>
+      </c>
       <c r="Z272" s="1"/>
       <c r="AA272" s="1"/>
       <c r="AB272" s="1"/>
@@ -28662,15 +29029,33 @@
       <c r="N273" s="1"/>
       <c r="O273" s="1"/>
       <c r="P273" s="1"/>
-      <c r="Q273" s="1"/>
-      <c r="R273" s="1"/>
-      <c r="S273" s="1"/>
+      <c r="Q273" t="s">
+        <v>288</v>
+      </c>
+      <c r="R273">
+        <v>763842</v>
+      </c>
+      <c r="S273">
+        <v>925.18332099914505</v>
+      </c>
       <c r="T273" s="1"/>
-      <c r="U273" s="1"/>
-      <c r="V273" s="1"/>
+      <c r="U273" s="10">
+        <f t="shared" si="75"/>
+        <v>-655</v>
+      </c>
+      <c r="V273" s="17">
+        <f t="shared" si="76"/>
+        <v>-8.5677249223999573E-4</v>
+      </c>
       <c r="W273" s="1"/>
-      <c r="X273" s="1"/>
-      <c r="Y273" s="1"/>
+      <c r="X273" s="10">
+        <f t="shared" si="77"/>
+        <v>2.7017309665681069</v>
+      </c>
+      <c r="Y273" s="17">
+        <f t="shared" si="78"/>
+        <v>2.9287641030025287E-3</v>
+      </c>
       <c r="Z273" s="1"/>
       <c r="AA273" s="1"/>
       <c r="AB273" s="1"/>
@@ -28708,15 +29093,33 @@
       <c r="N274" s="1"/>
       <c r="O274" s="1"/>
       <c r="P274" s="1"/>
-      <c r="Q274" s="1"/>
-      <c r="R274" s="1"/>
-      <c r="S274" s="1"/>
+      <c r="Q274" t="s">
+        <v>289</v>
+      </c>
+      <c r="R274">
+        <v>764165</v>
+      </c>
+      <c r="S274">
+        <v>925.12877488136201</v>
+      </c>
       <c r="T274" s="1"/>
-      <c r="U274" s="1"/>
-      <c r="V274" s="1"/>
+      <c r="U274" s="10">
+        <f t="shared" si="75"/>
+        <v>-228</v>
+      </c>
+      <c r="V274" s="17">
+        <f t="shared" si="76"/>
+        <v>-2.982758868801781E-4</v>
+      </c>
       <c r="W274" s="1"/>
-      <c r="X274" s="1"/>
-      <c r="Y274" s="1"/>
+      <c r="X274" s="10">
+        <f t="shared" si="77"/>
+        <v>1.428759574890023</v>
+      </c>
+      <c r="Y274" s="17">
+        <f t="shared" si="78"/>
+        <v>1.5467787714780741E-3</v>
+      </c>
       <c r="Z274" s="1"/>
       <c r="AA274" s="1"/>
       <c r="AB274" s="1"/>
@@ -28754,15 +29157,33 @@
       <c r="N275" s="1"/>
       <c r="O275" s="1"/>
       <c r="P275" s="1"/>
-      <c r="Q275" s="1"/>
-      <c r="R275" s="1"/>
-      <c r="S275" s="1"/>
+      <c r="Q275" t="s">
+        <v>290</v>
+      </c>
+      <c r="R275">
+        <v>763947</v>
+      </c>
+      <c r="S275">
+        <v>925.04690480232205</v>
+      </c>
       <c r="T275" s="1"/>
-      <c r="U275" s="1"/>
-      <c r="V275" s="1"/>
+      <c r="U275" s="10">
+        <f t="shared" si="75"/>
+        <v>-736</v>
+      </c>
+      <c r="V275" s="17">
+        <f t="shared" si="76"/>
+        <v>-9.6249033913399409E-4</v>
+      </c>
       <c r="W275" s="1"/>
-      <c r="X275" s="1"/>
-      <c r="Y275" s="1"/>
+      <c r="X275" s="10">
+        <f t="shared" si="77"/>
+        <v>2.5548586845400223</v>
+      </c>
+      <c r="Y275" s="17">
+        <f t="shared" si="78"/>
+        <v>2.7695183880358603E-3</v>
+      </c>
       <c r="Z275" s="1"/>
       <c r="AA275" s="1"/>
       <c r="AB275" s="1"/>
@@ -28800,15 +29221,33 @@
       <c r="N276" s="1"/>
       <c r="O276" s="1"/>
       <c r="P276" s="1"/>
-      <c r="Q276" s="1"/>
-      <c r="R276" s="1"/>
-      <c r="S276" s="1"/>
+      <c r="Q276" t="s">
+        <v>291</v>
+      </c>
+      <c r="R276">
+        <v>764411</v>
+      </c>
+      <c r="S276">
+        <v>929.17364501953102</v>
+      </c>
       <c r="T276" s="1"/>
-      <c r="U276" s="1"/>
-      <c r="V276" s="1"/>
+      <c r="U276" s="10">
+        <f t="shared" si="75"/>
+        <v>-592</v>
+      </c>
+      <c r="V276" s="17">
+        <f t="shared" si="76"/>
+        <v>-7.7385317443199567E-4</v>
+      </c>
       <c r="W276" s="1"/>
-      <c r="X276" s="1"/>
-      <c r="Y276" s="1"/>
+      <c r="X276" s="10">
+        <f t="shared" si="77"/>
+        <v>-38.157422065734977</v>
+      </c>
+      <c r="Y276" s="17">
+        <f t="shared" si="78"/>
+        <v>-3.9446083522066355E-2</v>
+      </c>
       <c r="Z276" s="1"/>
       <c r="AA276" s="1"/>
       <c r="AB276" s="1"/>
@@ -28846,15 +29285,33 @@
       <c r="N277" s="1"/>
       <c r="O277" s="1"/>
       <c r="P277" s="1"/>
-      <c r="Q277" s="1"/>
-      <c r="R277" s="1"/>
-      <c r="S277" s="1"/>
+      <c r="Q277" t="s">
+        <v>292</v>
+      </c>
+      <c r="R277">
+        <v>764879</v>
+      </c>
+      <c r="S277">
+        <v>928.37262701988197</v>
+      </c>
       <c r="T277" s="1"/>
-      <c r="U277" s="1"/>
-      <c r="V277" s="1"/>
+      <c r="U277" s="10">
+        <f t="shared" si="75"/>
+        <v>40</v>
+      </c>
+      <c r="V277" s="17">
+        <f t="shared" si="76"/>
+        <v>5.2298588330354493E-5</v>
+      </c>
       <c r="W277" s="1"/>
-      <c r="X277" s="1"/>
-      <c r="Y277" s="1"/>
+      <c r="X277" s="10">
+        <f t="shared" si="77"/>
+        <v>6.0152318477629478</v>
+      </c>
+      <c r="Y277" s="17">
+        <f t="shared" si="78"/>
+        <v>6.5215846690755471E-3</v>
+      </c>
       <c r="Z277" s="1"/>
       <c r="AA277" s="1"/>
       <c r="AB277" s="1"/>
@@ -28892,15 +29349,33 @@
       <c r="N278" s="1"/>
       <c r="O278" s="1"/>
       <c r="P278" s="1"/>
-      <c r="Q278" s="1"/>
-      <c r="R278" s="1"/>
-      <c r="S278" s="1"/>
+      <c r="Q278" t="s">
+        <v>293</v>
+      </c>
+      <c r="R278">
+        <v>804158</v>
+      </c>
+      <c r="S278">
+        <v>925.19710779189995</v>
+      </c>
       <c r="T278" s="1"/>
-      <c r="U278" s="1"/>
-      <c r="V278" s="1"/>
+      <c r="U278" s="10">
+        <f t="shared" si="75"/>
+        <v>-175</v>
+      </c>
+      <c r="V278" s="17">
+        <f t="shared" si="76"/>
+        <v>-2.1757157794097717E-4</v>
+      </c>
       <c r="W278" s="1"/>
-      <c r="X278" s="1"/>
-      <c r="Y278" s="1"/>
+      <c r="X278" s="10">
+        <f t="shared" si="77"/>
+        <v>2.631545782089006</v>
+      </c>
+      <c r="Y278" s="17">
+        <f t="shared" si="78"/>
+        <v>2.8524214326363737E-3</v>
+      </c>
       <c r="Z278" s="1"/>
       <c r="AA278" s="1"/>
       <c r="AB278" s="1"/>
@@ -28938,15 +29413,33 @@
       <c r="N279" s="1"/>
       <c r="O279" s="1"/>
       <c r="P279" s="1"/>
-      <c r="Q279" s="1"/>
-      <c r="R279" s="1"/>
-      <c r="S279" s="1"/>
+      <c r="Q279" t="s">
+        <v>294</v>
+      </c>
+      <c r="R279">
+        <v>803996</v>
+      </c>
+      <c r="S279">
+        <v>925.31088614463795</v>
+      </c>
       <c r="T279" s="1"/>
-      <c r="U279" s="1"/>
-      <c r="V279" s="1"/>
+      <c r="U279" s="10">
+        <f t="shared" si="75"/>
+        <v>614</v>
+      </c>
+      <c r="V279" s="17">
+        <f t="shared" si="76"/>
+        <v>7.6426905258021713E-4</v>
+      </c>
       <c r="W279" s="1"/>
-      <c r="X279" s="1"/>
-      <c r="Y279" s="1"/>
+      <c r="X279" s="10">
+        <f t="shared" si="77"/>
+        <v>3.1087441444399246</v>
+      </c>
+      <c r="Y279" s="17">
+        <f t="shared" si="78"/>
+        <v>3.3710007848141142E-3</v>
+      </c>
       <c r="Z279" s="1"/>
       <c r="AA279" s="1"/>
       <c r="AB279" s="1"/>
@@ -28984,15 +29477,33 @@
       <c r="N280" s="1"/>
       <c r="O280" s="1"/>
       <c r="P280" s="1"/>
-      <c r="Q280" s="1"/>
-      <c r="R280" s="1"/>
-      <c r="S280" s="1"/>
+      <c r="Q280" t="s">
+        <v>295</v>
+      </c>
+      <c r="R280">
+        <v>804650</v>
+      </c>
+      <c r="S280">
+        <v>925.21861290931702</v>
+      </c>
       <c r="T280" s="1"/>
-      <c r="U280" s="1"/>
-      <c r="V280" s="1"/>
+      <c r="U280" s="10">
+        <f t="shared" si="75"/>
+        <v>25</v>
+      </c>
+      <c r="V280" s="17">
+        <f t="shared" si="76"/>
+        <v>3.1070374398011494E-5</v>
+      </c>
       <c r="W280" s="1"/>
-      <c r="X280" s="1"/>
-      <c r="Y280" s="1"/>
+      <c r="X280" s="10">
+        <f t="shared" si="77"/>
+        <v>2.6246199607850258</v>
+      </c>
+      <c r="Y280" s="17">
+        <f t="shared" si="78"/>
+        <v>2.8448266310481421E-3</v>
+      </c>
       <c r="Z280" s="1"/>
       <c r="AA280" s="1"/>
       <c r="AB280" s="1"/>
@@ -29030,15 +29541,33 @@
       <c r="N281" s="1"/>
       <c r="O281" s="1"/>
       <c r="P281" s="1"/>
-      <c r="Q281" s="1"/>
-      <c r="R281" s="1"/>
-      <c r="S281" s="1"/>
+      <c r="Q281" t="s">
+        <v>296</v>
+      </c>
+      <c r="R281">
+        <v>798589</v>
+      </c>
+      <c r="S281">
+        <v>921.92955207824696</v>
+      </c>
       <c r="T281" s="1"/>
-      <c r="U281" s="1"/>
-      <c r="V281" s="1"/>
+      <c r="U281" s="10">
+        <f t="shared" si="75"/>
+        <v>-7484</v>
+      </c>
+      <c r="V281" s="17">
+        <f t="shared" si="76"/>
+        <v>-9.2845188959312618E-3</v>
+      </c>
       <c r="W281" s="1"/>
-      <c r="X281" s="1"/>
-      <c r="Y281" s="1"/>
+      <c r="X281" s="10">
+        <f t="shared" si="77"/>
+        <v>-0.45558404922405771</v>
+      </c>
+      <c r="Y281" s="17">
+        <f t="shared" si="78"/>
+        <v>-4.9391954768132477E-4</v>
+      </c>
       <c r="Z281" s="1"/>
       <c r="AA281" s="1"/>
       <c r="AB281" s="1"/>
@@ -29076,15 +29605,33 @@
       <c r="N282" s="1"/>
       <c r="O282" s="1"/>
       <c r="P282" s="1"/>
-      <c r="Q282" s="1"/>
-      <c r="R282" s="1"/>
-      <c r="S282" s="1"/>
+      <c r="Q282" t="s">
+        <v>297</v>
+      </c>
+      <c r="R282">
+        <v>798211</v>
+      </c>
+      <c r="S282">
+        <v>921.955177307128</v>
+      </c>
       <c r="T282" s="1"/>
-      <c r="U282" s="1"/>
-      <c r="V282" s="1"/>
+      <c r="U282" s="10">
+        <f t="shared" si="75"/>
+        <v>-6611</v>
+      </c>
+      <c r="V282" s="17">
+        <f t="shared" si="76"/>
+        <v>-8.214238676378131E-3</v>
+      </c>
       <c r="W282" s="1"/>
-      <c r="X282" s="1"/>
-      <c r="Y282" s="1"/>
+      <c r="X282" s="10">
+        <f t="shared" si="77"/>
+        <v>-0.43944859504699707</v>
+      </c>
+      <c r="Y282" s="17">
+        <f t="shared" si="78"/>
+        <v>-4.7642146073561685E-4</v>
+      </c>
       <c r="Z282" s="1"/>
       <c r="AA282" s="1"/>
       <c r="AB282" s="1"/>
@@ -29122,15 +29669,33 @@
       <c r="N283" s="1"/>
       <c r="O283" s="1"/>
       <c r="P283" s="1"/>
-      <c r="Q283" s="1"/>
-      <c r="R283" s="1"/>
-      <c r="S283" s="1"/>
+      <c r="Q283" t="s">
+        <v>298</v>
+      </c>
+      <c r="R283">
+        <v>6297987</v>
+      </c>
+      <c r="S283">
+        <v>922.27863478660504</v>
+      </c>
       <c r="T283" s="1"/>
-      <c r="U283" s="1"/>
-      <c r="V283" s="1"/>
+      <c r="U283" s="10">
+        <f t="shared" si="75"/>
+        <v>-2016636</v>
+      </c>
+      <c r="V283" s="17">
+        <f t="shared" si="76"/>
+        <v>-0.24254088249100411</v>
+      </c>
       <c r="W283" s="1"/>
-      <c r="X283" s="1"/>
-      <c r="Y283" s="1"/>
+      <c r="X283" s="10">
+        <f t="shared" si="77"/>
+        <v>-0.24644398689292757</v>
+      </c>
+      <c r="Y283" s="17">
+        <f t="shared" si="78"/>
+        <v>-2.6714069087484992E-4</v>
+      </c>
       <c r="Z283" s="1"/>
       <c r="AA283" s="1"/>
       <c r="AB283" s="1"/>
@@ -29168,15 +29733,33 @@
       <c r="N284" s="1"/>
       <c r="O284" s="1"/>
       <c r="P284" s="1"/>
-      <c r="Q284" s="1"/>
-      <c r="R284" s="1"/>
-      <c r="S284" s="1"/>
+      <c r="Q284" t="s">
+        <v>299</v>
+      </c>
+      <c r="R284">
+        <v>6202140</v>
+      </c>
+      <c r="S284">
+        <v>922.37359929084698</v>
+      </c>
       <c r="T284" s="1"/>
-      <c r="U284" s="1"/>
-      <c r="V284" s="1"/>
+      <c r="U284" s="10">
+        <f t="shared" si="75"/>
+        <v>-2036827</v>
+      </c>
+      <c r="V284" s="17">
+        <f t="shared" si="76"/>
+        <v>-0.247218735067151</v>
+      </c>
       <c r="W284" s="1"/>
-      <c r="X284" s="1"/>
-      <c r="Y284" s="1"/>
+      <c r="X284" s="10">
+        <f t="shared" si="77"/>
+        <v>0.2197742462150245</v>
+      </c>
+      <c r="Y284" s="17">
+        <f t="shared" si="78"/>
+        <v>2.3832709928236484E-4</v>
+      </c>
       <c r="Z284" s="1"/>
       <c r="AA284" s="1"/>
       <c r="AB284" s="1"/>
@@ -29214,15 +29797,33 @@
       <c r="N285" s="1"/>
       <c r="O285" s="1"/>
       <c r="P285" s="1"/>
-      <c r="Q285" s="1"/>
-      <c r="R285" s="1"/>
-      <c r="S285" s="1"/>
+      <c r="Q285" t="s">
+        <v>300</v>
+      </c>
+      <c r="R285">
+        <v>6483078</v>
+      </c>
+      <c r="S285">
+        <v>922.18164396285999</v>
+      </c>
       <c r="T285" s="1"/>
-      <c r="U285" s="1"/>
-      <c r="V285" s="1"/>
+      <c r="U285" s="10">
+        <f t="shared" si="75"/>
+        <v>-1788944</v>
+      </c>
+      <c r="V285" s="17">
+        <f t="shared" si="76"/>
+        <v>-0.21626441515750322</v>
+      </c>
       <c r="W285" s="1"/>
-      <c r="X285" s="1"/>
-      <c r="Y285" s="1"/>
+      <c r="X285" s="10">
+        <f t="shared" si="77"/>
+        <v>-0.23047924041702572</v>
+      </c>
+      <c r="Y285" s="17">
+        <f t="shared" si="78"/>
+        <v>-2.4986579709797865E-4</v>
+      </c>
       <c r="Z285" s="1"/>
       <c r="AA285" s="1"/>
       <c r="AB285" s="1"/>
@@ -29260,15 +29861,33 @@
       <c r="N286" s="1"/>
       <c r="O286" s="1"/>
       <c r="P286" s="1"/>
-      <c r="Q286" s="1"/>
-      <c r="R286" s="1"/>
-      <c r="S286" s="1"/>
+      <c r="Q286" t="s">
+        <v>301</v>
+      </c>
+      <c r="R286">
+        <v>6588382</v>
+      </c>
+      <c r="S286">
+        <v>921.96937108039799</v>
+      </c>
       <c r="T286" s="1"/>
-      <c r="U286" s="1"/>
-      <c r="V286" s="1"/>
+      <c r="U286" s="10">
+        <f t="shared" si="75"/>
+        <v>-1705242</v>
+      </c>
+      <c r="V286" s="17">
+        <f t="shared" si="76"/>
+        <v>-0.20560879056007361</v>
+      </c>
       <c r="W286" s="1"/>
-      <c r="X286" s="1"/>
-      <c r="Y286" s="1"/>
+      <c r="X286" s="10">
+        <f t="shared" si="77"/>
+        <v>-0.40212893486000212</v>
+      </c>
+      <c r="Y286" s="17">
+        <f t="shared" si="78"/>
+        <v>-4.359728535122237E-4</v>
+      </c>
       <c r="Z286" s="1"/>
       <c r="AA286" s="1"/>
       <c r="AB286" s="1"/>
@@ -29306,15 +29925,33 @@
       <c r="N287" s="1"/>
       <c r="O287" s="1"/>
       <c r="P287" s="1"/>
-      <c r="Q287" s="1"/>
-      <c r="R287" s="1"/>
-      <c r="S287" s="1"/>
+      <c r="Q287" t="s">
+        <v>302</v>
+      </c>
+      <c r="R287">
+        <v>6337262</v>
+      </c>
+      <c r="S287">
+        <v>922.50565624237004</v>
+      </c>
       <c r="T287" s="1"/>
-      <c r="U287" s="1"/>
-      <c r="V287" s="1"/>
+      <c r="U287" s="10">
+        <f t="shared" si="75"/>
+        <v>-1776336</v>
+      </c>
+      <c r="V287" s="17">
+        <f t="shared" si="76"/>
+        <v>-0.21893320324719071</v>
+      </c>
       <c r="W287" s="1"/>
-      <c r="X287" s="1"/>
-      <c r="Y287" s="1"/>
+      <c r="X287" s="10">
+        <f t="shared" si="77"/>
+        <v>-6.34765625E-3</v>
+      </c>
+      <c r="Y287" s="17">
+        <f t="shared" si="78"/>
+        <v>-6.880838648358205E-6</v>
+      </c>
       <c r="Z287" s="1"/>
       <c r="AA287" s="1"/>
       <c r="AB287" s="1"/>
@@ -29352,9 +29989,6 @@
       <c r="N288" s="1"/>
       <c r="O288" s="1"/>
       <c r="P288" s="1"/>
-      <c r="Q288" s="1"/>
-      <c r="R288" s="1"/>
-      <c r="S288" s="1"/>
       <c r="T288" s="1"/>
       <c r="U288" s="1"/>
       <c r="V288" s="1"/>
@@ -29444,15 +30078,28 @@
       <c r="N290" s="1"/>
       <c r="O290" s="1"/>
       <c r="P290" s="1"/>
-      <c r="Q290" s="1"/>
-      <c r="R290" s="1"/>
-      <c r="S290" s="1"/>
+      <c r="Q290" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="R290" s="23"/>
+      <c r="S290" s="7">
+        <f>SUM(S3:S242)</f>
+        <v>999.63952136039632</v>
+      </c>
       <c r="T290" s="1"/>
       <c r="U290" s="1"/>
-      <c r="V290" s="1"/>
-      <c r="W290" s="1"/>
-      <c r="X290" s="1"/>
-      <c r="Y290" s="1"/>
+      <c r="V290" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="W290" s="23"/>
+      <c r="X290" s="7">
+        <f>S290-C335</f>
+        <v>-10758.029428244399</v>
+      </c>
+      <c r="Y290" s="25">
+        <f>X290/C335</f>
+        <v>-0.91497978675492508</v>
+      </c>
       <c r="Z290" s="1"/>
       <c r="AA290" s="1"/>
       <c r="AB290" s="1"/>
@@ -29490,15 +30137,25 @@
       <c r="N291" s="1"/>
       <c r="O291" s="1"/>
       <c r="P291" s="1"/>
-      <c r="Q291" s="1"/>
-      <c r="R291" s="1"/>
-      <c r="S291" s="1"/>
+      <c r="Q291" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="R291" s="23"/>
+      <c r="S291" s="7">
+        <f>S290/60</f>
+        <v>16.66065868933994</v>
+      </c>
       <c r="T291" s="1"/>
       <c r="U291" s="1"/>
-      <c r="V291" s="1"/>
-      <c r="W291" s="1"/>
-      <c r="X291" s="1"/>
-      <c r="Y291" s="1"/>
+      <c r="V291" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="W291" s="23"/>
+      <c r="X291" s="7">
+        <f>S291-C336</f>
+        <v>-179.30049047073999</v>
+      </c>
+      <c r="Y291" s="26"/>
       <c r="Z291" s="1"/>
       <c r="AA291" s="1"/>
       <c r="AB291" s="1"/>
@@ -31470,7 +32127,7 @@
       <c r="AJ334" s="1"/>
     </row>
     <row r="335" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A335" s="22" t="s">
+      <c r="A335" s="24" t="s">
         <v>244</v>
       </c>
       <c r="B335" s="23"/>
@@ -31513,7 +32170,7 @@
       <c r="AJ335" s="1"/>
     </row>
     <row r="336" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A336" s="22" t="s">
+      <c r="A336" s="24" t="s">
         <v>246</v>
       </c>
       <c r="B336" s="23"/>
@@ -57254,140 +57911,197 @@
       <c r="B1033" s="1"/>
       <c r="C1033" s="1"/>
       <c r="D1033" s="1"/>
+      <c r="Q1033" s="1"/>
+      <c r="R1033" s="1"/>
+      <c r="S1033" s="1"/>
     </row>
     <row r="1034" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1034" s="1"/>
       <c r="B1034" s="1"/>
       <c r="C1034" s="1"/>
       <c r="D1034" s="1"/>
+      <c r="Q1034" s="1"/>
+      <c r="R1034" s="1"/>
+      <c r="S1034" s="1"/>
     </row>
     <row r="1035" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1035" s="1"/>
       <c r="B1035" s="1"/>
       <c r="C1035" s="1"/>
       <c r="D1035" s="1"/>
+      <c r="Q1035" s="1"/>
+      <c r="R1035" s="1"/>
+      <c r="S1035" s="1"/>
     </row>
     <row r="1036" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1036" s="1"/>
       <c r="B1036" s="1"/>
       <c r="C1036" s="1"/>
       <c r="D1036" s="1"/>
+      <c r="Q1036" s="1"/>
+      <c r="R1036" s="1"/>
+      <c r="S1036" s="1"/>
     </row>
     <row r="1037" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1037" s="1"/>
       <c r="B1037" s="1"/>
       <c r="C1037" s="1"/>
       <c r="D1037" s="1"/>
+      <c r="Q1037" s="1"/>
+      <c r="R1037" s="1"/>
+      <c r="S1037" s="1"/>
     </row>
     <row r="1038" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1038" s="1"/>
       <c r="B1038" s="1"/>
       <c r="C1038" s="1"/>
       <c r="D1038" s="1"/>
+      <c r="Q1038" s="1"/>
+      <c r="R1038" s="1"/>
+      <c r="S1038" s="1"/>
     </row>
     <row r="1039" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1039" s="1"/>
       <c r="B1039" s="1"/>
       <c r="C1039" s="1"/>
       <c r="D1039" s="1"/>
+      <c r="Q1039" s="1"/>
+      <c r="R1039" s="1"/>
+      <c r="S1039" s="1"/>
     </row>
     <row r="1040" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1040" s="1"/>
       <c r="B1040" s="1"/>
       <c r="C1040" s="1"/>
       <c r="D1040" s="1"/>
-    </row>
-    <row r="1041" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1040" s="1"/>
+      <c r="R1040" s="1"/>
+      <c r="S1040" s="1"/>
+    </row>
+    <row r="1041" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1041" s="1"/>
       <c r="B1041" s="1"/>
       <c r="C1041" s="1"/>
       <c r="D1041" s="1"/>
-    </row>
-    <row r="1042" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1041" s="1"/>
+      <c r="R1041" s="1"/>
+      <c r="S1041" s="1"/>
+    </row>
+    <row r="1042" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1042" s="1"/>
       <c r="B1042" s="1"/>
       <c r="C1042" s="1"/>
       <c r="D1042" s="1"/>
-    </row>
-    <row r="1043" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1042" s="1"/>
+      <c r="R1042" s="1"/>
+      <c r="S1042" s="1"/>
+    </row>
+    <row r="1043" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1043" s="1"/>
       <c r="B1043" s="1"/>
       <c r="C1043" s="1"/>
       <c r="D1043" s="1"/>
-    </row>
-    <row r="1044" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1043" s="1"/>
+      <c r="R1043" s="1"/>
+      <c r="S1043" s="1"/>
+    </row>
+    <row r="1044" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1044" s="1"/>
       <c r="B1044" s="1"/>
       <c r="C1044" s="1"/>
       <c r="D1044" s="1"/>
-    </row>
-    <row r="1045" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1044" s="1"/>
+      <c r="R1044" s="1"/>
+      <c r="S1044" s="1"/>
+    </row>
+    <row r="1045" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1045" s="1"/>
       <c r="B1045" s="1"/>
       <c r="C1045" s="1"/>
       <c r="D1045" s="1"/>
-    </row>
-    <row r="1046" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1045" s="1"/>
+      <c r="R1045" s="1"/>
+      <c r="S1045" s="1"/>
+    </row>
+    <row r="1046" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1046" s="1"/>
       <c r="B1046" s="1"/>
       <c r="C1046" s="1"/>
       <c r="D1046" s="1"/>
-    </row>
-    <row r="1047" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1046" s="1"/>
+      <c r="R1046" s="1"/>
+      <c r="S1046" s="1"/>
+    </row>
+    <row r="1047" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1047" s="1"/>
       <c r="B1047" s="1"/>
       <c r="C1047" s="1"/>
       <c r="D1047" s="1"/>
-    </row>
-    <row r="1048" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1047" s="1"/>
+      <c r="R1047" s="1"/>
+      <c r="S1047" s="1"/>
+    </row>
+    <row r="1048" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1048" s="1"/>
       <c r="B1048" s="1"/>
       <c r="C1048" s="1"/>
       <c r="D1048" s="1"/>
-    </row>
-    <row r="1049" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1048" s="1"/>
+      <c r="R1048" s="1"/>
+      <c r="S1048" s="1"/>
+    </row>
+    <row r="1049" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1049" s="1"/>
       <c r="B1049" s="1"/>
       <c r="C1049" s="1"/>
       <c r="D1049" s="1"/>
-    </row>
-    <row r="1050" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1049" s="1"/>
+      <c r="R1049" s="1"/>
+      <c r="S1049" s="1"/>
+    </row>
+    <row r="1050" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1050" s="1"/>
       <c r="B1050" s="1"/>
       <c r="C1050" s="1"/>
       <c r="D1050" s="1"/>
-    </row>
-    <row r="1051" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1050" s="1"/>
+      <c r="R1050" s="1"/>
+      <c r="S1050" s="1"/>
+    </row>
+    <row r="1051" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1051" s="1"/>
       <c r="B1051" s="1"/>
       <c r="C1051" s="1"/>
       <c r="D1051" s="1"/>
-    </row>
-    <row r="1052" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1051" s="1"/>
+      <c r="R1051" s="1"/>
+      <c r="S1051" s="1"/>
+    </row>
+    <row r="1052" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1052" s="1"/>
       <c r="B1052" s="1"/>
       <c r="C1052" s="1"/>
       <c r="D1052" s="1"/>
     </row>
-    <row r="1053" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1053" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1053" s="1"/>
       <c r="B1053" s="1"/>
       <c r="C1053" s="1"/>
       <c r="D1053" s="1"/>
     </row>
-    <row r="1054" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1054" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1054" s="1"/>
       <c r="B1054" s="1"/>
       <c r="C1054" s="1"/>
       <c r="D1054" s="1"/>
     </row>
-    <row r="1055" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1055" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1055" s="1"/>
       <c r="B1055" s="1"/>
       <c r="C1055" s="1"/>
       <c r="D1055" s="1"/>
     </row>
-    <row r="1056" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1056" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1056" s="1"/>
       <c r="B1056" s="1"/>
       <c r="C1056" s="1"/>
@@ -57635,12 +58349,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="F245:G245"/>
-    <mergeCell ref="F246:G246"/>
-    <mergeCell ref="L245:M245"/>
-    <mergeCell ref="O245:O246"/>
-    <mergeCell ref="L246:M246"/>
+    <mergeCell ref="V290:W290"/>
+    <mergeCell ref="Y290:Y291"/>
+    <mergeCell ref="Q291:R291"/>
+    <mergeCell ref="V291:W291"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A335:B335"/>
     <mergeCell ref="A336:B336"/>
     <mergeCell ref="AI245:AI246"/>
@@ -57655,13 +58368,14 @@
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Q271:R271"/>
+    <mergeCell ref="Q290:R290"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="V271:W271"/>
-    <mergeCell ref="Y271:Y272"/>
-    <mergeCell ref="Q272:R272"/>
-    <mergeCell ref="V272:W272"/>
-    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="F245:G245"/>
+    <mergeCell ref="F246:G246"/>
+    <mergeCell ref="L245:M245"/>
+    <mergeCell ref="O245:O246"/>
+    <mergeCell ref="L246:M246"/>
   </mergeCells>
   <conditionalFormatting sqref="AF3:AF242">
     <cfRule type="cellIs" dxfId="47" priority="1" operator="lessThan">
@@ -57721,7 +58435,7 @@
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y271:Y272">
+  <conditionalFormatting sqref="Y290:Y291">
     <cfRule type="cellIs" dxfId="33" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -57729,7 +58443,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y237 Y240 Y243 Y246 Y249 Y252 Y255 Y258 Y261 Y264 Y266 Y268">
+  <conditionalFormatting sqref="Y3:Y237 Y240 Y243 Y246 Y249 Y252 Y255 Y258 Y261 Y264 Y266 Y268:Y287">
     <cfRule type="cellIs" dxfId="31" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -57813,7 +58527,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V239 V244 V249 V254 V259 V264 V266 V268">
+  <conditionalFormatting sqref="V239 V244 V249 V254 V259 V264 V266 V268:V287">
     <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Analise de alguns casos de teste 1
</commit_message>
<xml_diff>
--- a/solutions.xlsx
+++ b/solutions.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solutions1" localSheetId="0">Plan1!$F$2:$I$17</definedName>
-    <definedName name="solutions1_1" localSheetId="0">Plan1!$AA$3:$AC$17</definedName>
-    <definedName name="solutions1_2" localSheetId="0">Plan1!$Q$2:$S$17</definedName>
-    <definedName name="solutions2" localSheetId="0">Plan1!$Z$4:$AC$224</definedName>
-    <definedName name="solutions2_1" localSheetId="0">Plan1!$AA$18:$AC$237</definedName>
+    <definedName name="solutions1" localSheetId="1">Plan1!$F$2:$I$17</definedName>
+    <definedName name="solutions1_1" localSheetId="1">Plan1!$AA$3:$AC$17</definedName>
+    <definedName name="solutions1_2" localSheetId="1">Plan1!$Q$2:$S$17</definedName>
+    <definedName name="solutions1_3" localSheetId="0">Plan3!$A$1:$C$15</definedName>
+    <definedName name="solutions2" localSheetId="1">Plan1!$Z$4:$AC$224</definedName>
+    <definedName name="solutions2_1" localSheetId="1">Plan1!$AA$18:$AC$237</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +37,16 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="solutions11" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="solutions1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Macbook/Documents/GitKraken_Projects/ICAlgoritmos/guloso/solutions1.csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="solutions11" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Macbook/Documents/GitKraken_Projects/ICAlgoritmos/gurobi/solutions1.csv" comma="1">
       <textFields count="4">
         <textField/>
@@ -45,7 +56,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="solutions111" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="solutions111" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Macbook/Documents/GitKraken_Projects/ICAlgoritmos/gurobi/solutions1.csv" comma="1">
       <textFields count="4">
         <textField/>
@@ -59,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="349">
   <si>
     <t>ILP</t>
   </si>
@@ -1289,9 +1300,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1299,742 +1311,17 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="134">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="52">
     <dxf>
       <font>
         <color theme="1"/>
@@ -2550,11 +1837,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1_3" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="solutions1_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2820,10 +2111,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="21">
+        <v>932590</v>
+      </c>
+      <c r="C1">
+        <v>2.6799E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="21">
+        <v>981514</v>
+      </c>
+      <c r="C2">
+        <v>3.1615999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="21">
+        <v>1015490</v>
+      </c>
+      <c r="C3">
+        <v>2.6675999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="21">
+        <v>1042620</v>
+      </c>
+      <c r="C4">
+        <v>3.3223999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="21">
+        <v>798562</v>
+      </c>
+      <c r="C5">
+        <v>4.4380000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="21">
+        <v>858082</v>
+      </c>
+      <c r="C6">
+        <v>4.8392999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="21">
+        <v>902389</v>
+      </c>
+      <c r="C7">
+        <v>4.2763000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="21">
+        <v>932503</v>
+      </c>
+      <c r="C8">
+        <v>4.4858000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="21">
+        <v>795352</v>
+      </c>
+      <c r="C9">
+        <v>8.0710000000000004E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="21">
+        <v>854872</v>
+      </c>
+      <c r="C10">
+        <v>8.6744000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="21">
+        <v>901456</v>
+      </c>
+      <c r="C11">
+        <v>8.8377999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="21">
+        <v>932503</v>
+      </c>
+      <c r="C12">
+        <v>8.5313E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="21">
+        <v>17764500</v>
+      </c>
+      <c r="C13">
+        <v>49.780200000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="21">
+        <v>13070000</v>
+      </c>
+      <c r="C14">
+        <v>49.730200000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="21">
+        <v>11702100</v>
+      </c>
+      <c r="C15">
+        <v>47.132599999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS1096"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE223" zoomScale="112" workbookViewId="0">
-      <selection activeCell="AS252" sqref="AS252"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="AO250" sqref="AO250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2856,77 +2332,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="24"/>
+      <c r="L1" s="25"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="24"/>
+      <c r="O1" s="25"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
       <c r="T1" s="15"/>
-      <c r="U1" s="28" t="s">
+      <c r="U1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="24"/>
+      <c r="V1" s="25"/>
       <c r="W1" s="1"/>
-      <c r="X1" s="28" t="s">
+      <c r="X1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="24"/>
+      <c r="Y1" s="25"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="28" t="s">
+      <c r="AA1" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="25"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="28" t="s">
+      <c r="AE1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AF1" s="24"/>
+      <c r="AF1" s="25"/>
       <c r="AG1" s="1"/>
-      <c r="AH1" s="28" t="s">
+      <c r="AH1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AI1" s="24"/>
+      <c r="AI1" s="25"/>
       <c r="AJ1" s="1"/>
-      <c r="AK1" s="28" t="s">
+      <c r="AK1" s="23" t="s">
         <v>348</v>
       </c>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="25"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="28" t="s">
+      <c r="AO1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AP1" s="24"/>
+      <c r="AP1" s="25"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="28" t="s">
+      <c r="AR1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AS1" s="24"/>
+      <c r="AS1" s="25"/>
     </row>
     <row r="2" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -3145,25 +2621,29 @@
       <c r="AK3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="AL3" s="9"/>
-      <c r="AM3" s="10"/>
+      <c r="AL3" s="21">
+        <v>932590</v>
+      </c>
+      <c r="AM3">
+        <v>2.6799E-2</v>
+      </c>
       <c r="AN3" s="1"/>
       <c r="AO3" s="6">
         <f>AL3-B3</f>
-        <v>-932615.75</v>
+        <v>-25.75</v>
       </c>
       <c r="AP3" s="8">
         <f>AO3/B3</f>
-        <v>-1</v>
+        <v>-2.7610513761964668E-5</v>
       </c>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="7">
         <f>AM3-C3</f>
-        <v>-0.143984794616699</v>
+        <v>-0.11718579461669899</v>
       </c>
       <c r="AS3" s="8">
         <f>AR3/C3</f>
-        <v>-1</v>
+        <v>-0.81387617997204875</v>
       </c>
     </row>
     <row r="4" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3270,25 +2750,29 @@
       <c r="AK4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="10"/>
+      <c r="AL4" s="21">
+        <v>981514</v>
+      </c>
+      <c r="AM4">
+        <v>3.1615999999999998E-2</v>
+      </c>
       <c r="AN4" s="1"/>
       <c r="AO4" s="6">
         <f t="shared" ref="AO4:AO48" si="12">AL4-B4</f>
-        <v>-977799.4</v>
+        <v>3714.5999999999767</v>
       </c>
       <c r="AP4" s="8">
         <f t="shared" ref="AP4:AP48" si="13">AO4/B4</f>
-        <v>-1</v>
+        <v>3.7989387189233054E-3</v>
       </c>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="7">
         <f t="shared" ref="AR4:AR67" si="14">AM4-C4</f>
-        <v>-0.14197301864624001</v>
+        <v>-0.11035701864624001</v>
       </c>
       <c r="AS4" s="8">
         <f t="shared" ref="AS4:AS67" si="15">AR4/C4</f>
-        <v>-1</v>
+        <v>-0.7773097994149234</v>
       </c>
     </row>
     <row r="5" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3395,25 +2879,29 @@
       <c r="AK5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="10"/>
+      <c r="AL5" s="21">
+        <v>1015490</v>
+      </c>
+      <c r="AM5">
+        <v>2.6675999999999998E-2</v>
+      </c>
       <c r="AN5" s="1"/>
       <c r="AO5" s="6">
         <f t="shared" si="12"/>
-        <v>-1010641.45</v>
+        <v>4848.5500000000466</v>
       </c>
       <c r="AP5" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>4.7974976684362659E-3</v>
       </c>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="7">
         <f t="shared" si="14"/>
-        <v>-5.4972887039184501E-2</v>
+        <v>-2.8296887039184503E-2</v>
       </c>
       <c r="AS5" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.51474260427716978</v>
       </c>
     </row>
     <row r="6" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3520,25 +3008,29 @@
       <c r="AK6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="AL6" s="9"/>
-      <c r="AM6" s="10"/>
+      <c r="AL6" s="21">
+        <v>1042620</v>
+      </c>
+      <c r="AM6">
+        <v>3.3223999999999997E-2</v>
+      </c>
       <c r="AN6" s="1"/>
       <c r="AO6" s="6">
         <f t="shared" si="12"/>
-        <v>-1034976.975</v>
+        <v>7643.0250000000233</v>
       </c>
       <c r="AP6" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>7.3847295008664547E-3</v>
       </c>
       <c r="AQ6" s="1"/>
       <c r="AR6" s="7">
         <f t="shared" si="14"/>
-        <v>-3.8845777511596603E-2</v>
+        <v>-5.6217775115966068E-3</v>
       </c>
       <c r="AS6" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.14472042707649091</v>
       </c>
     </row>
     <row r="7" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3645,25 +3137,29 @@
       <c r="AK7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="AL7" s="9"/>
-      <c r="AM7" s="10"/>
+      <c r="AL7" s="21">
+        <v>798562</v>
+      </c>
+      <c r="AM7">
+        <v>4.4380000000000003E-2</v>
+      </c>
       <c r="AN7" s="1"/>
       <c r="AO7" s="6">
         <f t="shared" si="12"/>
-        <v>-796648.4375</v>
+        <v>1913.5625</v>
       </c>
       <c r="AP7" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>2.402016259524767E-3</v>
       </c>
       <c r="AQ7" s="1"/>
       <c r="AR7" s="7">
         <f t="shared" si="14"/>
-        <v>-6.0125827789306599E-2</v>
+        <v>-1.5745827789306596E-2</v>
       </c>
       <c r="AS7" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.26188126414630414</v>
       </c>
     </row>
     <row r="8" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3770,25 +3266,29 @@
       <c r="AK8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="AL8" s="9"/>
-      <c r="AM8" s="10"/>
+      <c r="AL8" s="21">
+        <v>858082</v>
+      </c>
+      <c r="AM8">
+        <v>4.8392999999999999E-2</v>
+      </c>
       <c r="AN8" s="1"/>
       <c r="AO8" s="6">
         <f t="shared" si="12"/>
-        <v>-854704.2</v>
+        <v>3377.8000000000466</v>
       </c>
       <c r="AP8" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>3.9520105318308334E-3</v>
       </c>
       <c r="AQ8" s="1"/>
       <c r="AR8" s="7">
         <f t="shared" si="14"/>
-        <v>-5.8726072311401298E-2</v>
+        <v>-1.0333072311401299E-2</v>
       </c>
       <c r="AS8" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.17595374430302566</v>
       </c>
     </row>
     <row r="9" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3895,25 +3395,29 @@
       <c r="AK9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AL9" s="9"/>
-      <c r="AM9" s="10"/>
+      <c r="AL9" s="21">
+        <v>902389</v>
+      </c>
+      <c r="AM9">
+        <v>4.2763000000000002E-2</v>
+      </c>
       <c r="AN9" s="1"/>
       <c r="AO9" s="6">
         <f t="shared" si="12"/>
-        <v>-893782.11250000005</v>
+        <v>8606.8874999999534</v>
       </c>
       <c r="AP9" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>9.6297379189270275E-3</v>
       </c>
       <c r="AQ9" s="1"/>
       <c r="AR9" s="7">
         <f t="shared" si="14"/>
-        <v>-6.0395002365112298E-2</v>
+        <v>-1.7632002365112295E-2</v>
       </c>
       <c r="AS9" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.2919447251366874</v>
       </c>
     </row>
     <row r="10" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4020,25 +3524,29 @@
       <c r="AK10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="AL10" s="9"/>
-      <c r="AM10" s="10"/>
+      <c r="AL10" s="21">
+        <v>932503</v>
+      </c>
+      <c r="AM10">
+        <v>4.4858000000000002E-2</v>
+      </c>
       <c r="AN10" s="1"/>
       <c r="AO10" s="6">
         <f t="shared" si="12"/>
-        <v>-928941.75</v>
+        <v>3561.25</v>
       </c>
       <c r="AP10" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>3.8336634132333917E-3</v>
       </c>
       <c r="AQ10" s="1"/>
       <c r="AR10" s="7">
         <f t="shared" si="14"/>
-        <v>-6.0109138488769497E-2</v>
+        <v>-1.5251138488769495E-2</v>
       </c>
       <c r="AS10" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.25372412368909503</v>
       </c>
     </row>
     <row r="11" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4145,25 +3653,29 @@
       <c r="AK11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="AL11" s="9"/>
-      <c r="AM11" s="10"/>
+      <c r="AL11" s="21">
+        <v>795352</v>
+      </c>
+      <c r="AM11">
+        <v>8.0710000000000004E-2</v>
+      </c>
       <c r="AN11" s="1"/>
       <c r="AO11" s="6">
         <f t="shared" si="12"/>
-        <v>-793439.5625</v>
+        <v>1912.4375</v>
       </c>
       <c r="AP11" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>2.410312757753367E-3</v>
       </c>
       <c r="AQ11" s="1"/>
       <c r="AR11" s="7">
         <f t="shared" si="14"/>
-        <v>-0.125276803970336</v>
+        <v>-4.4566803970335994E-2</v>
       </c>
       <c r="AS11" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.35574665507023046</v>
       </c>
     </row>
     <row r="12" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4270,25 +3782,29 @@
       <c r="AK12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="AL12" s="9"/>
-      <c r="AM12" s="10"/>
+      <c r="AL12" s="21">
+        <v>854872</v>
+      </c>
+      <c r="AM12">
+        <v>8.6744000000000002E-2</v>
+      </c>
       <c r="AN12" s="1"/>
       <c r="AO12" s="6">
         <f t="shared" si="12"/>
-        <v>-851495.32499999995</v>
+        <v>3376.6750000000466</v>
       </c>
       <c r="AP12" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>3.9655825473851507E-3</v>
       </c>
       <c r="AQ12" s="1"/>
       <c r="AR12" s="7">
         <f t="shared" si="14"/>
-        <v>-0.121948957443237</v>
+        <v>-3.5204957443236998E-2</v>
       </c>
       <c r="AS12" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.28868600586129389</v>
       </c>
     </row>
     <row r="13" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4395,25 +3911,29 @@
       <c r="AK13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="AL13" s="9"/>
-      <c r="AM13" s="10"/>
+      <c r="AL13" s="21">
+        <v>901456</v>
+      </c>
+      <c r="AM13">
+        <v>8.8377999999999998E-2</v>
+      </c>
       <c r="AN13" s="1"/>
       <c r="AO13" s="6">
         <f t="shared" si="12"/>
-        <v>-893076.71250000002</v>
+        <v>8379.2874999999767</v>
       </c>
       <c r="AP13" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>9.382494675674322E-3</v>
       </c>
       <c r="AQ13" s="1"/>
       <c r="AR13" s="7">
         <f t="shared" si="14"/>
-        <v>-0.14457798004150299</v>
+        <v>-5.6199980041502992E-2</v>
       </c>
       <c r="AS13" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.38871742450247304</v>
       </c>
     </row>
     <row r="14" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4520,25 +4040,29 @@
       <c r="AK14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AL14" s="9"/>
-      <c r="AM14" s="10"/>
+      <c r="AL14" s="21">
+        <v>932503</v>
+      </c>
+      <c r="AM14">
+        <v>8.5313E-2</v>
+      </c>
       <c r="AN14" s="1"/>
       <c r="AO14" s="6">
         <f t="shared" si="12"/>
-        <v>-928941.75</v>
+        <v>3561.25</v>
       </c>
       <c r="AP14" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>3.8336634132333917E-3</v>
       </c>
       <c r="AQ14" s="1"/>
       <c r="AR14" s="7">
         <f t="shared" si="14"/>
-        <v>-0.12414598464965799</v>
+        <v>-3.8832984649657995E-2</v>
       </c>
       <c r="AS14" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-0.31280097184975669</v>
       </c>
     </row>
     <row r="15" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4645,25 +4169,29 @@
       <c r="AK15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AL15" s="9"/>
-      <c r="AM15" s="10"/>
+      <c r="AL15" s="21">
+        <v>17764500</v>
+      </c>
+      <c r="AM15">
+        <v>49.780200000000001</v>
+      </c>
       <c r="AN15" s="1"/>
       <c r="AO15" s="6">
         <f t="shared" si="12"/>
-        <v>-17156454.478299901</v>
+        <v>608045.52170009911</v>
       </c>
       <c r="AP15" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>3.544121091389698E-2</v>
       </c>
       <c r="AQ15" s="1"/>
       <c r="AR15" s="7">
         <f t="shared" si="14"/>
-        <v>-7.2306706905364901</v>
+        <v>42.549529309463509</v>
       </c>
       <c r="AS15" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>5.8845895672101873</v>
       </c>
     </row>
     <row r="16" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4770,25 +4298,29 @@
       <c r="AK16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="AL16" s="9"/>
-      <c r="AM16" s="10"/>
+      <c r="AL16" s="21">
+        <v>13070000</v>
+      </c>
+      <c r="AM16">
+        <v>49.730200000000004</v>
+      </c>
       <c r="AN16" s="1"/>
       <c r="AO16" s="6">
         <f t="shared" si="12"/>
-        <v>-12979071.581429901</v>
+        <v>90928.418570099398</v>
       </c>
       <c r="AP16" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>7.0057721771253105E-3</v>
       </c>
       <c r="AQ16" s="1"/>
       <c r="AR16" s="7">
         <f t="shared" si="14"/>
-        <v>-6.8251147270202601</v>
+        <v>42.905085272979747</v>
       </c>
       <c r="AS16" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>6.2863537081832241</v>
       </c>
     </row>
     <row r="17" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4895,25 +4427,29 @@
       <c r="AK17" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AL17" s="9"/>
-      <c r="AM17" s="10"/>
+      <c r="AL17" s="21">
+        <v>11702100</v>
+      </c>
+      <c r="AM17">
+        <v>47.132599999999996</v>
+      </c>
       <c r="AN17" s="1"/>
       <c r="AO17" s="6">
         <f t="shared" si="12"/>
-        <v>-11505594.3287799</v>
+        <v>196505.67122009955</v>
       </c>
       <c r="AP17" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>1.7079141294645123E-2</v>
       </c>
       <c r="AQ17" s="1"/>
       <c r="AR17" s="7">
         <f t="shared" si="14"/>
-        <v>-14.8222358226776</v>
+        <v>32.310364177322398</v>
       </c>
       <c r="AS17" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>2.1798576519669495</v>
       </c>
     </row>
     <row r="18" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -33092,10 +32628,10 @@
         <v>0</v>
       </c>
       <c r="E245" s="1"/>
-      <c r="F245" s="23" t="s">
+      <c r="F245" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="G245" s="24"/>
+      <c r="G245" s="25"/>
       <c r="H245" s="7">
         <f>SUM(H3:H242)</f>
         <v>442.46593046188286</v>
@@ -33103,15 +32639,15 @@
       <c r="I245" s="1"/>
       <c r="J245" s="1"/>
       <c r="K245" s="1"/>
-      <c r="L245" s="23" t="s">
+      <c r="L245" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="M245" s="24"/>
+      <c r="M245" s="25"/>
       <c r="N245" s="7">
         <f>H245-C335</f>
         <v>-11315.203019142911</v>
       </c>
-      <c r="O245" s="25">
+      <c r="O245" s="26">
         <f>N245/C335</f>
         <v>-0.96236788666542994</v>
       </c>
@@ -33143,50 +32679,50 @@
         <v>7.3130313726978255E-4</v>
       </c>
       <c r="Z245" s="1"/>
-      <c r="AA245" s="23" t="s">
+      <c r="AA245" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="AB245" s="24"/>
+      <c r="AB245" s="25"/>
       <c r="AC245" s="7">
         <f>SUM(AC3:AC242)</f>
         <v>6444.9016520000005</v>
       </c>
       <c r="AD245" s="1"/>
       <c r="AE245" s="1"/>
-      <c r="AF245" s="23" t="s">
+      <c r="AF245" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AG245" s="24"/>
+      <c r="AG245" s="25"/>
       <c r="AH245" s="7">
         <f>AC245-C335</f>
         <v>-5312.7672976047943</v>
       </c>
-      <c r="AI245" s="25">
+      <c r="AI245" s="26">
         <f>AH245/C335</f>
         <v>-0.45185549281716847</v>
       </c>
       <c r="AJ245" s="1"/>
-      <c r="AK245" s="23" t="s">
+      <c r="AK245" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="AL245" s="24"/>
+      <c r="AL245" s="25"/>
       <c r="AM245" s="7">
         <f>SUM(AM3:AM242)</f>
-        <v>0</v>
+        <v>147.28285399999999</v>
       </c>
       <c r="AN245" s="1"/>
       <c r="AO245" s="1"/>
-      <c r="AP245" s="23" t="s">
+      <c r="AP245" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AQ245" s="24"/>
+      <c r="AQ245" s="25"/>
       <c r="AR245" s="7">
         <f>AM245-C335</f>
-        <v>-11757.668949604795</v>
-      </c>
-      <c r="AS245" s="25">
+        <v>-11610.386095604796</v>
+      </c>
+      <c r="AS245" s="26">
         <f>AR245/C335</f>
-        <v>-1</v>
+        <v>-0.98747346479720799</v>
       </c>
     </row>
     <row r="246" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -33203,10 +32739,10 @@
         <v>0</v>
       </c>
       <c r="E246" s="1"/>
-      <c r="F246" s="23" t="s">
+      <c r="F246" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="G246" s="24"/>
+      <c r="G246" s="25"/>
       <c r="H246" s="7">
         <f>H245/60</f>
         <v>7.3744321743647143</v>
@@ -33214,15 +32750,15 @@
       <c r="I246" s="1"/>
       <c r="J246" s="1"/>
       <c r="K246" s="1"/>
-      <c r="L246" s="23" t="s">
+      <c r="L246" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="M246" s="24"/>
+      <c r="M246" s="25"/>
       <c r="N246" s="7">
         <f>H246-C336</f>
         <v>-188.58671698571519</v>
       </c>
-      <c r="O246" s="26"/>
+      <c r="O246" s="27"/>
       <c r="P246" s="1"/>
       <c r="Q246" t="s">
         <v>261</v>
@@ -33251,45 +32787,45 @@
         <v>1.5635693068758426E-3</v>
       </c>
       <c r="Z246" s="1"/>
-      <c r="AA246" s="23" t="s">
+      <c r="AA246" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="AB246" s="24"/>
+      <c r="AB246" s="25"/>
       <c r="AC246" s="7">
         <f>AC245/60</f>
         <v>107.41502753333334</v>
       </c>
       <c r="AD246" s="1"/>
       <c r="AE246" s="1"/>
-      <c r="AF246" s="23" t="s">
+      <c r="AF246" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="AG246" s="24"/>
+      <c r="AG246" s="25"/>
       <c r="AH246" s="7">
         <f>AC246-C336</f>
         <v>-88.546121626746569</v>
       </c>
-      <c r="AI246" s="26"/>
+      <c r="AI246" s="27"/>
       <c r="AJ246" s="1"/>
-      <c r="AK246" s="23" t="s">
+      <c r="AK246" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="AL246" s="24"/>
+      <c r="AL246" s="25"/>
       <c r="AM246" s="7">
         <f>AM245/60</f>
-        <v>0</v>
+        <v>2.4547142333333332</v>
       </c>
       <c r="AN246" s="1"/>
       <c r="AO246" s="1"/>
-      <c r="AP246" s="23" t="s">
+      <c r="AP246" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="AQ246" s="24"/>
+      <c r="AQ246" s="25"/>
       <c r="AR246" s="7">
         <f>AM246-C336</f>
-        <v>-195.96114916007991</v>
-      </c>
-      <c r="AS246" s="26"/>
+        <v>-193.50643492674658</v>
+      </c>
+      <c r="AS246" s="27"/>
     </row>
     <row r="247" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="10" t="s">
@@ -36025,25 +35561,25 @@
       <c r="N290" s="1"/>
       <c r="O290" s="1"/>
       <c r="P290" s="1"/>
-      <c r="Q290" s="23" t="s">
+      <c r="Q290" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="R290" s="24"/>
+      <c r="R290" s="25"/>
       <c r="S290" s="7">
         <f>SUM(S3:S242)</f>
         <v>999.63952136039632</v>
       </c>
       <c r="T290" s="1"/>
       <c r="U290" s="1"/>
-      <c r="V290" s="23" t="s">
+      <c r="V290" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="W290" s="24"/>
+      <c r="W290" s="25"/>
       <c r="X290" s="7">
         <f>S290-C335</f>
         <v>-10758.029428244399</v>
       </c>
-      <c r="Y290" s="25">
+      <c r="Y290" s="26">
         <f>X290/C335</f>
         <v>-0.91497978675492508</v>
       </c>
@@ -36084,25 +35620,25 @@
       <c r="N291" s="1"/>
       <c r="O291" s="1"/>
       <c r="P291" s="1"/>
-      <c r="Q291" s="23" t="s">
+      <c r="Q291" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="R291" s="24"/>
+      <c r="R291" s="25"/>
       <c r="S291" s="7">
         <f>S290/60</f>
         <v>16.66065868933994</v>
       </c>
       <c r="T291" s="1"/>
       <c r="U291" s="1"/>
-      <c r="V291" s="23" t="s">
+      <c r="V291" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="W291" s="24"/>
+      <c r="W291" s="25"/>
       <c r="X291" s="7">
         <f>S291-C336</f>
         <v>-179.30049047073999</v>
       </c>
-      <c r="Y291" s="26"/>
+      <c r="Y291" s="27"/>
       <c r="Z291" s="1"/>
       <c r="AA291" s="1"/>
       <c r="AB291" s="1"/>
@@ -38074,10 +37610,10 @@
       <c r="AJ334" s="1"/>
     </row>
     <row r="335" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A335" s="23" t="s">
+      <c r="A335" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="B335" s="24"/>
+      <c r="B335" s="25"/>
       <c r="C335" s="7">
         <f>SUM(C3:C242)</f>
         <v>11757.668949604795</v>
@@ -38117,10 +37653,10 @@
       <c r="AJ335" s="1"/>
     </row>
     <row r="336" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A336" s="23" t="s">
+      <c r="A336" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="B336" s="24"/>
+      <c r="B336" s="25"/>
       <c r="C336" s="7">
         <f>C335/60</f>
         <v>195.96114916007991</v>
@@ -64296,20 +63832,11 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AS245:AS246"/>
-    <mergeCell ref="AK246:AL246"/>
-    <mergeCell ref="AP246:AQ246"/>
-    <mergeCell ref="AK245:AL245"/>
-    <mergeCell ref="AP245:AQ245"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="F245:G245"/>
-    <mergeCell ref="F246:G246"/>
-    <mergeCell ref="L245:M245"/>
-    <mergeCell ref="O245:O246"/>
-    <mergeCell ref="L246:M246"/>
+    <mergeCell ref="V290:W290"/>
+    <mergeCell ref="Y290:Y291"/>
+    <mergeCell ref="Q291:R291"/>
+    <mergeCell ref="V291:W291"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A335:B335"/>
     <mergeCell ref="A336:B336"/>
     <mergeCell ref="AI245:AI246"/>
@@ -64326,217 +63853,226 @@
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="Q290:R290"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="V290:W290"/>
-    <mergeCell ref="Y290:Y291"/>
-    <mergeCell ref="Q291:R291"/>
-    <mergeCell ref="V291:W291"/>
-    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="F245:G245"/>
+    <mergeCell ref="F246:G246"/>
+    <mergeCell ref="L245:M245"/>
+    <mergeCell ref="O245:O246"/>
+    <mergeCell ref="L246:M246"/>
+    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AS245:AS246"/>
+    <mergeCell ref="AK246:AL246"/>
+    <mergeCell ref="AP246:AQ246"/>
+    <mergeCell ref="AK245:AL245"/>
+    <mergeCell ref="AP245:AQ245"/>
   </mergeCells>
   <conditionalFormatting sqref="AF3:AF242">
-    <cfRule type="cellIs" dxfId="133" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="62" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3:AF242">
-    <cfRule type="cellIs" dxfId="131" priority="63" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="63" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3:AF242">
-    <cfRule type="cellIs" dxfId="130" priority="64" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="48" priority="64" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3:AF242">
-    <cfRule type="cellIs" dxfId="129" priority="65" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="65" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI245:AI246">
-    <cfRule type="cellIs" dxfId="128" priority="57" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="57" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="58" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="45" priority="58" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O245:O246">
-    <cfRule type="cellIs" dxfId="126" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="56" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="43" priority="56" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI3:AI237 O3:O237">
-    <cfRule type="cellIs" dxfId="124" priority="59" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="59" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="60" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="60" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L237">
-    <cfRule type="cellIs" dxfId="122" priority="52" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="52" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="53" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="54" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y290:Y291">
-    <cfRule type="cellIs" dxfId="119" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="48" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="49" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="49" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y237 Y240 Y243 Y246 Y249 Y252 Y255 Y258 Y261 Y264 Y266 Y268:Y287">
-    <cfRule type="cellIs" dxfId="117" priority="50" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="50" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="51" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="51" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V237 V240:V242 V245:V247 V250:V252 V255:V257 V260:V262">
-    <cfRule type="cellIs" dxfId="115" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="45" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="47" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI238 O238 O240:O242 AI242">
-    <cfRule type="cellIs" dxfId="112" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="40" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="40" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L238 L240:L242">
-    <cfRule type="cellIs" dxfId="110" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="38" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y238 Y241 Y244 Y247 Y250 Y253 Y256 Y259 Y262">
-    <cfRule type="cellIs" dxfId="107" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="34" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="35" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V238 V243 V248 V253 V258 V263 V265 V267">
-    <cfRule type="cellIs" dxfId="105" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="33" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O239 AI239:AI241">
-    <cfRule type="cellIs" dxfId="102" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="26" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L239">
-    <cfRule type="cellIs" dxfId="100" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y239 Y242 Y245 Y248 Y251 Y254 Y257 Y260 Y263 Y265 Y267">
-    <cfRule type="cellIs" dxfId="97" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V239 V244 V249 V254 V259 V264 V266 V268:V287">
-    <cfRule type="cellIs" dxfId="95" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="lessThan">
       <formula>0%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D332">
-    <cfRule type="cellIs" dxfId="92" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP3:AP242">
-    <cfRule type="cellIs" dxfId="77" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP3:AP242">
-    <cfRule type="cellIs" dxfId="73" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP3:AP242">
-    <cfRule type="cellIs" dxfId="71" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP3:AP242">
-    <cfRule type="cellIs" dxfId="69" priority="13" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="13" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS245:AS246">
-    <cfRule type="cellIs" dxfId="67" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS3:AS242">
-    <cfRule type="cellIs" dxfId="63" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>